<commit_message>
docs: adicionei mais um BDD de login ate finalizar de compra
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFB7C75D-B821-4E03-AF10-8A706B8C5568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59F10922-A01A-4046-AC13-9C385E3B478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>O sistema deverá aceitar o dado inserido no campo.</t>
   </si>
   <si>
-    <t>Preencher o campo de senha com uma senha válida.</t>
+    <t>Preencher o campo de Password com uma senha válida.</t>
   </si>
   <si>
     <t>Clicar no botão "Login"</t>
@@ -98,13 +98,13 @@
     <t>003</t>
   </si>
   <si>
-    <t>Preencher o campo de senha com a senha invalida.</t>
+    <t>Preencher o campo de Password com a senha invalida.</t>
   </si>
   <si>
     <t>004</t>
   </si>
   <si>
-    <t>Não preencher o campo de senha.</t>
+    <t>Não preencher o campo de Password.</t>
   </si>
   <si>
     <t>O sistema deverá aceitar deixar o campo em branco</t>
@@ -137,7 +137,7 @@
     <t>Preencher o campo de Username com mais de 255 caracteres.</t>
   </si>
   <si>
-    <t>Preencher o campo de senha com mais de 255 caracteres.</t>
+    <t>Preencher o campo de Password com mais de 255 caracteres.</t>
   </si>
   <si>
     <t>009</t>
@@ -146,7 +146,7 @@
     <t>Preencher o campo de Username com máximo de 3 caracteres.</t>
   </si>
   <si>
-    <t>Preencher o campo de senha com máximo de 3 caracteres.</t>
+    <t>Preencher o campo de Password com máximo de 3 caracteres.</t>
   </si>
   <si>
     <t>010</t>
@@ -158,7 +158,7 @@
     <t>011</t>
   </si>
   <si>
-    <t>Preencher o campo de senha com caracteres especiais</t>
+    <t>Preencher o campo de Password com caracteres especiais</t>
   </si>
   <si>
     <t>Adicionar o produto ao carrinho.</t>
@@ -1823,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2428,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
   <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -2948,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B30"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
docs: atualizado o cenario
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59F10922-A01A-4046-AC13-9C385E3B478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E37F01-C963-4E7F-940F-0C09D0B5A7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
-    <sheet name="PRODUCTS - YOUR CART" sheetId="2" r:id="rId2"/>
-    <sheet name="CHECKOUT - FINISH" sheetId="4" r:id="rId3"/>
+    <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
+    <sheet name="LOGIN" sheetId="1" r:id="rId2"/>
+    <sheet name="PRODUCTS - YOUR CART" sheetId="2" r:id="rId3"/>
+    <sheet name="CHECKOUT - FINISH" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,59 +34,149 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="118">
   <si>
     <t>Cenário</t>
   </si>
   <si>
+    <t>Processo completo de login, compra e finalização do pedido</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Para garantir uma experiência de compra bem-sucedida.</t>
+  </si>
+  <si>
+    <t>Requisito</t>
+  </si>
+  <si>
+    <t>Realizar login, selecionar produtos, finalizar a compra e deslogar</t>
+  </si>
+  <si>
+    <t>Caso de Teste</t>
+  </si>
+  <si>
+    <t>Passo</t>
+  </si>
+  <si>
+    <t>Descrição do Teste</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Username com um username valido.</t>
+  </si>
+  <si>
+    <t>O sistema deverá aceitar o dado inserido no campo.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Password com uma senha válida.</t>
+  </si>
+  <si>
+    <t>Clicar no botão "Login"</t>
+  </si>
+  <si>
+    <t>O usuário é redirecionada para tela 'Products'.</t>
+  </si>
+  <si>
+    <t>Identificar o produto desejado.</t>
+  </si>
+  <si>
+    <t>O usuario esta na tela de 'Product'. A imagem do produto, nome, descriação e preço estão visíveis.</t>
+  </si>
+  <si>
+    <t>Clicar no botão "ADD TO CART" do produto selecionado.</t>
+  </si>
+  <si>
+    <t>O produto é adicionado ao carrinho.</t>
+  </si>
+  <si>
+    <t>Verificar o número de itens no ícone do carrinho</t>
+  </si>
+  <si>
+    <t>O ícone do carrinho é atualizado com o produto adicionado, e visualmente alterado e o número de itens no carrinho é corretamente atualizado para 1 ou 2.</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'iconé do carrinho'</t>
+  </si>
+  <si>
+    <t>O usuário será redirecionado para a tela 'Your Cart'</t>
+  </si>
+  <si>
+    <t>Validar as quantidades, nomes e descrições dos produtos no carrinho.</t>
+  </si>
+  <si>
+    <t>As quantidades, nomes e descrições dos produtos no carrinho devem corresponder exatamente às selecionadas e exibidas na página de carrinho.</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'CHECKOUT'.</t>
+  </si>
+  <si>
+    <t>O usuário será redirecionado para a tela 'Checkout: Your Information'</t>
+  </si>
+  <si>
+    <t>Preencher o campo de FirstName com 'Ricardo'.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de LastName com 'Costa'.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Postal Code com o numero '90619-900'.</t>
+  </si>
+  <si>
+    <t>Clicar no botão "CONTINUE".</t>
+  </si>
+  <si>
+    <t>O usuario é redirecionada para tela 'Checkout: Overview'.</t>
+  </si>
+  <si>
+    <t>Verificar as quantidades, nomes e descrições dos produtos no checkout.</t>
+  </si>
+  <si>
+    <t>As quantidades, nomes e descrições dos produtos no checkout devem corresponder exatamente às selecionadas e exibidas na página.</t>
+  </si>
+  <si>
+    <t>Verificar a forma de pagamento, informação de envio, o valor total dos itens, o valor da taxa e o valor total geral.</t>
+  </si>
+  <si>
+    <t>A forma de pagamento, informação de envio, o valor total dos itens, o valor da taxa e o valor total geral devem corresponder exatamente e exibidas na página.</t>
+  </si>
+  <si>
+    <t>Clicar no botão "FINISH".</t>
+  </si>
+  <si>
+    <t>O usuario é redirecionada para tela 'FINISH'.</t>
+  </si>
+  <si>
+    <t>Verificar se o pedido foi realizado com sucesso.</t>
+  </si>
+  <si>
+    <t>O sistema exibirá a mensagem: "THANK YOU FOR YOUR ORDER".</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Logout'.</t>
+  </si>
+  <si>
+    <t>O usuario é redirecionada para tela de login.</t>
+  </si>
+  <si>
     <t>Login de Usuário</t>
   </si>
   <si>
-    <t>Objetivo</t>
-  </si>
-  <si>
     <t>Testar o fluxo dos campos obrigatórios e as mensagens de erro.</t>
   </si>
   <si>
-    <t>Requisito</t>
-  </si>
-  <si>
     <t>Validar os campos obrigatórios</t>
   </si>
   <si>
-    <t>Caso de Teste</t>
-  </si>
-  <si>
-    <t>Passo</t>
-  </si>
-  <si>
-    <t>Descrição do Teste</t>
-  </si>
-  <si>
-    <t>Resultado Esperado</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>Preencher o campo de Username com um username valido.</t>
-  </si>
-  <si>
-    <t>O sistema deverá aceitar o dado inserido no campo.</t>
-  </si>
-  <si>
-    <t>Preencher o campo de Password com uma senha válida.</t>
-  </si>
-  <si>
-    <t>Clicar no botão "Login"</t>
-  </si>
-  <si>
-    <t>O usuário é redirecionada para tela 'Products'.</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -173,40 +264,13 @@
     <t>Descriação do Teste</t>
   </si>
   <si>
-    <t>Identificar o produto desejado.</t>
-  </si>
-  <si>
-    <t>O usuario esta na tela de 'Product'. A imagem do produto, nome, descriação e preço estão visíveis.</t>
-  </si>
-  <si>
-    <t>Clicar no botão "ADD TO CART" do produto selecionado.</t>
-  </si>
-  <si>
-    <t>O produto é adicionado ao carrinho.</t>
-  </si>
-  <si>
-    <t>Verificar o número de itens no ícone do carrinho</t>
-  </si>
-  <si>
-    <t>O ícone do carrinho é atualizado com o produto adicionado, e visualmente alterado e o número de itens no carrinho é corretamente atualizado para 1 ou 2.</t>
-  </si>
-  <si>
-    <t>Clicar no botão 'iconé do carrinho'</t>
-  </si>
-  <si>
-    <t>O usuário será redirecionado para a tela 'Your Cart'</t>
-  </si>
-  <si>
-    <t>Validar as quantidades, nomes e descrições dos produtos no carrinho.</t>
-  </si>
-  <si>
-    <t>As quantidades, nomes e descrições dos produtos no carrinho devem corresponder exatamente às selecionadas e exibidas na página de carrinho.</t>
-  </si>
-  <si>
-    <t>Clicar no botão 'CHECKOUT'.</t>
-  </si>
-  <si>
-    <t>O usuário será redirecionado para a tela 'Checkout: Your Information'</t>
+    <t>O ícone do carrinho é atualizado com o produto adicionado, e visualmente alterado e o número de itens no carrinho é corretamente atualizado para 1.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de quantidade para '2'</t>
+  </si>
+  <si>
+    <t>O sistema deverá aceitar o número inserido no campo.</t>
   </si>
   <si>
     <t>Atualizar a pagina e o carrinho mantém os itens</t>
@@ -258,51 +322,6 @@
   </si>
   <si>
     <t xml:space="preserve">Validar os campos obrigatorios, </t>
-  </si>
-  <si>
-    <t>Preencher o campo de FirstName com 'Ricardo'.</t>
-  </si>
-  <si>
-    <t>Preencher o campo de LastName com 'Costa'.</t>
-  </si>
-  <si>
-    <t>Preencher o campo de Postal Code com o numero '90619-900'.</t>
-  </si>
-  <si>
-    <t>Clicar no botão "CONTINUE".</t>
-  </si>
-  <si>
-    <t>O usuario é redirecionada para tela 'Checkout: Overview'.</t>
-  </si>
-  <si>
-    <t>Verificar as quantidades, nomes e descrições dos produtos no checkout.</t>
-  </si>
-  <si>
-    <t>As quantidades, nomes e descrições dos produtos no checkout devem corresponder exatamente às selecionadas e exibidas na página.</t>
-  </si>
-  <si>
-    <t>Verificar a forma de pagamento, informação de envio, o valor total dos itens, o valor da taxa e o valor total geral.</t>
-  </si>
-  <si>
-    <t>A forma de pagamento, informação de envio, o valor total dos itens, o valor da taxa e o valor total geral devem corresponder exatamente e exibidas na página.</t>
-  </si>
-  <si>
-    <t>Clicar no botão "FINISH".</t>
-  </si>
-  <si>
-    <t>O usuario é redirecionada para tela 'FINISH'.</t>
-  </si>
-  <si>
-    <t>Verificar se o pedido foi realizado com sucesso.</t>
-  </si>
-  <si>
-    <t>O sistema exibirá a mensagem: "THANK YOU FOR YOUR ORDER".</t>
-  </si>
-  <si>
-    <t>Clicar no botão 'Logout'.</t>
-  </si>
-  <si>
-    <t>O usuario é redirecionada para tela de login.</t>
   </si>
   <si>
     <t>Não preencher o campo de FirstName.</t>
@@ -375,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +406,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1037,11 +1064,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1358,15 +1429,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1487,6 +1549,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1820,11 +1954,395 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
+  <dimension ref="B2:G30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="80"/>
+      <c r="E3" s="81"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="82"/>
+      <c r="E4" s="83"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="85"/>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="168" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="33">
+        <v>1</v>
+      </c>
+      <c r="D6" s="174" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="177"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="169"/>
+      <c r="C7" s="28">
+        <v>2</v>
+      </c>
+      <c r="D7" s="165" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="165"/>
+      <c r="F7" s="159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="171"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="169"/>
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="165" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="165"/>
+      <c r="F8" s="159" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="171"/>
+    </row>
+    <row r="9" spans="2:7" ht="29.25">
+      <c r="B9" s="169"/>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="166" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="166"/>
+      <c r="F9" s="157" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="171"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="169"/>
+      <c r="C10" s="28">
+        <v>5</v>
+      </c>
+      <c r="D10" s="167" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="166"/>
+      <c r="F10" s="158" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="171"/>
+    </row>
+    <row r="11" spans="2:7" ht="43.5">
+      <c r="B11" s="169"/>
+      <c r="C11" s="28">
+        <v>6</v>
+      </c>
+      <c r="D11" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="167"/>
+      <c r="F11" s="157" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="171"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="169"/>
+      <c r="C12" s="28">
+        <v>7</v>
+      </c>
+      <c r="D12" s="166" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="166"/>
+      <c r="F12" s="158" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="171"/>
+    </row>
+    <row r="13" spans="2:7" ht="43.5">
+      <c r="B13" s="169"/>
+      <c r="C13" s="28">
+        <v>8</v>
+      </c>
+      <c r="D13" s="167" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="167"/>
+      <c r="F13" s="157" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="171"/>
+    </row>
+    <row r="14" spans="2:7" ht="15" customHeight="1">
+      <c r="B14" s="169"/>
+      <c r="C14" s="28">
+        <v>9</v>
+      </c>
+      <c r="D14" s="166" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="166"/>
+      <c r="F14" s="157" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="171"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="169"/>
+      <c r="C15" s="28">
+        <v>10</v>
+      </c>
+      <c r="D15" s="165" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="165"/>
+      <c r="F15" s="159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="171"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="169"/>
+      <c r="C16" s="28">
+        <v>11</v>
+      </c>
+      <c r="D16" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="165"/>
+      <c r="F16" s="159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="171"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="169"/>
+      <c r="C17" s="28">
+        <v>12</v>
+      </c>
+      <c r="D17" s="165" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="165"/>
+      <c r="F17" s="159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="171"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="169"/>
+      <c r="C18" s="28">
+        <v>13</v>
+      </c>
+      <c r="D18" s="166" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="166"/>
+      <c r="F18" s="157" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="171"/>
+    </row>
+    <row r="19" spans="2:7" ht="43.5">
+      <c r="B19" s="169"/>
+      <c r="C19" s="28">
+        <v>14</v>
+      </c>
+      <c r="D19" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="167"/>
+      <c r="F19" s="157" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="171"/>
+    </row>
+    <row r="20" spans="2:7" ht="43.5">
+      <c r="B20" s="169"/>
+      <c r="C20" s="28">
+        <v>15</v>
+      </c>
+      <c r="D20" s="167" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="167"/>
+      <c r="F20" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="171"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="169"/>
+      <c r="C21" s="28">
+        <v>16</v>
+      </c>
+      <c r="D21" s="165" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="165"/>
+      <c r="F21" s="172" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="171"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="169"/>
+      <c r="C22" s="28">
+        <v>17</v>
+      </c>
+      <c r="D22" s="166" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="166"/>
+      <c r="F22" s="172" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="171"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="170"/>
+      <c r="C23" s="20">
+        <v>18</v>
+      </c>
+      <c r="D23" s="173" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="173"/>
+      <c r="F23" s="172" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="171"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="D25" s="164"/>
+      <c r="E25" s="164"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" s="164"/>
+      <c r="E28" s="164"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B6:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1842,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D2" s="78"/>
       <c r="E2" s="79"/>
@@ -1852,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="81"/>
@@ -1862,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D4" s="82"/>
       <c r="E4" s="83"/>
@@ -1931,13 +2449,13 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="68" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C9" s="24">
         <v>1</v>
       </c>
       <c r="D9" s="71" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E9" s="72"/>
       <c r="F9" s="9" t="s">
@@ -1969,13 +2487,13 @@
       </c>
       <c r="E11" s="76"/>
       <c r="F11" s="19" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="68" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C12" s="24">
         <v>1</v>
@@ -1995,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="73" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E13" s="74"/>
       <c r="F13" s="11" t="s">
@@ -2013,13 +2531,13 @@
       </c>
       <c r="E14" s="76"/>
       <c r="F14" s="19" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="68" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C15" s="24">
         <v>1</v>
@@ -2039,11 +2557,11 @@
         <v>2</v>
       </c>
       <c r="D16" s="73" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E16" s="74"/>
       <c r="F16" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G16" s="12"/>
     </row>
@@ -2057,23 +2575,23 @@
       </c>
       <c r="E17" s="87"/>
       <c r="F17" s="16" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="68" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C18" s="24">
         <v>1</v>
       </c>
       <c r="D18" s="71" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E18" s="72"/>
       <c r="F18" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G18" s="15"/>
     </row>
@@ -2101,23 +2619,23 @@
       </c>
       <c r="E20" s="87"/>
       <c r="F20" s="16" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="68" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C21" s="24">
         <v>1</v>
       </c>
       <c r="D21" s="71" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E21" s="72"/>
       <c r="F21" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G21" s="15"/>
     </row>
@@ -2127,11 +2645,11 @@
         <v>2</v>
       </c>
       <c r="D22" s="73" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E22" s="74"/>
       <c r="F22" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G22" s="12"/>
     </row>
@@ -2145,19 +2663,19 @@
       </c>
       <c r="E23" s="89"/>
       <c r="F23" s="8" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="68" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C24" s="24">
         <v>1</v>
       </c>
       <c r="D24" s="71" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E24" s="72"/>
       <c r="F24" s="9" t="s">
@@ -2171,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="73" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E25" s="74"/>
       <c r="F25" s="11" t="s">
@@ -2189,19 +2707,19 @@
       </c>
       <c r="E26" s="76"/>
       <c r="F26" s="26" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="68" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C27" s="24">
         <v>1</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E27" s="72"/>
       <c r="F27" s="9" t="s">
@@ -2215,7 +2733,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E28" s="74"/>
       <c r="F28" s="11" t="s">
@@ -2233,19 +2751,19 @@
       </c>
       <c r="E29" s="76"/>
       <c r="F29" s="26" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G29" s="17"/>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="68" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C30" s="24">
         <v>1</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="E30" s="72"/>
       <c r="F30" s="9" t="s">
@@ -2259,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="73" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="E31" s="74"/>
       <c r="F31" s="11" t="s">
@@ -2277,19 +2795,19 @@
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="26" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G32" s="17"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="68" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C33" s="24">
         <v>1</v>
       </c>
       <c r="D33" s="71" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E33" s="72"/>
       <c r="F33" s="9" t="s">
@@ -2327,7 +2845,7 @@
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="68" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C36" s="24">
         <v>1</v>
@@ -2347,7 +2865,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="73" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E37" s="74"/>
       <c r="F37" s="11" t="s">
@@ -2424,12 +2942,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
-  <dimension ref="B2:G42"/>
+  <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2447,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="93" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D2" s="94"/>
       <c r="E2" s="95"/>
@@ -2457,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="D3" s="100"/>
       <c r="E3" s="101"/>
@@ -2467,7 +2985,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="99" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D4" s="100"/>
       <c r="E4" s="101"/>
@@ -2479,10 +2997,10 @@
       <c r="C5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="115" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="116"/>
+      <c r="D5" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="113"/>
       <c r="F5" s="29" t="s">
         <v>9</v>
       </c>
@@ -2491,432 +3009,547 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="29.25">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="90" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="45">
         <v>1</v>
       </c>
       <c r="D6" s="106" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="E6" s="107"/>
       <c r="F6" s="48" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="113"/>
+      <c r="B7" s="91"/>
       <c r="C7" s="28">
         <v>2</v>
       </c>
       <c r="D7" s="110" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="117"/>
+        <v>19</v>
+      </c>
+      <c r="E7" s="114"/>
       <c r="F7" s="28" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7" ht="43.5">
-      <c r="B8" s="113"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
       <c r="D8" s="110" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E8" s="111"/>
       <c r="F8" s="44" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="113"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D9" s="118" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="117"/>
+      <c r="D9" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="114"/>
       <c r="F9" s="28" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="2:7" ht="43.5">
-      <c r="B10" s="113"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="28">
         <v>5</v>
       </c>
       <c r="D10" s="110" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E10" s="111"/>
       <c r="F10" s="44" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="114"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="20">
         <v>6</v>
       </c>
-      <c r="D11" s="119" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="120"/>
-      <c r="F11" s="54" t="s">
-        <v>57</v>
+      <c r="D11" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="117"/>
+      <c r="F11" s="156" t="s">
+        <v>28</v>
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="13" spans="2:7" ht="15" customHeight="1"/>
+    <row r="12" spans="2:7" ht="29.25">
+      <c r="B12" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="57">
+        <v>1</v>
+      </c>
+      <c r="D12" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="107"/>
+      <c r="F12" s="160" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" customHeight="1">
+      <c r="B13" s="91"/>
+      <c r="C13" s="40">
+        <v>2</v>
+      </c>
+      <c r="D13" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="114"/>
+      <c r="F13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" ht="43.5">
+      <c r="B14" s="91"/>
+      <c r="C14" s="40">
+        <v>3</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="111"/>
+      <c r="F14" s="161" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="12"/>
+    </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="91"/>
+      <c r="C15" s="40">
+        <v>4</v>
+      </c>
+      <c r="D15" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="114"/>
+      <c r="F15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="91"/>
+      <c r="C16" s="40">
+        <v>5</v>
+      </c>
+      <c r="D16" s="108" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="155"/>
+      <c r="F16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7" ht="43.5">
+      <c r="B17" s="91"/>
+      <c r="C17" s="40">
+        <v>6</v>
+      </c>
+      <c r="D17" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="111"/>
+      <c r="F17" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="2:7" ht="29.25">
+      <c r="B18" s="92"/>
+      <c r="C18" s="50">
+        <v>7</v>
+      </c>
+      <c r="D18" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="117"/>
+      <c r="F18" s="162" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="163"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="153"/>
+      <c r="G19" s="154"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="93" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="95"/>
-    </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1">
-      <c r="B16" s="2" t="s">
+      <c r="C23" s="93" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="100"/>
-      <c r="E16" s="101"/>
-    </row>
-    <row r="17" spans="2:7" ht="15" customHeight="1">
-      <c r="B17" s="42" t="s">
+      <c r="C24" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="100"/>
+      <c r="E24" s="101"/>
+    </row>
+    <row r="25" spans="2:7" ht="15" customHeight="1">
+      <c r="B25" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="100"/>
-      <c r="E17" s="101"/>
-    </row>
-    <row r="18" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B18" s="2" t="s">
+      <c r="C25" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="100"/>
+      <c r="E25" s="101"/>
+    </row>
+    <row r="26" spans="2:7" ht="29.25" customHeight="1">
+      <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="29" t="s">
+      <c r="D26" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="85"/>
+      <c r="F26" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G26" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="29.25">
-      <c r="B19" s="90" t="s">
+    <row r="27" spans="2:7" ht="29.25">
+      <c r="B27" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C27" s="33">
         <v>1</v>
       </c>
-      <c r="D19" s="102" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="103"/>
-      <c r="F19" s="39" t="s">
+      <c r="D27" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="103"/>
+      <c r="F27" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="36"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="91"/>
+      <c r="C28" s="23">
+        <v>2</v>
+      </c>
+      <c r="D28" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="105"/>
+      <c r="F28" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" spans="2:7" ht="29.25" customHeight="1">
+      <c r="B29" s="91"/>
+      <c r="C29" s="23">
+        <v>3</v>
+      </c>
+      <c r="D29" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="105"/>
+      <c r="F29" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="91"/>
+      <c r="C30" s="23">
+        <v>4</v>
+      </c>
+      <c r="D30" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="109"/>
+      <c r="F30" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" spans="2:7" ht="43.5">
+      <c r="B31" s="91"/>
+      <c r="C31" s="34">
+        <v>5</v>
+      </c>
+      <c r="D31" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="111"/>
+      <c r="F31" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="37"/>
+    </row>
+    <row r="32" spans="2:7" ht="29.25">
+      <c r="B32" s="92"/>
+      <c r="C32" s="35">
+        <v>6</v>
+      </c>
+      <c r="D32" s="118" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="119"/>
+      <c r="F32" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="38"/>
+    </row>
+    <row r="35" spans="2:7" ht="15" customHeight="1"/>
+    <row r="36" spans="2:7">
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="94"/>
+      <c r="E36" s="95"/>
+    </row>
+    <row r="37" spans="2:7" ht="28.5" customHeight="1">
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="100"/>
+      <c r="E37" s="101"/>
+    </row>
+    <row r="38" spans="2:7" ht="48" customHeight="1">
+      <c r="B38" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="97"/>
+      <c r="E38" s="98"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="85"/>
+      <c r="F39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="29.25">
+      <c r="B40" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="30">
+        <v>1</v>
+      </c>
+      <c r="D40" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="103"/>
+      <c r="F40" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="91"/>
+      <c r="C41" s="28">
+        <v>2</v>
+      </c>
+      <c r="D41" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="105"/>
+      <c r="F41" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="2:7" ht="15" customHeight="1">
+      <c r="B42" s="91"/>
+      <c r="C42" s="28">
+        <v>3</v>
+      </c>
+      <c r="D42" s="108" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="109"/>
+      <c r="F42" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1">
+      <c r="B43" s="92"/>
+      <c r="C43" s="64">
+        <v>4</v>
+      </c>
+      <c r="D43" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="121"/>
+      <c r="F43" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="2:7" ht="29.25">
+      <c r="B44" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="36"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="91"/>
-      <c r="C20" s="23">
+      <c r="C44" s="57">
+        <v>1</v>
+      </c>
+      <c r="D44" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="103"/>
+      <c r="F44" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="36"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="91"/>
+      <c r="C45" s="40">
         <v>2</v>
       </c>
-      <c r="D20" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="105"/>
-      <c r="F20" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="37"/>
-    </row>
-    <row r="21" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B21" s="91"/>
-      <c r="C21" s="23">
+      <c r="D45" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="105"/>
+      <c r="F45" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="37"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="91"/>
+      <c r="C46" s="40">
         <v>3</v>
       </c>
-      <c r="D21" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="37"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="91"/>
-      <c r="C22" s="23">
+      <c r="D46" s="108" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="109"/>
+      <c r="F46" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="37"/>
+    </row>
+    <row r="47" spans="2:7" ht="43.5">
+      <c r="B47" s="91"/>
+      <c r="C47" s="40">
         <v>4</v>
       </c>
-      <c r="D22" s="108" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="109"/>
-      <c r="F22" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="2:7" ht="43.5">
-      <c r="B23" s="91"/>
-      <c r="C23" s="34">
+      <c r="D47" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="109"/>
+      <c r="F47" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="G47" s="37"/>
+    </row>
+    <row r="48" spans="2:7" ht="35.25" customHeight="1">
+      <c r="B48" s="92"/>
+      <c r="C48" s="50">
         <v>5</v>
       </c>
-      <c r="D23" s="110" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="111"/>
-      <c r="F23" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="37"/>
-    </row>
-    <row r="24" spans="2:7" ht="29.25">
-      <c r="B24" s="92"/>
-      <c r="C24" s="35">
-        <v>6</v>
-      </c>
-      <c r="D24" s="121" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="122"/>
-      <c r="F24" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="38"/>
-    </row>
-    <row r="27" spans="2:7" ht="15" customHeight="1"/>
-    <row r="28" spans="2:7">
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="93" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="94"/>
-      <c r="E28" s="95"/>
-    </row>
-    <row r="29" spans="2:7" ht="28.5" customHeight="1">
-      <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-    </row>
-    <row r="30" spans="2:7" ht="48" customHeight="1">
-      <c r="B30" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="96" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="97"/>
-      <c r="E30" s="98"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="85"/>
-      <c r="F31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="30">
-        <v>1</v>
-      </c>
-      <c r="D32" s="102" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="103"/>
-      <c r="F32" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="91"/>
-      <c r="C33" s="28">
-        <v>2</v>
-      </c>
-      <c r="D33" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="105"/>
-      <c r="F33" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="2:7" ht="15" customHeight="1">
-      <c r="B34" s="91"/>
-      <c r="C34" s="28">
-        <v>3</v>
-      </c>
-      <c r="D34" s="108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="109"/>
-      <c r="F34" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1">
-      <c r="B35" s="92"/>
-      <c r="C35" s="64">
-        <v>4</v>
-      </c>
-      <c r="D35" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="124"/>
-      <c r="F35" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="2:7" ht="29.25">
-      <c r="B36" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="57">
-        <v>1</v>
-      </c>
-      <c r="D36" s="102" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="103"/>
-      <c r="F36" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" s="36"/>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="91"/>
-      <c r="C37" s="40">
-        <v>2</v>
-      </c>
-      <c r="D37" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="105"/>
-      <c r="F37" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="37"/>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="91"/>
-      <c r="C38" s="40">
-        <v>3</v>
-      </c>
-      <c r="D38" s="108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="109"/>
-      <c r="F38" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="37"/>
-    </row>
-    <row r="39" spans="2:7" ht="43.5">
-      <c r="B39" s="91"/>
-      <c r="C39" s="40">
-        <v>4</v>
-      </c>
-      <c r="D39" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="109"/>
-      <c r="F39" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="37"/>
-    </row>
-    <row r="40" spans="2:7" ht="35.25" customHeight="1">
-      <c r="B40" s="92"/>
-      <c r="C40" s="50">
-        <v>5</v>
-      </c>
-      <c r="D40" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="124"/>
-      <c r="F40" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="G40" s="38"/>
-    </row>
-    <row r="41" spans="2:7">
-      <c r="D41" s="123"/>
-      <c r="E41" s="123"/>
-    </row>
-    <row r="42" spans="2:7">
-      <c r="D42" s="123"/>
-      <c r="E42" s="123"/>
+      <c r="D48" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="121"/>
+      <c r="F48" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="38"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="120"/>
+      <c r="E49" s="120"/>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="120"/>
+      <c r="E50" s="120"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="C17:E17"/>
+  <mergeCells count="47">
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
@@ -2927,29 +3560,29 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2966,18 +3599,18 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="147" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="148"/>
-      <c r="E2" s="149"/>
+      <c r="C2" s="144" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="145"/>
+      <c r="E2" s="146"/>
     </row>
     <row r="3" spans="2:7" ht="30" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D3" s="82"/>
       <c r="E3" s="83"/>
@@ -2987,7 +3620,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D4" s="82"/>
       <c r="E4" s="83"/>
@@ -2999,10 +3632,10 @@
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="150" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="116"/>
+      <c r="D5" s="147" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="113"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3017,10 +3650,10 @@
       <c r="C6" s="57">
         <v>1</v>
       </c>
-      <c r="D6" s="132" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="138"/>
+      <c r="D6" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="135"/>
       <c r="F6" s="46" t="s">
         <v>13</v>
       </c>
@@ -3031,10 +3664,10 @@
       <c r="C7" s="40">
         <v>2</v>
       </c>
-      <c r="D7" s="126" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="135"/>
+      <c r="D7" s="123" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="132"/>
       <c r="F7" s="47" t="s">
         <v>13</v>
       </c>
@@ -3045,10 +3678,10 @@
       <c r="C8" s="40">
         <v>3</v>
       </c>
-      <c r="D8" s="126" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="135"/>
+      <c r="D8" s="123" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="132"/>
       <c r="F8" s="47" t="s">
         <v>13</v>
       </c>
@@ -3059,12 +3692,12 @@
       <c r="C9" s="40">
         <v>4</v>
       </c>
-      <c r="D9" s="118" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="117"/>
+      <c r="D9" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="114"/>
       <c r="F9" s="44" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="G9" s="37"/>
     </row>
@@ -3074,11 +3707,11 @@
         <v>5</v>
       </c>
       <c r="D10" s="110" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="E10" s="111"/>
       <c r="F10" s="44" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="G10" s="37"/>
     </row>
@@ -3088,11 +3721,11 @@
         <v>6</v>
       </c>
       <c r="D11" s="110" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E11" s="111"/>
       <c r="F11" s="44" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="G11" s="37"/>
     </row>
@@ -3101,12 +3734,12 @@
       <c r="C12" s="40">
         <v>7</v>
       </c>
-      <c r="D12" s="126" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="135"/>
+      <c r="D12" s="123" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="132"/>
       <c r="F12" s="56" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="G12" s="37"/>
     </row>
@@ -3115,12 +3748,12 @@
       <c r="C13" s="40">
         <v>8</v>
       </c>
-      <c r="D13" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="117"/>
+      <c r="D13" s="115" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="114"/>
       <c r="F13" s="56" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="G13" s="37"/>
     </row>
@@ -3129,28 +3762,28 @@
       <c r="C14" s="60">
         <v>9</v>
       </c>
-      <c r="D14" s="152" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="153"/>
+      <c r="D14" s="149" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="150"/>
       <c r="F14" s="59" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="G14" s="58"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="90" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C15" s="33">
         <v>1</v>
       </c>
-      <c r="D15" s="151" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="138"/>
+      <c r="D15" s="148" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="135"/>
       <c r="F15" s="9" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G15" s="15"/>
     </row>
@@ -3159,12 +3792,12 @@
       <c r="C16" s="23">
         <v>2</v>
       </c>
-      <c r="D16" s="134" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="135"/>
+      <c r="D16" s="131" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="132"/>
       <c r="F16" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G16" s="12"/>
     </row>
@@ -3173,12 +3806,12 @@
       <c r="C17" s="23">
         <v>3</v>
       </c>
-      <c r="D17" s="136" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="137"/>
+      <c r="D17" s="133" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="134"/>
       <c r="F17" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G17" s="12"/>
     </row>
@@ -3187,26 +3820,26 @@
       <c r="C18" s="35">
         <v>4</v>
       </c>
-      <c r="D18" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="120"/>
+      <c r="D18" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="117"/>
       <c r="F18" s="55" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="G18" s="17"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="90" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C19" s="33">
         <v>1</v>
       </c>
-      <c r="D19" s="132" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="138"/>
+      <c r="D19" s="129" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="135"/>
       <c r="F19" s="65" t="s">
         <v>13</v>
       </c>
@@ -3217,12 +3850,12 @@
       <c r="C20" s="23">
         <v>2</v>
       </c>
-      <c r="D20" s="134" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="135"/>
+      <c r="D20" s="131" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="132"/>
       <c r="F20" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G20" s="12"/>
     </row>
@@ -3231,12 +3864,12 @@
       <c r="C21" s="23">
         <v>3</v>
       </c>
-      <c r="D21" s="136" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="137"/>
+      <c r="D21" s="133" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="134"/>
       <c r="F21" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G21" s="12"/>
     </row>
@@ -3245,28 +3878,28 @@
       <c r="C22" s="35">
         <v>4</v>
       </c>
-      <c r="D22" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="120"/>
+      <c r="D22" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="117"/>
       <c r="F22" s="55" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="90" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C23" s="33">
         <v>1</v>
       </c>
-      <c r="D23" s="132" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="138"/>
+      <c r="D23" s="129" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="135"/>
       <c r="F23" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G23" s="15"/>
     </row>
@@ -3275,10 +3908,10 @@
       <c r="C24" s="23">
         <v>2</v>
       </c>
-      <c r="D24" s="134" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="135"/>
+      <c r="D24" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="132"/>
       <c r="F24" s="11" t="s">
         <v>13</v>
       </c>
@@ -3289,12 +3922,12 @@
       <c r="C25" s="23">
         <v>3</v>
       </c>
-      <c r="D25" s="136" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="137"/>
+      <c r="D25" s="133" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="134"/>
       <c r="F25" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G25" s="12"/>
     </row>
@@ -3303,28 +3936,28 @@
       <c r="C26" s="35">
         <v>4</v>
       </c>
-      <c r="D26" s="131" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="120"/>
+      <c r="D26" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="117"/>
       <c r="F26" s="55" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="90" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C27" s="52">
         <v>1</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="154"/>
+        <v>96</v>
+      </c>
+      <c r="E27" s="151"/>
       <c r="F27" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G27" s="15"/>
     </row>
@@ -3333,12 +3966,12 @@
       <c r="C28" s="51">
         <v>2</v>
       </c>
-      <c r="D28" s="134" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="135"/>
+      <c r="D28" s="131" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="132"/>
       <c r="F28" s="18" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G28" s="12"/>
     </row>
@@ -3347,10 +3980,10 @@
       <c r="C29" s="51">
         <v>3</v>
       </c>
-      <c r="D29" s="136" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="137"/>
+      <c r="D29" s="133" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="134"/>
       <c r="F29" s="23" t="s">
         <v>13</v>
       </c>
@@ -3361,26 +3994,26 @@
       <c r="C30" s="53">
         <v>4</v>
       </c>
-      <c r="D30" s="131" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="120"/>
+      <c r="D30" s="128" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="117"/>
       <c r="F30" s="55" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G30" s="17"/>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="91" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C31" s="33">
         <v>1</v>
       </c>
-      <c r="D31" s="132" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="138"/>
+      <c r="D31" s="129" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="135"/>
       <c r="F31" s="9" t="s">
         <v>13</v>
       </c>
@@ -3391,10 +4024,10 @@
       <c r="C32" s="23">
         <v>2</v>
       </c>
-      <c r="D32" s="132" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="138"/>
+      <c r="D32" s="129" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="135"/>
       <c r="F32" s="11" t="s">
         <v>13</v>
       </c>
@@ -3405,10 +4038,10 @@
       <c r="C33" s="23">
         <v>3</v>
       </c>
-      <c r="D33" s="139" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="140"/>
+      <c r="D33" s="136" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="137"/>
       <c r="F33" s="23" t="s">
         <v>13</v>
       </c>
@@ -3419,26 +4052,26 @@
       <c r="C34" s="35">
         <v>4</v>
       </c>
-      <c r="D34" s="141" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="142"/>
+      <c r="D34" s="138" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="139"/>
       <c r="F34" s="55" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="G34" s="17"/>
     </row>
     <row r="35" spans="2:7" ht="31.5" customHeight="1">
       <c r="B35" s="90" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C35" s="45">
         <v>1</v>
       </c>
-      <c r="D35" s="143" t="s">
-        <v>105</v>
-      </c>
-      <c r="E35" s="144"/>
+      <c r="D35" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="141"/>
       <c r="F35" s="52" t="s">
         <v>13</v>
       </c>
@@ -3449,10 +4082,10 @@
       <c r="C36" s="28">
         <v>2</v>
       </c>
-      <c r="D36" s="128" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="129"/>
+      <c r="D36" s="125" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="126"/>
       <c r="F36" s="51" t="s">
         <v>13</v>
       </c>
@@ -3463,10 +4096,10 @@
       <c r="C37" s="28">
         <v>3</v>
       </c>
-      <c r="D37" s="128" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="129"/>
+      <c r="D37" s="125" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="126"/>
       <c r="F37" s="51" t="s">
         <v>13</v>
       </c>
@@ -3477,26 +4110,26 @@
       <c r="C38" s="20">
         <v>4</v>
       </c>
-      <c r="D38" s="145" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="146"/>
+      <c r="D38" s="142" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="143"/>
       <c r="F38" s="63" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G38" s="17"/>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
       <c r="B39" s="91" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C39" s="45">
         <v>1</v>
       </c>
-      <c r="D39" s="132" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="133"/>
+      <c r="D39" s="129" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="130"/>
       <c r="F39" s="61" t="s">
         <v>13</v>
       </c>
@@ -3507,10 +4140,10 @@
       <c r="C40" s="28">
         <v>2</v>
       </c>
-      <c r="D40" s="126" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="127"/>
+      <c r="D40" s="123" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="124"/>
       <c r="F40" s="62" t="s">
         <v>13</v>
       </c>
@@ -3521,10 +4154,10 @@
       <c r="C41" s="28">
         <v>3</v>
       </c>
-      <c r="D41" s="128" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="129"/>
+      <c r="D41" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="126"/>
       <c r="F41" s="51" t="s">
         <v>13</v>
       </c>
@@ -3535,178 +4168,178 @@
       <c r="C42" s="20">
         <v>4</v>
       </c>
-      <c r="D42" s="119" t="s">
-        <v>100</v>
-      </c>
-      <c r="E42" s="130"/>
+      <c r="D42" s="116" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="127"/>
       <c r="F42" s="63" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="D43" s="125"/>
-      <c r="E43" s="125"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="122"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="D45" s="125"/>
-      <c r="E45" s="125"/>
+      <c r="D45" s="122"/>
+      <c r="E45" s="122"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="D46" s="125"/>
-      <c r="E46" s="125"/>
+      <c r="D46" s="122"/>
+      <c r="E46" s="122"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="D47" s="125"/>
-      <c r="E47" s="125"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="122"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="D48" s="125"/>
-      <c r="E48" s="125"/>
+      <c r="D48" s="122"/>
+      <c r="E48" s="122"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="125"/>
-      <c r="E49" s="125"/>
+      <c r="D49" s="122"/>
+      <c r="E49" s="122"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="125"/>
-      <c r="E50" s="125"/>
+      <c r="D50" s="122"/>
+      <c r="E50" s="122"/>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="125"/>
-      <c r="E51" s="125"/>
+      <c r="D51" s="122"/>
+      <c r="E51" s="122"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="125"/>
-      <c r="E52" s="125"/>
+      <c r="D52" s="122"/>
+      <c r="E52" s="122"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="125"/>
-      <c r="E53" s="125"/>
+      <c r="D53" s="122"/>
+      <c r="E53" s="122"/>
     </row>
     <row r="54" spans="4:5">
-      <c r="D54" s="125"/>
-      <c r="E54" s="125"/>
+      <c r="D54" s="122"/>
+      <c r="E54" s="122"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="125"/>
-      <c r="E55" s="125"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
     </row>
     <row r="56" spans="4:5">
-      <c r="D56" s="125"/>
-      <c r="E56" s="125"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="122"/>
     </row>
     <row r="57" spans="4:5">
-      <c r="D57" s="125"/>
-      <c r="E57" s="125"/>
+      <c r="D57" s="122"/>
+      <c r="E57" s="122"/>
     </row>
     <row r="58" spans="4:5">
-      <c r="D58" s="125"/>
-      <c r="E58" s="125"/>
+      <c r="D58" s="122"/>
+      <c r="E58" s="122"/>
     </row>
     <row r="59" spans="4:5">
-      <c r="D59" s="125"/>
-      <c r="E59" s="125"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="122"/>
     </row>
     <row r="60" spans="4:5">
-      <c r="D60" s="125"/>
-      <c r="E60" s="125"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="122"/>
     </row>
     <row r="61" spans="4:5">
-      <c r="D61" s="125"/>
-      <c r="E61" s="125"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="122"/>
     </row>
     <row r="62" spans="4:5">
-      <c r="D62" s="125"/>
-      <c r="E62" s="125"/>
+      <c r="D62" s="122"/>
+      <c r="E62" s="122"/>
     </row>
     <row r="63" spans="4:5">
-      <c r="D63" s="125"/>
-      <c r="E63" s="125"/>
+      <c r="D63" s="122"/>
+      <c r="E63" s="122"/>
     </row>
     <row r="64" spans="4:5">
-      <c r="D64" s="125"/>
-      <c r="E64" s="125"/>
+      <c r="D64" s="122"/>
+      <c r="E64" s="122"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="125"/>
-      <c r="E65" s="125"/>
+      <c r="D65" s="122"/>
+      <c r="E65" s="122"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="125"/>
-      <c r="E66" s="125"/>
+      <c r="D66" s="122"/>
+      <c r="E66" s="122"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="125"/>
-      <c r="E67" s="125"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="122"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="125"/>
-      <c r="E68" s="125"/>
+      <c r="D68" s="122"/>
+      <c r="E68" s="122"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="125"/>
-      <c r="E69" s="125"/>
+      <c r="D69" s="122"/>
+      <c r="E69" s="122"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="125"/>
-      <c r="E70" s="125"/>
+      <c r="D70" s="122"/>
+      <c r="E70" s="122"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="125"/>
-      <c r="E71" s="125"/>
+      <c r="D71" s="122"/>
+      <c r="E71" s="122"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="125"/>
-      <c r="E72" s="125"/>
+      <c r="D72" s="122"/>
+      <c r="E72" s="122"/>
     </row>
     <row r="73" spans="4:5">
-      <c r="D73" s="125"/>
-      <c r="E73" s="125"/>
+      <c r="D73" s="122"/>
+      <c r="E73" s="122"/>
     </row>
     <row r="74" spans="4:5">
-      <c r="D74" s="125"/>
-      <c r="E74" s="125"/>
+      <c r="D74" s="122"/>
+      <c r="E74" s="122"/>
     </row>
     <row r="75" spans="4:5">
-      <c r="D75" s="125"/>
-      <c r="E75" s="125"/>
+      <c r="D75" s="122"/>
+      <c r="E75" s="122"/>
     </row>
     <row r="76" spans="4:5">
-      <c r="D76" s="125"/>
-      <c r="E76" s="125"/>
+      <c r="D76" s="122"/>
+      <c r="E76" s="122"/>
     </row>
     <row r="77" spans="4:5">
-      <c r="D77" s="125"/>
-      <c r="E77" s="125"/>
+      <c r="D77" s="122"/>
+      <c r="E77" s="122"/>
     </row>
     <row r="78" spans="4:5">
-      <c r="D78" s="125"/>
-      <c r="E78" s="125"/>
+      <c r="D78" s="122"/>
+      <c r="E78" s="122"/>
     </row>
     <row r="79" spans="4:5">
-      <c r="D79" s="125"/>
-      <c r="E79" s="125"/>
+      <c r="D79" s="122"/>
+      <c r="E79" s="122"/>
     </row>
     <row r="80" spans="4:5">
-      <c r="D80" s="125"/>
-      <c r="E80" s="125"/>
+      <c r="D80" s="122"/>
+      <c r="E80" s="122"/>
     </row>
     <row r="81" spans="4:5">
-      <c r="D81" s="125"/>
-      <c r="E81" s="125"/>
+      <c r="D81" s="122"/>
+      <c r="E81" s="122"/>
     </row>
     <row r="82" spans="4:5">
-      <c r="D82" s="125"/>
-      <c r="E82" s="125"/>
+      <c r="D82" s="122"/>
+      <c r="E82" s="122"/>
     </row>
     <row r="83" spans="4:5">
-      <c r="D83" s="125"/>
-      <c r="E83" s="125"/>
+      <c r="D83" s="122"/>
+      <c r="E83" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="90">

</xml_diff>

<commit_message>
test: login ate realizar a compra com sucesso.
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E37F01-C963-4E7F-940F-0C09D0B5A7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{001B39F3-9D75-4316-B1DF-A3B26B63972A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="119">
   <si>
     <t>Cenário</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>O sistema deverá aceitar o dado inserido no campo.</t>
+  </si>
+  <si>
+    <t>passou</t>
   </si>
   <si>
     <t>Preencher o campo de Password com uma senha válida.</t>
@@ -439,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1065,26 +1068,15 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1092,19 +1084,10 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1112,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1297,6 +1280,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1324,33 +1397,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1363,6 +1409,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1370,6 +1434,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1390,237 +1490,93 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1957,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E19"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1968,37 +1924,38 @@
     <col min="3" max="3" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="81"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="93"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="49" t="s">
@@ -2007,301 +1964,351 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="95"/>
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="168" t="s">
+      <c r="B6" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="45">
         <v>1</v>
       </c>
-      <c r="D6" s="174" t="s">
+      <c r="D6" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="175"/>
-      <c r="F6" s="176" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="177"/>
+      <c r="G6" s="33" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="169"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="28">
         <v>2</v>
       </c>
-      <c r="D7" s="165" t="s">
+      <c r="D7" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="80"/>
+      <c r="F7" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="165"/>
-      <c r="F7" s="159" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="171"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="169"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
-      <c r="D8" s="165" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="165"/>
-      <c r="F8" s="159" t="s">
+      <c r="D8" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="171"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="29.25">
-      <c r="B9" s="169"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D9" s="166" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="166"/>
-      <c r="F9" s="157" t="s">
+      <c r="D9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="171"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="169"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="28">
         <v>5</v>
       </c>
-      <c r="D10" s="167" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="166"/>
-      <c r="F10" s="158" t="s">
+      <c r="D10" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="171"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="169"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="28">
         <v>6</v>
       </c>
-      <c r="D11" s="167" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="167"/>
-      <c r="F11" s="157" t="s">
+      <c r="D11" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="171"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="169"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="28">
         <v>7</v>
       </c>
-      <c r="D12" s="166" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="166"/>
-      <c r="F12" s="158" t="s">
+      <c r="D12" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="171"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="43.5">
-      <c r="B13" s="169"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="28">
         <v>8</v>
       </c>
-      <c r="D13" s="167" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="157" t="s">
+      <c r="D13" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="171"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1">
-      <c r="B14" s="169"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="28">
         <v>9</v>
       </c>
-      <c r="D14" s="166" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="166"/>
-      <c r="F14" s="157" t="s">
+      <c r="D14" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="171"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="169"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="28">
         <v>10</v>
       </c>
-      <c r="D15" s="165" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="165"/>
-      <c r="F15" s="159" t="s">
+      <c r="D15" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="80"/>
+      <c r="F15" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="171"/>
+      <c r="G15" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="169"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="28">
         <v>11</v>
       </c>
-      <c r="D16" s="165" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="165"/>
-      <c r="F16" s="159" t="s">
+      <c r="D16" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="80"/>
+      <c r="F16" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="171"/>
+      <c r="G16" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="169"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="28">
         <v>12</v>
       </c>
-      <c r="D17" s="165" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="165"/>
-      <c r="F17" s="159" t="s">
+      <c r="D17" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="80"/>
+      <c r="F17" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="171"/>
+      <c r="G17" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="169"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="28">
         <v>13</v>
       </c>
-      <c r="D18" s="166" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="157" t="s">
+      <c r="D18" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="171"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="43.5">
-      <c r="B19" s="169"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="28">
         <v>14</v>
       </c>
-      <c r="D19" s="167" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="167"/>
-      <c r="F19" s="157" t="s">
+      <c r="D19" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="171"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="43.5">
-      <c r="B20" s="169"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="28">
         <v>15</v>
       </c>
-      <c r="D20" s="167" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="167"/>
-      <c r="F20" s="157" t="s">
+      <c r="D20" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="171"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="169"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="28">
         <v>16</v>
       </c>
-      <c r="D21" s="165" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="165"/>
-      <c r="F21" s="172" t="s">
+      <c r="D21" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="171"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="169"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="28">
         <v>17</v>
       </c>
-      <c r="D22" s="166" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="166"/>
-      <c r="F22" s="172" t="s">
+      <c r="D22" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="171"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="170"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="20">
         <v>18</v>
       </c>
-      <c r="D23" s="173" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="173"/>
-      <c r="F23" s="172" t="s">
+      <c r="D23" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="171"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="164"/>
-      <c r="E25" s="164"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="D27" s="164"/>
-      <c r="E27" s="164"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
@@ -2318,20 +2325,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2341,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2359,31 +2352,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="77" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
+      <c r="C2" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="80" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="81"/>
+      <c r="C3" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83"/>
+      <c r="C4" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="93"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
@@ -2392,10 +2385,10 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="85"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2404,523 +2397,491 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="98" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="22">
         <v>1</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="72"/>
+      <c r="E6" s="102"/>
       <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="69"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="23">
         <v>2</v>
       </c>
-      <c r="D7" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="74"/>
+      <c r="D7" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="104"/>
       <c r="F7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="70"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="87"/>
+      <c r="D8" s="107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="108"/>
       <c r="F8" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="68" t="s">
-        <v>47</v>
+      <c r="B9" s="98" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="24">
         <v>1</v>
       </c>
-      <c r="D9" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="72"/>
+      <c r="D9" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="102"/>
       <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="69"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="23">
         <v>2</v>
       </c>
-      <c r="D10" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="74"/>
+      <c r="D10" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="104"/>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="70"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="22">
         <v>3</v>
       </c>
-      <c r="D11" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="76"/>
+      <c r="D11" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="106"/>
       <c r="F11" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="68" t="s">
-        <v>50</v>
+      <c r="B12" s="98" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="24">
         <v>1</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="72"/>
+      <c r="E12" s="102"/>
       <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="15"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="69"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="74"/>
+      <c r="D13" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="104"/>
       <c r="F13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="2:7" ht="29.25">
-      <c r="B14" s="70"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="21">
         <v>3</v>
       </c>
-      <c r="D14" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="76"/>
+      <c r="D14" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="106"/>
       <c r="F14" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="68" t="s">
-        <v>52</v>
+      <c r="B15" s="98" t="s">
+        <v>53</v>
       </c>
       <c r="C15" s="24">
         <v>1</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="72"/>
+      <c r="E15" s="102"/>
       <c r="F15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="69"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="23">
         <v>2</v>
       </c>
-      <c r="D16" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="74"/>
+      <c r="D16" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="104"/>
       <c r="F16" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="70"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="21">
         <v>3</v>
       </c>
-      <c r="D17" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="87"/>
+      <c r="D17" s="107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="108"/>
       <c r="F17" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="68" t="s">
-        <v>56</v>
+      <c r="B18" s="98" t="s">
+        <v>57</v>
       </c>
       <c r="C18" s="24">
         <v>1</v>
       </c>
-      <c r="D18" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="72"/>
+      <c r="D18" s="101" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="102"/>
       <c r="F18" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G18" s="15"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="69"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="23">
         <v>2</v>
       </c>
-      <c r="D19" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="74"/>
+      <c r="D19" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="104"/>
       <c r="F19" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="70"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="21">
         <v>3</v>
       </c>
-      <c r="D20" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="87"/>
+      <c r="D20" s="107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="108"/>
       <c r="F20" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="68" t="s">
-        <v>59</v>
+      <c r="B21" s="98" t="s">
+        <v>60</v>
       </c>
       <c r="C21" s="24">
         <v>1</v>
       </c>
-      <c r="D21" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="72"/>
+      <c r="D21" s="101" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="102"/>
       <c r="F21" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="69"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="23">
         <v>2</v>
       </c>
-      <c r="D22" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="74"/>
+      <c r="D22" s="103" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="104"/>
       <c r="F22" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="70"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="22">
         <v>3</v>
       </c>
-      <c r="D23" s="88" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="89"/>
+      <c r="D23" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="110"/>
       <c r="F23" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="68" t="s">
-        <v>60</v>
+      <c r="B24" s="98" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="24">
         <v>1</v>
       </c>
-      <c r="D24" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="72"/>
+      <c r="D24" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="102"/>
       <c r="F24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="15"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="69"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="23">
         <v>2</v>
       </c>
-      <c r="D25" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="74"/>
+      <c r="D25" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="104"/>
       <c r="F25" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="29.25">
-      <c r="B26" s="70"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="21">
         <v>3</v>
       </c>
-      <c r="D26" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="76"/>
+      <c r="D26" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="106"/>
       <c r="F26" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="68" t="s">
-        <v>62</v>
+      <c r="B27" s="98" t="s">
+        <v>63</v>
       </c>
       <c r="C27" s="24">
         <v>1</v>
       </c>
-      <c r="D27" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="72"/>
+      <c r="D27" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="102"/>
       <c r="F27" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="15"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="69"/>
+      <c r="B28" s="99"/>
       <c r="C28" s="23">
         <v>2</v>
       </c>
-      <c r="D28" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="74"/>
+      <c r="D28" s="103" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="104"/>
       <c r="F28" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="2:7" ht="29.25">
-      <c r="B29" s="70"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="21">
         <v>3</v>
       </c>
-      <c r="D29" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="76"/>
+      <c r="D29" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="106"/>
       <c r="F29" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G29" s="17"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="68" t="s">
-        <v>65</v>
+      <c r="B30" s="98" t="s">
+        <v>66</v>
       </c>
       <c r="C30" s="24">
         <v>1</v>
       </c>
-      <c r="D30" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="72"/>
+      <c r="D30" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="102"/>
       <c r="F30" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="69"/>
+      <c r="B31" s="99"/>
       <c r="C31" s="23">
         <v>2</v>
       </c>
-      <c r="D31" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="74"/>
+      <c r="D31" s="103" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="104"/>
       <c r="F31" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="12"/>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="70"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="21">
         <v>3</v>
       </c>
-      <c r="D32" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="76"/>
+      <c r="D32" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="106"/>
       <c r="F32" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G32" s="17"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="68" t="s">
-        <v>68</v>
+      <c r="B33" s="98" t="s">
+        <v>69</v>
       </c>
       <c r="C33" s="24">
         <v>1</v>
       </c>
-      <c r="D33" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="72"/>
+      <c r="D33" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="102"/>
       <c r="F33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="15"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="69"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="23">
         <v>2</v>
       </c>
-      <c r="D34" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="74"/>
+      <c r="D34" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="104"/>
       <c r="F34" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="70"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="21">
         <v>3</v>
       </c>
-      <c r="D35" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="76"/>
+      <c r="D35" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="106"/>
       <c r="F35" s="67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="68" t="s">
-        <v>70</v>
+      <c r="B36" s="98" t="s">
+        <v>71</v>
       </c>
       <c r="C36" s="24">
         <v>1</v>
       </c>
-      <c r="D36" s="71" t="s">
+      <c r="D36" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="72"/>
+      <c r="E36" s="102"/>
       <c r="F36" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="15"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="69"/>
+      <c r="B37" s="99"/>
       <c r="C37" s="23">
         <v>2</v>
       </c>
-      <c r="D37" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="74"/>
+      <c r="D37" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="104"/>
       <c r="F37" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="70"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="21">
         <v>3</v>
       </c>
-      <c r="D38" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="76"/>
+      <c r="D38" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="106"/>
       <c r="F38" s="67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G38" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -2937,6 +2898,38 @@
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2946,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
   <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2964,31 +2957,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
+      <c r="C2" s="132" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="133"/>
+      <c r="E2" s="134"/>
     </row>
     <row r="3" spans="2:7" ht="28.5" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
+      <c r="C3" s="123" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="124"/>
+      <c r="E3" s="125"/>
     </row>
     <row r="4" spans="2:7" ht="29.25" customHeight="1">
       <c r="B4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="99" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="C4" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="124"/>
+      <c r="E4" s="125"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="4" t="s">
@@ -2997,10 +2990,10 @@
       <c r="C5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="113"/>
+      <c r="D5" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="95"/>
       <c r="F5" s="29" t="s">
         <v>9</v>
       </c>
@@ -3009,228 +3002,224 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="29.25">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="45">
         <v>1</v>
       </c>
-      <c r="D6" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="107"/>
+      <c r="D6" s="120" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="121"/>
       <c r="F6" s="48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="91"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="28">
         <v>2</v>
       </c>
-      <c r="D7" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="114"/>
+      <c r="D7" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="82"/>
       <c r="F7" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7" ht="43.5">
-      <c r="B8" s="91"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
-      <c r="D8" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="111"/>
+      <c r="D8" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="86"/>
       <c r="F8" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="91"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D9" s="115" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="114"/>
+      <c r="D9" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="82"/>
       <c r="F9" s="28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="2:7" ht="43.5">
-      <c r="B10" s="91"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="28">
         <v>5</v>
       </c>
-      <c r="D10" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="111"/>
+      <c r="D10" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="86"/>
       <c r="F10" s="44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="91"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="20">
         <v>6</v>
       </c>
-      <c r="D11" s="116" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="117"/>
-      <c r="F11" s="156" t="s">
+      <c r="D11" s="113" t="s">
         <v>28</v>
       </c>
+      <c r="E11" s="114"/>
+      <c r="F11" s="68" t="s">
+        <v>29</v>
+      </c>
       <c r="G11" s="38"/>
     </row>
     <row r="12" spans="2:7" ht="29.25">
-      <c r="B12" s="90" t="s">
-        <v>47</v>
+      <c r="B12" s="117" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="57">
         <v>1</v>
       </c>
-      <c r="D12" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="160" t="s">
+      <c r="D12" s="120" t="s">
         <v>18</v>
       </c>
+      <c r="E12" s="121"/>
+      <c r="F12" s="69" t="s">
+        <v>19</v>
+      </c>
       <c r="G12" s="15"/>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1">
-      <c r="B13" s="91"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="40">
         <v>2</v>
       </c>
-      <c r="D13" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="114"/>
+      <c r="D13" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="82"/>
       <c r="F13" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="2:7" ht="43.5">
-      <c r="B14" s="91"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="40">
         <v>3</v>
       </c>
-      <c r="D14" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="111"/>
-      <c r="F14" s="161" t="s">
-        <v>76</v>
+      <c r="D14" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="86"/>
+      <c r="F14" s="70" t="s">
+        <v>77</v>
       </c>
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="91"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="40">
         <v>4</v>
       </c>
-      <c r="D15" s="115" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="114"/>
+      <c r="D15" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="82"/>
       <c r="F15" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="91"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="40">
         <v>5</v>
       </c>
-      <c r="D16" s="108" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="155"/>
+      <c r="D16" s="115" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="116"/>
       <c r="F16" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="2:7" ht="43.5">
-      <c r="B17" s="91"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="40">
         <v>6</v>
       </c>
-      <c r="D17" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="111"/>
-      <c r="F17" s="161" t="s">
+      <c r="D17" s="85" t="s">
         <v>26</v>
       </c>
+      <c r="E17" s="86"/>
+      <c r="F17" s="70" t="s">
+        <v>27</v>
+      </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="2:7" ht="29.25">
-      <c r="B18" s="92"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="50">
         <v>7</v>
       </c>
-      <c r="D18" s="116" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="162" t="s">
+      <c r="D18" s="113" t="s">
         <v>28</v>
       </c>
+      <c r="E18" s="114"/>
+      <c r="F18" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="17"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="163"/>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="154"/>
+      <c r="B19" s="72"/>
+      <c r="F19" s="31"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95"/>
+      <c r="C23" s="132" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="133"/>
+      <c r="E23" s="134"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="101"/>
+      <c r="C24" s="123" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="124"/>
+      <c r="E24" s="125"/>
     </row>
     <row r="25" spans="2:7" ht="15" customHeight="1">
       <c r="B25" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="99" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="101"/>
+      <c r="C25" s="123" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="124"/>
+      <c r="E25" s="125"/>
     </row>
     <row r="26" spans="2:7" ht="29.25" customHeight="1">
       <c r="B26" s="2" t="s">
@@ -3239,10 +3228,10 @@
       <c r="C26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="85"/>
+      <c r="D26" s="111" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="112"/>
       <c r="F26" s="29" t="s">
         <v>9</v>
       </c>
@@ -3251,88 +3240,88 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="29.25">
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="33">
         <v>1</v>
       </c>
-      <c r="D27" s="102" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="103"/>
+      <c r="D27" s="126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="127"/>
       <c r="F27" s="39" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G27" s="36"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="91"/>
+      <c r="B28" s="118"/>
       <c r="C28" s="23">
         <v>2</v>
       </c>
-      <c r="D28" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="105"/>
+      <c r="D28" s="129" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="130"/>
       <c r="F28" s="40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G28" s="37"/>
     </row>
     <row r="29" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B29" s="91"/>
+      <c r="B29" s="118"/>
       <c r="C29" s="23">
         <v>3</v>
       </c>
-      <c r="D29" s="104" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="105"/>
+      <c r="D29" s="129" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="130"/>
       <c r="F29" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="91"/>
+      <c r="B30" s="118"/>
       <c r="C30" s="23">
         <v>4</v>
       </c>
-      <c r="D30" s="108" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="109"/>
+      <c r="D30" s="115" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="128"/>
       <c r="F30" s="40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G30" s="37"/>
     </row>
     <row r="31" spans="2:7" ht="43.5">
-      <c r="B31" s="91"/>
+      <c r="B31" s="118"/>
       <c r="C31" s="34">
         <v>5</v>
       </c>
-      <c r="D31" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="111"/>
+      <c r="D31" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="86"/>
       <c r="F31" s="44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="92"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="35">
         <v>6</v>
       </c>
-      <c r="D32" s="118" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="119"/>
+      <c r="D32" s="138" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="139"/>
       <c r="F32" s="41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G32" s="38"/>
     </row>
@@ -3341,31 +3330,31 @@
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="93" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="94"/>
-      <c r="E36" s="95"/>
+      <c r="C36" s="132" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="133"/>
+      <c r="E36" s="134"/>
     </row>
     <row r="37" spans="2:7" ht="28.5" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="99" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="100"/>
-      <c r="E37" s="101"/>
+      <c r="C37" s="123" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
     </row>
     <row r="38" spans="2:7" ht="48" customHeight="1">
       <c r="B38" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="96" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="97"/>
-      <c r="E38" s="98"/>
+      <c r="C38" s="135" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="136"/>
+      <c r="E38" s="137"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="6" t="s">
@@ -3374,10 +3363,10 @@
       <c r="C39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="85"/>
+      <c r="D39" s="111" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="112"/>
       <c r="F39" s="7" t="s">
         <v>9</v>
       </c>
@@ -3386,167 +3375,155 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="29.25">
-      <c r="B40" s="90" t="s">
+      <c r="B40" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="30">
         <v>1</v>
       </c>
-      <c r="D40" s="102" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="103"/>
+      <c r="D40" s="126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="127"/>
       <c r="F40" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="91"/>
+      <c r="B41" s="118"/>
       <c r="C41" s="28">
         <v>2</v>
       </c>
-      <c r="D41" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="105"/>
+      <c r="D41" s="129" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="130"/>
       <c r="F41" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="2:7" ht="15" customHeight="1">
-      <c r="B42" s="91"/>
+      <c r="B42" s="118"/>
       <c r="C42" s="28">
         <v>3</v>
       </c>
-      <c r="D42" s="108" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="109"/>
+      <c r="D42" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="128"/>
       <c r="F42" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="92"/>
+      <c r="B43" s="119"/>
       <c r="C43" s="64">
         <v>4</v>
       </c>
-      <c r="D43" s="75" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="121"/>
+      <c r="D43" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="131"/>
       <c r="F43" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G43" s="14"/>
     </row>
     <row r="44" spans="2:7" ht="29.25">
-      <c r="B44" s="90" t="s">
-        <v>47</v>
+      <c r="B44" s="117" t="s">
+        <v>48</v>
       </c>
       <c r="C44" s="57">
         <v>1</v>
       </c>
-      <c r="D44" s="102" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="103"/>
+      <c r="D44" s="126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="127"/>
       <c r="F44" s="48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G44" s="36"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="91"/>
+      <c r="B45" s="118"/>
       <c r="C45" s="40">
         <v>2</v>
       </c>
-      <c r="D45" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="105"/>
+      <c r="D45" s="129" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="130"/>
       <c r="F45" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G45" s="37"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="91"/>
+      <c r="B46" s="118"/>
       <c r="C46" s="40">
         <v>3</v>
       </c>
-      <c r="D46" s="108" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="109"/>
+      <c r="D46" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="128"/>
       <c r="F46" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G46" s="37"/>
     </row>
     <row r="47" spans="2:7" ht="43.5">
-      <c r="B47" s="91"/>
+      <c r="B47" s="118"/>
       <c r="C47" s="40">
         <v>4</v>
       </c>
-      <c r="D47" s="108" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="109"/>
+      <c r="D47" s="115" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="128"/>
       <c r="F47" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G47" s="37"/>
     </row>
     <row r="48" spans="2:7" ht="35.25" customHeight="1">
-      <c r="B48" s="92"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="50">
         <v>5</v>
       </c>
-      <c r="D48" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="121"/>
+      <c r="D48" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="131"/>
       <c r="F48" s="54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G48" s="38"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="120"/>
-      <c r="E49" s="120"/>
+      <c r="D49" s="122"/>
+      <c r="E49" s="122"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="120"/>
-      <c r="E50" s="120"/>
+      <c r="D50" s="122"/>
+      <c r="E50" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -3562,16 +3539,28 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3581,8 +3570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3599,31 +3588,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="144" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="145"/>
-      <c r="E2" s="146"/>
+      <c r="C2" s="145" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="146"/>
+      <c r="E2" s="147"/>
     </row>
     <row r="3" spans="2:7" ht="30" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="83"/>
+      <c r="C3" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83"/>
+      <c r="C4" s="92" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="93"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="49" t="s">
@@ -3632,10 +3621,10 @@
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="147" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="113"/>
+      <c r="D5" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="95"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3644,705 +3633,779 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="57">
         <v>1</v>
       </c>
-      <c r="D6" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="135"/>
+      <c r="D6" s="149" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="141"/>
       <c r="F6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="91"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="40">
         <v>2</v>
       </c>
-      <c r="D7" s="123" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="132"/>
+      <c r="D7" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="80"/>
       <c r="F7" s="47" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="91"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="40">
         <v>3</v>
       </c>
-      <c r="D8" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="132"/>
+      <c r="D8" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="80"/>
       <c r="F8" s="47" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="91"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="40">
         <v>4</v>
       </c>
-      <c r="D9" s="115" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="114"/>
+      <c r="D9" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="82"/>
       <c r="F9" s="44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="2:7" ht="45.75" customHeight="1">
-      <c r="B10" s="91"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="40">
         <v>5</v>
       </c>
-      <c r="D10" s="110" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="111"/>
+      <c r="D10" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="86"/>
       <c r="F10" s="44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="91"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="40">
         <v>6</v>
       </c>
-      <c r="D11" s="110" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="111"/>
+      <c r="D11" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="86"/>
       <c r="F11" s="44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="91"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="40">
         <v>7</v>
       </c>
-      <c r="D12" s="123" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="132"/>
+      <c r="D12" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="80"/>
       <c r="F12" s="56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="91"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="40">
         <v>8</v>
       </c>
-      <c r="D13" s="115" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="114"/>
+      <c r="D13" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="82"/>
       <c r="F13" s="56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="92"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="60">
         <v>9</v>
       </c>
-      <c r="D14" s="149" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="150"/>
+      <c r="D14" s="142" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="143"/>
       <c r="F14" s="59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" s="58"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="90" t="s">
-        <v>47</v>
+      <c r="B15" s="117" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="33">
         <v>1</v>
       </c>
-      <c r="D15" s="148" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="135"/>
+      <c r="D15" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="141"/>
       <c r="F15" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="91"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="23">
         <v>2</v>
       </c>
-      <c r="D16" s="131" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="132"/>
+      <c r="D16" s="150" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="80"/>
       <c r="F16" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="91"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="23">
         <v>3</v>
       </c>
-      <c r="D17" s="133" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="134"/>
+      <c r="D17" s="151" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="152"/>
       <c r="F17" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="92"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="35">
         <v>4</v>
       </c>
-      <c r="D18" s="128" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="117"/>
+      <c r="D18" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="114"/>
       <c r="F18" s="55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G18" s="17"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="90" t="s">
-        <v>50</v>
+      <c r="B19" s="117" t="s">
+        <v>51</v>
       </c>
       <c r="C19" s="33">
         <v>1</v>
       </c>
-      <c r="D19" s="129" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="135"/>
+      <c r="D19" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="141"/>
       <c r="F19" s="65" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="15"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="91"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="23">
         <v>2</v>
       </c>
-      <c r="D20" s="131" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="132"/>
+      <c r="D20" s="150" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="80"/>
       <c r="F20" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="91"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="23">
         <v>3</v>
       </c>
-      <c r="D21" s="133" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="134"/>
+      <c r="D21" s="151" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="152"/>
       <c r="F21" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="92"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="35">
         <v>4</v>
       </c>
-      <c r="D22" s="128" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="117"/>
+      <c r="D22" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="114"/>
       <c r="F22" s="55" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="90" t="s">
-        <v>52</v>
+      <c r="B23" s="117" t="s">
+        <v>53</v>
       </c>
       <c r="C23" s="33">
         <v>1</v>
       </c>
-      <c r="D23" s="129" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="135"/>
+      <c r="D23" s="149" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="141"/>
       <c r="F23" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="91"/>
+      <c r="B24" s="118"/>
       <c r="C24" s="23">
         <v>2</v>
       </c>
-      <c r="D24" s="131" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="132"/>
+      <c r="D24" s="150" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="80"/>
       <c r="F24" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="91"/>
+      <c r="B25" s="118"/>
       <c r="C25" s="23">
         <v>3</v>
       </c>
-      <c r="D25" s="133" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="134"/>
+      <c r="D25" s="151" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="152"/>
       <c r="F25" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="91"/>
+      <c r="B26" s="118"/>
       <c r="C26" s="35">
         <v>4</v>
       </c>
-      <c r="D26" s="128" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="117"/>
+      <c r="D26" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="114"/>
       <c r="F26" s="55" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="90" t="s">
-        <v>56</v>
+      <c r="B27" s="117" t="s">
+        <v>57</v>
       </c>
       <c r="C27" s="52">
         <v>1</v>
       </c>
-      <c r="D27" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="151"/>
+      <c r="D27" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="144"/>
       <c r="F27" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G27" s="15"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="91"/>
+      <c r="B28" s="118"/>
       <c r="C28" s="51">
         <v>2</v>
       </c>
-      <c r="D28" s="131" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="132"/>
+      <c r="D28" s="150" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="80"/>
       <c r="F28" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="91"/>
+      <c r="B29" s="118"/>
       <c r="C29" s="51">
         <v>3</v>
       </c>
-      <c r="D29" s="133" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="134"/>
+      <c r="D29" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="152"/>
       <c r="F29" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="12"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="92"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="53">
         <v>4</v>
       </c>
-      <c r="D30" s="128" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" s="117"/>
+      <c r="D30" s="153" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="114"/>
       <c r="F30" s="55" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G30" s="17"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="91" t="s">
-        <v>59</v>
+      <c r="B31" s="118" t="s">
+        <v>60</v>
       </c>
       <c r="C31" s="33">
         <v>1</v>
       </c>
-      <c r="D31" s="129" t="s">
-        <v>107</v>
-      </c>
-      <c r="E31" s="135"/>
+      <c r="D31" s="149" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="141"/>
       <c r="F31" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="15"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="91"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="23">
         <v>2</v>
       </c>
-      <c r="D32" s="129" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="135"/>
+      <c r="D32" s="149" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="141"/>
       <c r="F32" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="12"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="91"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="23">
         <v>3</v>
       </c>
-      <c r="D33" s="136" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="137"/>
+      <c r="D33" s="155" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="156"/>
       <c r="F33" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="2:7" ht="29.25">
-      <c r="B34" s="92"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="35">
         <v>4</v>
       </c>
-      <c r="D34" s="138" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="139"/>
+      <c r="D34" s="157" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="158"/>
       <c r="F34" s="55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G34" s="17"/>
     </row>
     <row r="35" spans="2:7" ht="31.5" customHeight="1">
-      <c r="B35" s="90" t="s">
-        <v>60</v>
+      <c r="B35" s="117" t="s">
+        <v>61</v>
       </c>
       <c r="C35" s="45">
         <v>1</v>
       </c>
-      <c r="D35" s="140" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="141"/>
+      <c r="D35" s="159" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="160"/>
       <c r="F35" s="52" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B36" s="91"/>
+      <c r="B36" s="118"/>
       <c r="C36" s="28">
         <v>2</v>
       </c>
-      <c r="D36" s="125" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" s="126"/>
+      <c r="D36" s="161" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="162"/>
       <c r="F36" s="51" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="12"/>
     </row>
     <row r="37" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B37" s="91"/>
+      <c r="B37" s="118"/>
       <c r="C37" s="28">
         <v>3</v>
       </c>
-      <c r="D37" s="125" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="126"/>
+      <c r="D37" s="161" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="162"/>
       <c r="F37" s="51" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="2:7" ht="29.25">
-      <c r="B38" s="92"/>
+      <c r="B38" s="119"/>
       <c r="C38" s="20">
         <v>4</v>
       </c>
-      <c r="D38" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="143"/>
+      <c r="D38" s="163" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="164"/>
       <c r="F38" s="63" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G38" s="17"/>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
-      <c r="B39" s="91" t="s">
-        <v>62</v>
+      <c r="B39" s="118" t="s">
+        <v>63</v>
       </c>
       <c r="C39" s="45">
         <v>1</v>
       </c>
-      <c r="D39" s="129" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="130"/>
+      <c r="D39" s="149" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="154"/>
       <c r="F39" s="61" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="15"/>
     </row>
     <row r="40" spans="2:7" ht="15" customHeight="1">
-      <c r="B40" s="91"/>
+      <c r="B40" s="118"/>
       <c r="C40" s="28">
         <v>2</v>
       </c>
-      <c r="D40" s="123" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="124"/>
+      <c r="D40" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="165"/>
       <c r="F40" s="62" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1">
-      <c r="B41" s="91"/>
+      <c r="B41" s="118"/>
       <c r="C41" s="28">
         <v>3</v>
       </c>
-      <c r="D41" s="125" t="s">
-        <v>117</v>
-      </c>
-      <c r="E41" s="126"/>
+      <c r="D41" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="162"/>
       <c r="F41" s="51" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="92"/>
+      <c r="B42" s="119"/>
       <c r="C42" s="20">
         <v>4</v>
       </c>
-      <c r="D42" s="116" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="127"/>
+      <c r="D42" s="113" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="166"/>
       <c r="F42" s="63" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="D43" s="122"/>
-      <c r="E43" s="122"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="D44" s="122"/>
-      <c r="E44" s="122"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="D45" s="122"/>
-      <c r="E45" s="122"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="D46" s="122"/>
-      <c r="E46" s="122"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="D47" s="122"/>
-      <c r="E47" s="122"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="D48" s="122"/>
-      <c r="E48" s="122"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="75"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="122"/>
-      <c r="E49" s="122"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="122"/>
-      <c r="E50" s="122"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="75"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="122"/>
-      <c r="E52" s="122"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="122"/>
-      <c r="E53" s="122"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
     </row>
     <row r="54" spans="4:5">
-      <c r="D54" s="122"/>
-      <c r="E54" s="122"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="122"/>
-      <c r="E55" s="122"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
     </row>
     <row r="56" spans="4:5">
-      <c r="D56" s="122"/>
-      <c r="E56" s="122"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
     </row>
     <row r="57" spans="4:5">
-      <c r="D57" s="122"/>
-      <c r="E57" s="122"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
     </row>
     <row r="58" spans="4:5">
-      <c r="D58" s="122"/>
-      <c r="E58" s="122"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
     </row>
     <row r="59" spans="4:5">
-      <c r="D59" s="122"/>
-      <c r="E59" s="122"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="75"/>
     </row>
     <row r="60" spans="4:5">
-      <c r="D60" s="122"/>
-      <c r="E60" s="122"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
     </row>
     <row r="61" spans="4:5">
-      <c r="D61" s="122"/>
-      <c r="E61" s="122"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
     </row>
     <row r="62" spans="4:5">
-      <c r="D62" s="122"/>
-      <c r="E62" s="122"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
     </row>
     <row r="63" spans="4:5">
-      <c r="D63" s="122"/>
-      <c r="E63" s="122"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
     </row>
     <row r="64" spans="4:5">
-      <c r="D64" s="122"/>
-      <c r="E64" s="122"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="122"/>
-      <c r="E65" s="122"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="122"/>
-      <c r="E66" s="122"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="75"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="122"/>
-      <c r="E67" s="122"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="122"/>
-      <c r="E68" s="122"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="122"/>
-      <c r="E69" s="122"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="75"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="122"/>
-      <c r="E70" s="122"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="122"/>
-      <c r="E71" s="122"/>
+      <c r="D71" s="75"/>
+      <c r="E71" s="75"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="122"/>
-      <c r="E72" s="122"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="75"/>
     </row>
     <row r="73" spans="4:5">
-      <c r="D73" s="122"/>
-      <c r="E73" s="122"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="75"/>
     </row>
     <row r="74" spans="4:5">
-      <c r="D74" s="122"/>
-      <c r="E74" s="122"/>
+      <c r="D74" s="75"/>
+      <c r="E74" s="75"/>
     </row>
     <row r="75" spans="4:5">
-      <c r="D75" s="122"/>
-      <c r="E75" s="122"/>
+      <c r="D75" s="75"/>
+      <c r="E75" s="75"/>
     </row>
     <row r="76" spans="4:5">
-      <c r="D76" s="122"/>
-      <c r="E76" s="122"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="75"/>
     </row>
     <row r="77" spans="4:5">
-      <c r="D77" s="122"/>
-      <c r="E77" s="122"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
     </row>
     <row r="78" spans="4:5">
-      <c r="D78" s="122"/>
-      <c r="E78" s="122"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="75"/>
     </row>
     <row r="79" spans="4:5">
-      <c r="D79" s="122"/>
-      <c r="E79" s="122"/>
+      <c r="D79" s="75"/>
+      <c r="E79" s="75"/>
     </row>
     <row r="80" spans="4:5">
-      <c r="D80" s="122"/>
-      <c r="E80" s="122"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="75"/>
     </row>
     <row r="81" spans="4:5">
-      <c r="D81" s="122"/>
-      <c r="E81" s="122"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="75"/>
     </row>
     <row r="82" spans="4:5">
-      <c r="D82" s="122"/>
-      <c r="E82" s="122"/>
+      <c r="D82" s="75"/>
+      <c r="E82" s="75"/>
     </row>
     <row r="83" spans="4:5">
-      <c r="D83" s="122"/>
-      <c r="E83" s="122"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="D9:E9"/>
@@ -4359,80 +4422,6 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testou com ajuster quantidade do produto sem sucesso
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{001B39F3-9D75-4316-B1DF-A3B26B63972A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0604CC6-319D-4FA8-88EB-F5EC09812933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="119">
   <si>
     <t>Cenário</t>
   </si>
@@ -1095,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1117,9 +1117,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1129,21 +1126,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1161,9 +1149,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,9 +1262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1301,6 +1283,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1313,63 +1352,12 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,6 +1385,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1409,24 +1403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1436,14 +1412,23 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1460,48 +1445,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1511,71 +1565,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1913,402 +1916,388 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="27"/>
+    <col min="7" max="7" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="89"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="40">
         <v>1</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="73" t="s">
+      <c r="E6" s="83"/>
+      <c r="F6" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="77"/>
-      <c r="C7" s="28">
+      <c r="B7" s="90"/>
+      <c r="C7" s="23">
         <v>2</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="47" t="s">
+      <c r="E7" s="72"/>
+      <c r="F7" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="77"/>
-      <c r="C8" s="28">
+      <c r="B8" s="90"/>
+      <c r="C8" s="23">
         <v>3</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="47" t="s">
+      <c r="E8" s="72"/>
+      <c r="F8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="29.25">
-      <c r="B9" s="77"/>
-      <c r="C9" s="28">
+      <c r="B9" s="90"/>
+      <c r="C9" s="23">
         <v>4</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="44" t="s">
+      <c r="E9" s="87"/>
+      <c r="F9" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="77"/>
-      <c r="C10" s="28">
+      <c r="B10" s="90"/>
+      <c r="C10" s="23">
         <v>5</v>
       </c>
-      <c r="D10" s="85" t="s">
+      <c r="D10" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="87"/>
+      <c r="F10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="77"/>
-      <c r="C11" s="28">
+      <c r="B11" s="90"/>
+      <c r="C11" s="23">
         <v>6</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="86"/>
-      <c r="F11" s="44" t="s">
+      <c r="E11" s="85"/>
+      <c r="F11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="77"/>
-      <c r="C12" s="28">
+      <c r="B12" s="90"/>
+      <c r="C12" s="23">
         <v>7</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="28" t="s">
+      <c r="E12" s="87"/>
+      <c r="F12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="43.5">
-      <c r="B13" s="77"/>
-      <c r="C13" s="28">
+      <c r="B13" s="90"/>
+      <c r="C13" s="23">
         <v>8</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="86"/>
-      <c r="F13" s="44" t="s">
+      <c r="E13" s="85"/>
+      <c r="F13" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1">
-      <c r="B14" s="77"/>
-      <c r="C14" s="28">
+      <c r="B14" s="90"/>
+      <c r="C14" s="23">
         <v>9</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="82"/>
-      <c r="F14" s="44" t="s">
+      <c r="E14" s="87"/>
+      <c r="F14" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="77"/>
-      <c r="C15" s="28">
+      <c r="B15" s="90"/>
+      <c r="C15" s="23">
         <v>10</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="80"/>
-      <c r="F15" s="47" t="s">
+      <c r="E15" s="72"/>
+      <c r="F15" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="77"/>
-      <c r="C16" s="28">
+      <c r="B16" s="90"/>
+      <c r="C16" s="23">
         <v>11</v>
       </c>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="47" t="s">
+      <c r="E16" s="72"/>
+      <c r="F16" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="77"/>
-      <c r="C17" s="28">
+      <c r="B17" s="90"/>
+      <c r="C17" s="23">
         <v>12</v>
       </c>
-      <c r="D17" s="79" t="s">
+      <c r="D17" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="47" t="s">
+      <c r="E17" s="72"/>
+      <c r="F17" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="77"/>
-      <c r="C18" s="28">
+      <c r="B18" s="90"/>
+      <c r="C18" s="23">
         <v>13</v>
       </c>
-      <c r="D18" s="81" t="s">
+      <c r="D18" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="82"/>
-      <c r="F18" s="44" t="s">
+      <c r="E18" s="87"/>
+      <c r="F18" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="43.5">
-      <c r="B19" s="77"/>
-      <c r="C19" s="28">
-        <v>14</v>
-      </c>
-      <c r="D19" s="85" t="s">
+      <c r="B19" s="90"/>
+      <c r="C19" s="23">
+        <v>14</v>
+      </c>
+      <c r="D19" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="44" t="s">
+      <c r="E19" s="85"/>
+      <c r="F19" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="43.5">
-      <c r="B20" s="77"/>
-      <c r="C20" s="28">
+      <c r="B20" s="90"/>
+      <c r="C20" s="23">
         <v>15</v>
       </c>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="86"/>
-      <c r="F20" s="44" t="s">
+      <c r="E20" s="85"/>
+      <c r="F20" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="77"/>
-      <c r="C21" s="28">
+      <c r="B21" s="90"/>
+      <c r="C21" s="23">
         <v>16</v>
       </c>
-      <c r="D21" s="79" t="s">
+      <c r="D21" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="80"/>
-      <c r="F21" s="56" t="s">
+      <c r="E21" s="72"/>
+      <c r="F21" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="77"/>
-      <c r="C22" s="28">
+      <c r="B22" s="90"/>
+      <c r="C22" s="23">
         <v>17</v>
       </c>
-      <c r="D22" s="81" t="s">
+      <c r="D22" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="82"/>
-      <c r="F22" s="56" t="s">
+      <c r="E22" s="87"/>
+      <c r="F22" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="78"/>
-      <c r="C23" s="20">
+      <c r="B23" s="91"/>
+      <c r="C23" s="16">
         <v>18</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="74" t="s">
+      <c r="E23" s="93"/>
+      <c r="F23" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
@@ -2325,6 +2314,20 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2334,16 +2337,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="25"/>
-    <col min="5" max="5" width="61.42578125" style="25" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="21"/>
+    <col min="5" max="5" width="61.42578125" style="21" customWidth="1"/>
     <col min="6" max="6" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2352,31 +2355,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="89"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
@@ -2385,503 +2388,601 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="18">
         <v>1</v>
       </c>
-      <c r="D6" s="101" t="s">
+      <c r="D6" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="98"/>
+      <c r="F6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="99"/>
-      <c r="C7" s="23">
+      <c r="B7" s="95"/>
+      <c r="C7" s="19">
         <v>2</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="104"/>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="100"/>
+      <c r="F7" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="100"/>
-      <c r="C8" s="22">
+      <c r="B8" s="96"/>
+      <c r="C8" s="18">
         <v>3</v>
       </c>
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="108"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="106"/>
+      <c r="F8" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="98"/>
+      <c r="F9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="99"/>
-      <c r="C10" s="23">
+      <c r="B10" s="95"/>
+      <c r="C10" s="19">
         <v>2</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="104"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="100"/>
+      <c r="F10" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="100"/>
-      <c r="C11" s="22">
+      <c r="B11" s="96"/>
+      <c r="C11" s="18">
         <v>3</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="106"/>
-      <c r="F11" s="19" t="s">
+      <c r="E11" s="102"/>
+      <c r="F11" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="20">
         <v>1</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="102"/>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="98"/>
+      <c r="F12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="99"/>
-      <c r="C13" s="23">
+      <c r="B13" s="95"/>
+      <c r="C13" s="19">
         <v>2</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="104"/>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="100"/>
+      <c r="F13" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="2:7" ht="29.25">
-      <c r="B14" s="100"/>
-      <c r="C14" s="21">
+      <c r="B14" s="96"/>
+      <c r="C14" s="17">
         <v>3</v>
       </c>
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="106"/>
-      <c r="F14" s="19" t="s">
+      <c r="E14" s="102"/>
+      <c r="F14" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="20">
         <v>1</v>
       </c>
-      <c r="D15" s="101" t="s">
+      <c r="D15" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="102"/>
-      <c r="F15" s="9" t="s">
+      <c r="E15" s="98"/>
+      <c r="F15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="99"/>
-      <c r="C16" s="23">
+      <c r="B16" s="95"/>
+      <c r="C16" s="19">
         <v>2</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="104"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="100"/>
+      <c r="F16" s="164" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="100"/>
-      <c r="C17" s="21">
+      <c r="B17" s="96"/>
+      <c r="C17" s="17">
         <v>3</v>
       </c>
-      <c r="D17" s="107" t="s">
+      <c r="D17" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="16" t="s">
+      <c r="E17" s="106"/>
+      <c r="F17" s="165" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="17"/>
+      <c r="G17" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="20">
         <v>1</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="102"/>
-      <c r="F18" s="18" t="s">
+      <c r="E18" s="98"/>
+      <c r="F18" s="164" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="99"/>
-      <c r="C19" s="23">
+      <c r="B19" s="95"/>
+      <c r="C19" s="19">
         <v>2</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="104"/>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="100"/>
+      <c r="F19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="G19" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="100"/>
-      <c r="C20" s="21">
+      <c r="B20" s="96"/>
+      <c r="C20" s="17">
         <v>3</v>
       </c>
-      <c r="D20" s="107" t="s">
+      <c r="D20" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="108"/>
-      <c r="F20" s="16" t="s">
+      <c r="E20" s="106"/>
+      <c r="F20" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="20">
         <v>1</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="102"/>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="98"/>
+      <c r="F21" s="164" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="99"/>
-      <c r="C22" s="23">
+      <c r="B22" s="95"/>
+      <c r="C22" s="19">
         <v>2</v>
       </c>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="104"/>
-      <c r="F22" s="18" t="s">
+      <c r="E22" s="100"/>
+      <c r="F22" s="164" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="100"/>
-      <c r="C23" s="22">
+      <c r="B23" s="96"/>
+      <c r="C23" s="18">
         <v>3</v>
       </c>
-      <c r="D23" s="109" t="s">
+      <c r="D23" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="8" t="s">
+      <c r="E23" s="108"/>
+      <c r="F23" s="166" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="20">
         <v>1</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="102"/>
-      <c r="F24" s="9" t="s">
+      <c r="E24" s="98"/>
+      <c r="F24" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="15"/>
+      <c r="G24" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="99"/>
-      <c r="C25" s="23">
+      <c r="B25" s="95"/>
+      <c r="C25" s="19">
         <v>2</v>
       </c>
-      <c r="D25" s="103" t="s">
+      <c r="D25" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="104"/>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="100"/>
+      <c r="F25" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="2:7" ht="29.25">
-      <c r="B26" s="100"/>
-      <c r="C26" s="21">
+      <c r="B26" s="96"/>
+      <c r="C26" s="17">
         <v>3</v>
       </c>
-      <c r="D26" s="105" t="s">
+      <c r="D26" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="106"/>
-      <c r="F26" s="26" t="s">
+      <c r="E26" s="102"/>
+      <c r="F26" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="20">
         <v>1</v>
       </c>
-      <c r="D27" s="101" t="s">
+      <c r="D27" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="102"/>
-      <c r="F27" s="9" t="s">
+      <c r="E27" s="98"/>
+      <c r="F27" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="15"/>
+      <c r="G27" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="99"/>
-      <c r="C28" s="23">
+      <c r="B28" s="95"/>
+      <c r="C28" s="19">
         <v>2</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="104"/>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="100"/>
+      <c r="F28" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="29.25">
-      <c r="B29" s="100"/>
-      <c r="C29" s="21">
+      <c r="B29" s="96"/>
+      <c r="C29" s="17">
         <v>3</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D29" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="106"/>
-      <c r="F29" s="26" t="s">
+      <c r="E29" s="102"/>
+      <c r="F29" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="20">
         <v>1</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="102"/>
-      <c r="F30" s="9" t="s">
+      <c r="E30" s="98"/>
+      <c r="F30" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="15"/>
+      <c r="G30" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="99"/>
-      <c r="C31" s="23">
+      <c r="B31" s="95"/>
+      <c r="C31" s="19">
         <v>2</v>
       </c>
-      <c r="D31" s="103" t="s">
+      <c r="D31" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="104"/>
-      <c r="F31" s="11" t="s">
+      <c r="E31" s="100"/>
+      <c r="F31" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="12"/>
+      <c r="G31" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="100"/>
-      <c r="C32" s="21">
+      <c r="B32" s="96"/>
+      <c r="C32" s="17">
         <v>3</v>
       </c>
-      <c r="D32" s="105" t="s">
+      <c r="D32" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="106"/>
-      <c r="F32" s="26" t="s">
+      <c r="E32" s="102"/>
+      <c r="F32" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="17"/>
+      <c r="G32" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="20">
         <v>1</v>
       </c>
-      <c r="D33" s="101" t="s">
+      <c r="D33" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="102"/>
-      <c r="F33" s="9" t="s">
+      <c r="E33" s="98"/>
+      <c r="F33" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="15"/>
+      <c r="G33" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="99"/>
-      <c r="C34" s="23">
+      <c r="B34" s="95"/>
+      <c r="C34" s="19">
         <v>2</v>
       </c>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="104"/>
-      <c r="F34" s="11" t="s">
+      <c r="E34" s="100"/>
+      <c r="F34" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="12"/>
+      <c r="G34" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="100"/>
-      <c r="C35" s="21">
+      <c r="B35" s="96"/>
+      <c r="C35" s="17">
         <v>3</v>
       </c>
-      <c r="D35" s="105" t="s">
+      <c r="D35" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="106"/>
-      <c r="F35" s="67" t="s">
+      <c r="E35" s="102"/>
+      <c r="F35" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="17"/>
+      <c r="G35" s="53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="20">
         <v>1</v>
       </c>
-      <c r="D36" s="101" t="s">
+      <c r="D36" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="102"/>
-      <c r="F36" s="9" t="s">
+      <c r="E36" s="98"/>
+      <c r="F36" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="15"/>
+      <c r="G36" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="99"/>
-      <c r="C37" s="23">
+      <c r="B37" s="95"/>
+      <c r="C37" s="19">
         <v>2</v>
       </c>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="104"/>
-      <c r="F37" s="11" t="s">
+      <c r="E37" s="100"/>
+      <c r="F37" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="12"/>
+      <c r="G37" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="100"/>
-      <c r="C38" s="21">
+      <c r="B38" s="96"/>
+      <c r="C38" s="17">
         <v>3</v>
       </c>
-      <c r="D38" s="105" t="s">
+      <c r="D38" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="106"/>
-      <c r="F38" s="67" t="s">
+      <c r="E38" s="102"/>
+      <c r="F38" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="17"/>
+      <c r="G38" s="33" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -2898,38 +2999,6 @@
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2947,414 +3016,414 @@
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
-    <col min="5" max="5" width="45.42578125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
+    <col min="5" max="5" width="45.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="134"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="114"/>
     </row>
     <row r="3" spans="2:7" ht="28.5" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="125"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="120"/>
     </row>
     <row r="4" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="125"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="120"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="81"/>
+      <c r="F5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="29.25">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="40">
         <v>1</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="121"/>
-      <c r="F6" s="48" t="s">
+      <c r="E6" s="128"/>
+      <c r="F6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="118"/>
-      <c r="C7" s="28">
+      <c r="B7" s="110"/>
+      <c r="C7" s="23">
         <v>2</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="87"/>
+      <c r="F7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="2:7" ht="43.5">
-      <c r="B8" s="118"/>
-      <c r="C8" s="28">
+      <c r="B8" s="110"/>
+      <c r="C8" s="23">
         <v>3</v>
       </c>
-      <c r="D8" s="85" t="s">
+      <c r="D8" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="44" t="s">
+      <c r="E8" s="85"/>
+      <c r="F8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="118"/>
-      <c r="C9" s="28">
+      <c r="B9" s="110"/>
+      <c r="C9" s="23">
         <v>4</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="28" t="s">
+      <c r="E9" s="87"/>
+      <c r="F9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:7" ht="43.5">
-      <c r="B10" s="118"/>
-      <c r="C10" s="28">
+      <c r="B10" s="110"/>
+      <c r="C10" s="23">
         <v>5</v>
       </c>
-      <c r="D10" s="85" t="s">
+      <c r="D10" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="86"/>
-      <c r="F10" s="44" t="s">
+      <c r="E10" s="85"/>
+      <c r="F10" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="118"/>
-      <c r="C11" s="20">
+      <c r="B11" s="110"/>
+      <c r="C11" s="16">
         <v>6</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="68" t="s">
+      <c r="E11" s="132"/>
+      <c r="F11" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="2:7" ht="29.25">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="52">
         <v>1</v>
       </c>
-      <c r="D12" s="120" t="s">
+      <c r="D12" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="69" t="s">
+      <c r="E12" s="128"/>
+      <c r="F12" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1">
-      <c r="B13" s="118"/>
-      <c r="C13" s="40">
+      <c r="B13" s="110"/>
+      <c r="C13" s="35">
         <v>2</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="82"/>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="87"/>
+      <c r="F13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:7" ht="43.5">
-      <c r="B14" s="118"/>
-      <c r="C14" s="40">
+      <c r="B14" s="110"/>
+      <c r="C14" s="35">
         <v>3</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="70" t="s">
+      <c r="E14" s="85"/>
+      <c r="F14" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="118"/>
-      <c r="C15" s="40">
+      <c r="B15" s="110"/>
+      <c r="C15" s="35">
         <v>4</v>
       </c>
-      <c r="D15" s="81" t="s">
+      <c r="D15" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="82"/>
-      <c r="F15" s="23" t="s">
+      <c r="E15" s="87"/>
+      <c r="F15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="118"/>
-      <c r="C16" s="40">
+      <c r="B16" s="110"/>
+      <c r="C16" s="35">
         <v>5</v>
       </c>
-      <c r="D16" s="115" t="s">
+      <c r="D16" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="116"/>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="135"/>
+      <c r="F16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="2:7" ht="43.5">
-      <c r="B17" s="118"/>
-      <c r="C17" s="40">
+      <c r="B17" s="110"/>
+      <c r="C17" s="35">
         <v>6</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="86"/>
-      <c r="F17" s="70" t="s">
+      <c r="E17" s="85"/>
+      <c r="F17" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="2:7" ht="29.25">
-      <c r="B18" s="119"/>
-      <c r="C18" s="50">
+      <c r="B18" s="111"/>
+      <c r="C18" s="45">
         <v>7</v>
       </c>
-      <c r="D18" s="113" t="s">
+      <c r="D18" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="71" t="s">
+      <c r="E18" s="132"/>
+      <c r="F18" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="72"/>
-      <c r="F19" s="31"/>
+      <c r="B19" s="66"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="132" t="s">
+      <c r="C23" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="133"/>
-      <c r="E23" s="134"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="114"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="124"/>
-      <c r="E24" s="125"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="120"/>
     </row>
     <row r="25" spans="2:7" ht="15" customHeight="1">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="125"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="120"/>
     </row>
     <row r="26" spans="2:7" ht="29.25" customHeight="1">
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="111" t="s">
+      <c r="D26" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="112"/>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="104"/>
+      <c r="F26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="29.25">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="28">
         <v>1</v>
       </c>
-      <c r="D27" s="126" t="s">
+      <c r="D27" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="127"/>
-      <c r="F27" s="39" t="s">
+      <c r="E27" s="122"/>
+      <c r="F27" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="118"/>
-      <c r="C28" s="23">
+      <c r="B28" s="110"/>
+      <c r="C28" s="19">
         <v>2</v>
       </c>
-      <c r="D28" s="129" t="s">
+      <c r="D28" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="130"/>
-      <c r="F28" s="40" t="s">
+      <c r="E28" s="124"/>
+      <c r="F28" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="37"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B29" s="118"/>
-      <c r="C29" s="23">
+      <c r="B29" s="110"/>
+      <c r="C29" s="19">
         <v>3</v>
       </c>
-      <c r="D29" s="129" t="s">
+      <c r="D29" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="130"/>
-      <c r="F29" s="31" t="s">
+      <c r="E29" s="124"/>
+      <c r="F29" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="37"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="118"/>
-      <c r="C30" s="23">
+      <c r="B30" s="110"/>
+      <c r="C30" s="19">
         <v>4</v>
       </c>
-      <c r="D30" s="115" t="s">
+      <c r="D30" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="128"/>
-      <c r="F30" s="40" t="s">
+      <c r="E30" s="130"/>
+      <c r="F30" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="37"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="2:7" ht="43.5">
-      <c r="B31" s="118"/>
-      <c r="C31" s="34">
+      <c r="B31" s="110"/>
+      <c r="C31" s="29">
         <v>5</v>
       </c>
-      <c r="D31" s="85" t="s">
+      <c r="D31" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="86"/>
-      <c r="F31" s="44" t="s">
+      <c r="E31" s="85"/>
+      <c r="F31" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="119"/>
-      <c r="C32" s="35">
+      <c r="B32" s="111"/>
+      <c r="C32" s="30">
         <v>6</v>
       </c>
-      <c r="D32" s="138" t="s">
+      <c r="D32" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="139"/>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="126"/>
+      <c r="F32" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="38"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1"/>
     <row r="36" spans="2:7">
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="132" t="s">
+      <c r="C36" s="112" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="133"/>
-      <c r="E36" s="134"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="114"/>
     </row>
     <row r="37" spans="2:7" ht="28.5" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="123" t="s">
+      <c r="C37" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="124"/>
-      <c r="E37" s="125"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="120"/>
     </row>
     <row r="38" spans="2:7" ht="48" customHeight="1">
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="135" t="s">
+      <c r="C38" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="136"/>
-      <c r="E38" s="137"/>
+      <c r="D38" s="116"/>
+      <c r="E38" s="117"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="6" t="s">
@@ -3363,10 +3432,10 @@
       <c r="C39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="111" t="s">
+      <c r="D39" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="112"/>
+      <c r="E39" s="104"/>
       <c r="F39" s="7" t="s">
         <v>9</v>
       </c>
@@ -3375,155 +3444,166 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="29.25">
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C40" s="25">
         <v>1</v>
       </c>
-      <c r="D40" s="126" t="s">
+      <c r="D40" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="127"/>
-      <c r="F40" s="32" t="s">
+      <c r="E40" s="122"/>
+      <c r="F40" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="10"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="118"/>
-      <c r="C41" s="28">
+      <c r="B41" s="110"/>
+      <c r="C41" s="23">
         <v>2</v>
       </c>
-      <c r="D41" s="129" t="s">
+      <c r="D41" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="130"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="124"/>
+      <c r="F41" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="12"/>
+      <c r="G41" s="11"/>
     </row>
     <row r="42" spans="2:7" ht="15" customHeight="1">
-      <c r="B42" s="118"/>
-      <c r="C42" s="28">
+      <c r="B42" s="110"/>
+      <c r="C42" s="23">
         <v>3</v>
       </c>
-      <c r="D42" s="115" t="s">
+      <c r="D42" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="128"/>
-      <c r="F42" s="23" t="s">
+      <c r="E42" s="130"/>
+      <c r="F42" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="12"/>
+      <c r="G42" s="11"/>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="119"/>
-      <c r="C43" s="64">
+      <c r="B43" s="111"/>
+      <c r="C43" s="59">
         <v>4</v>
       </c>
-      <c r="D43" s="105" t="s">
+      <c r="D43" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="131"/>
-      <c r="F43" s="66" t="s">
+      <c r="E43" s="134"/>
+      <c r="F43" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="14"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="2:7" ht="29.25">
-      <c r="B44" s="117" t="s">
+      <c r="B44" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="57">
+      <c r="C44" s="52">
         <v>1</v>
       </c>
-      <c r="D44" s="126" t="s">
+      <c r="D44" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="127"/>
-      <c r="F44" s="48" t="s">
+      <c r="E44" s="122"/>
+      <c r="F44" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G44" s="36"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="118"/>
-      <c r="C45" s="40">
+      <c r="B45" s="110"/>
+      <c r="C45" s="35">
         <v>2</v>
       </c>
-      <c r="D45" s="129" t="s">
+      <c r="D45" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="130"/>
-      <c r="F45" s="28" t="s">
+      <c r="E45" s="124"/>
+      <c r="F45" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="37"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="118"/>
-      <c r="C46" s="40">
+      <c r="B46" s="110"/>
+      <c r="C46" s="35">
         <v>3</v>
       </c>
-      <c r="D46" s="115" t="s">
+      <c r="D46" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="128"/>
-      <c r="F46" s="28" t="s">
+      <c r="E46" s="130"/>
+      <c r="F46" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="37"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="2:7" ht="43.5">
-      <c r="B47" s="118"/>
-      <c r="C47" s="40">
+      <c r="B47" s="110"/>
+      <c r="C47" s="35">
         <v>4</v>
       </c>
-      <c r="D47" s="115" t="s">
+      <c r="D47" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="128"/>
-      <c r="F47" s="66" t="s">
+      <c r="E47" s="130"/>
+      <c r="F47" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="G47" s="37"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="2:7" ht="35.25" customHeight="1">
-      <c r="B48" s="119"/>
-      <c r="C48" s="50">
+      <c r="B48" s="111"/>
+      <c r="C48" s="45">
         <v>5</v>
       </c>
-      <c r="D48" s="105" t="s">
+      <c r="D48" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="131"/>
-      <c r="F48" s="54" t="s">
+      <c r="E48" s="134"/>
+      <c r="F48" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="38"/>
+      <c r="G48" s="33"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="122"/>
-      <c r="E49" s="122"/>
+      <c r="D49" s="133"/>
+      <c r="E49" s="133"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="122"/>
-      <c r="E50" s="122"/>
+      <c r="D50" s="133"/>
+      <c r="E50" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -3539,28 +3619,17 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3578,8 +3647,8 @@
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
     <col min="5" max="5" width="52.85546875" customWidth="1"/>
     <col min="6" max="6" width="57.85546875" customWidth="1"/>
   </cols>
@@ -3588,757 +3657,817 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="155" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="146"/>
-      <c r="E2" s="147"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="157"/>
     </row>
     <row r="3" spans="2:7" ht="30" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="158" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="52">
         <v>1</v>
       </c>
-      <c r="D6" s="149" t="s">
+      <c r="D6" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="141"/>
-      <c r="F6" s="46" t="s">
+      <c r="E6" s="146"/>
+      <c r="F6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="118"/>
-      <c r="C7" s="40">
+      <c r="B7" s="110"/>
+      <c r="C7" s="35">
         <v>2</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="47" t="s">
+      <c r="E7" s="72"/>
+      <c r="F7" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="118"/>
-      <c r="C8" s="40">
+      <c r="B8" s="110"/>
+      <c r="C8" s="35">
         <v>3</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="47" t="s">
+      <c r="E8" s="72"/>
+      <c r="F8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="118"/>
-      <c r="C9" s="40">
+      <c r="B9" s="110"/>
+      <c r="C9" s="35">
         <v>4</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="44" t="s">
+      <c r="E9" s="87"/>
+      <c r="F9" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:7" ht="45.75" customHeight="1">
-      <c r="B10" s="118"/>
-      <c r="C10" s="40">
+      <c r="B10" s="110"/>
+      <c r="C10" s="35">
         <v>5</v>
       </c>
-      <c r="D10" s="85" t="s">
+      <c r="D10" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="86"/>
-      <c r="F10" s="44" t="s">
+      <c r="E10" s="85"/>
+      <c r="F10" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="118"/>
-      <c r="C11" s="40">
+      <c r="B11" s="110"/>
+      <c r="C11" s="35">
         <v>6</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="86"/>
-      <c r="F11" s="44" t="s">
+      <c r="E11" s="85"/>
+      <c r="F11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="118"/>
-      <c r="C12" s="40">
+      <c r="B12" s="110"/>
+      <c r="C12" s="35">
         <v>7</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="56" t="s">
+      <c r="E12" s="72"/>
+      <c r="F12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="118"/>
-      <c r="C13" s="40">
+      <c r="B13" s="110"/>
+      <c r="C13" s="35">
         <v>8</v>
       </c>
-      <c r="D13" s="81" t="s">
+      <c r="D13" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="82"/>
-      <c r="F13" s="56" t="s">
+      <c r="E13" s="87"/>
+      <c r="F13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="119"/>
-      <c r="C14" s="60">
+      <c r="B14" s="111"/>
+      <c r="C14" s="55">
         <v>9</v>
       </c>
-      <c r="D14" s="142" t="s">
+      <c r="D14" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="143"/>
-      <c r="F14" s="59" t="s">
+      <c r="E14" s="161"/>
+      <c r="F14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="58"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="28">
         <v>1</v>
       </c>
-      <c r="D15" s="140" t="s">
+      <c r="D15" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="141"/>
-      <c r="F15" s="9" t="s">
+      <c r="E15" s="146"/>
+      <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="118"/>
-      <c r="C16" s="23">
+      <c r="B16" s="110"/>
+      <c r="C16" s="19">
         <v>2</v>
       </c>
-      <c r="D16" s="150" t="s">
+      <c r="D16" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="72"/>
+      <c r="F16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="118"/>
-      <c r="C17" s="23">
+      <c r="B17" s="110"/>
+      <c r="C17" s="19">
         <v>3</v>
       </c>
-      <c r="D17" s="151" t="s">
+      <c r="D17" s="144" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="152"/>
-      <c r="F17" s="18" t="s">
+      <c r="E17" s="145"/>
+      <c r="F17" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="119"/>
-      <c r="C18" s="35">
+      <c r="B18" s="111"/>
+      <c r="C18" s="30">
         <v>4</v>
       </c>
-      <c r="D18" s="153" t="s">
+      <c r="D18" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="55" t="s">
+      <c r="E18" s="132"/>
+      <c r="F18" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="28">
         <v>1</v>
       </c>
-      <c r="D19" s="149" t="s">
+      <c r="D19" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="141"/>
-      <c r="F19" s="65" t="s">
+      <c r="E19" s="146"/>
+      <c r="F19" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="118"/>
-      <c r="C20" s="23">
+      <c r="B20" s="110"/>
+      <c r="C20" s="19">
         <v>2</v>
       </c>
-      <c r="D20" s="150" t="s">
+      <c r="D20" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="80"/>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="72"/>
+      <c r="F20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="118"/>
-      <c r="C21" s="23">
+      <c r="B21" s="110"/>
+      <c r="C21" s="19">
         <v>3</v>
       </c>
-      <c r="D21" s="151" t="s">
+      <c r="D21" s="144" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="152"/>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="145"/>
+      <c r="F21" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="119"/>
-      <c r="C22" s="35">
+      <c r="B22" s="111"/>
+      <c r="C22" s="30">
         <v>4</v>
       </c>
-      <c r="D22" s="153" t="s">
+      <c r="D22" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="114"/>
-      <c r="F22" s="55" t="s">
+      <c r="E22" s="132"/>
+      <c r="F22" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="17"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="28">
         <v>1</v>
       </c>
-      <c r="D23" s="149" t="s">
+      <c r="D23" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="141"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="146"/>
+      <c r="F23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="118"/>
-      <c r="C24" s="23">
+      <c r="B24" s="110"/>
+      <c r="C24" s="19">
         <v>2</v>
       </c>
-      <c r="D24" s="150" t="s">
+      <c r="D24" s="143" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="80"/>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="72"/>
+      <c r="F24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="118"/>
-      <c r="C25" s="23">
+      <c r="B25" s="110"/>
+      <c r="C25" s="19">
         <v>3</v>
       </c>
-      <c r="D25" s="151" t="s">
+      <c r="D25" s="144" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="152"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="145"/>
+      <c r="F25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="118"/>
-      <c r="C26" s="35">
+      <c r="B26" s="110"/>
+      <c r="C26" s="30">
         <v>4</v>
       </c>
-      <c r="D26" s="153" t="s">
+      <c r="D26" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="55" t="s">
+      <c r="E26" s="132"/>
+      <c r="F26" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="47">
         <v>1</v>
       </c>
-      <c r="D27" s="101" t="s">
+      <c r="D27" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="144"/>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="162"/>
+      <c r="F27" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="15"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="118"/>
-      <c r="C28" s="51">
+      <c r="B28" s="110"/>
+      <c r="C28" s="46">
         <v>2</v>
       </c>
-      <c r="D28" s="150" t="s">
+      <c r="D28" s="143" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="80"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="72"/>
+      <c r="F28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="118"/>
-      <c r="C29" s="51">
+      <c r="B29" s="110"/>
+      <c r="C29" s="46">
         <v>3</v>
       </c>
-      <c r="D29" s="151" t="s">
+      <c r="D29" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="152"/>
-      <c r="F29" s="23" t="s">
+      <c r="E29" s="145"/>
+      <c r="F29" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="12"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="119"/>
-      <c r="C30" s="53">
+      <c r="B30" s="111"/>
+      <c r="C30" s="48">
         <v>4</v>
       </c>
-      <c r="D30" s="153" t="s">
+      <c r="D30" s="140" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="114"/>
-      <c r="F30" s="55" t="s">
+      <c r="E30" s="132"/>
+      <c r="F30" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="118" t="s">
+      <c r="B31" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="33">
+      <c r="C31" s="28">
         <v>1</v>
       </c>
-      <c r="D31" s="149" t="s">
+      <c r="D31" s="141" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="141"/>
-      <c r="F31" s="9" t="s">
+      <c r="E31" s="146"/>
+      <c r="F31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="15"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="118"/>
-      <c r="C32" s="23">
+      <c r="B32" s="110"/>
+      <c r="C32" s="19">
         <v>2</v>
       </c>
-      <c r="D32" s="149" t="s">
+      <c r="D32" s="141" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="141"/>
-      <c r="F32" s="11" t="s">
+      <c r="E32" s="146"/>
+      <c r="F32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="12"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="118"/>
-      <c r="C33" s="23">
+      <c r="B33" s="110"/>
+      <c r="C33" s="19">
         <v>3</v>
       </c>
-      <c r="D33" s="155" t="s">
+      <c r="D33" s="147" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="156"/>
-      <c r="F33" s="23" t="s">
+      <c r="E33" s="148"/>
+      <c r="F33" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="12"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" spans="2:7" ht="29.25">
-      <c r="B34" s="119"/>
-      <c r="C34" s="35">
+      <c r="B34" s="111"/>
+      <c r="C34" s="30">
         <v>4</v>
       </c>
-      <c r="D34" s="157" t="s">
+      <c r="D34" s="149" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="158"/>
-      <c r="F34" s="55" t="s">
+      <c r="E34" s="150"/>
+      <c r="F34" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="17"/>
+      <c r="G34" s="14"/>
     </row>
     <row r="35" spans="2:7" ht="31.5" customHeight="1">
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="40">
         <v>1</v>
       </c>
-      <c r="D35" s="159" t="s">
+      <c r="D35" s="151" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="160"/>
-      <c r="F35" s="52" t="s">
+      <c r="E35" s="152"/>
+      <c r="F35" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="15"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B36" s="118"/>
-      <c r="C36" s="28">
+      <c r="B36" s="110"/>
+      <c r="C36" s="23">
         <v>2</v>
       </c>
-      <c r="D36" s="161" t="s">
+      <c r="D36" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="162"/>
-      <c r="F36" s="51" t="s">
+      <c r="E36" s="138"/>
+      <c r="F36" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="12"/>
+      <c r="G36" s="11"/>
     </row>
     <row r="37" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B37" s="118"/>
-      <c r="C37" s="28">
+      <c r="B37" s="110"/>
+      <c r="C37" s="23">
         <v>3</v>
       </c>
-      <c r="D37" s="161" t="s">
+      <c r="D37" s="137" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="162"/>
-      <c r="F37" s="51" t="s">
+      <c r="E37" s="138"/>
+      <c r="F37" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="12"/>
+      <c r="G37" s="11"/>
     </row>
     <row r="38" spans="2:7" ht="29.25">
-      <c r="B38" s="119"/>
-      <c r="C38" s="20">
+      <c r="B38" s="111"/>
+      <c r="C38" s="16">
         <v>4</v>
       </c>
-      <c r="D38" s="163" t="s">
+      <c r="D38" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="164"/>
-      <c r="F38" s="63" t="s">
+      <c r="E38" s="154"/>
+      <c r="F38" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="G38" s="17"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="40">
         <v>1</v>
       </c>
-      <c r="D39" s="149" t="s">
+      <c r="D39" s="141" t="s">
         <v>116</v>
       </c>
-      <c r="E39" s="154"/>
-      <c r="F39" s="61" t="s">
+      <c r="E39" s="142"/>
+      <c r="F39" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="2:7" ht="15" customHeight="1">
-      <c r="B40" s="118"/>
-      <c r="C40" s="28">
+      <c r="B40" s="110"/>
+      <c r="C40" s="23">
         <v>2</v>
       </c>
-      <c r="D40" s="79" t="s">
+      <c r="D40" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="165"/>
-      <c r="F40" s="62" t="s">
+      <c r="E40" s="136"/>
+      <c r="F40" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="12"/>
+      <c r="G40" s="11"/>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1">
-      <c r="B41" s="118"/>
-      <c r="C41" s="28">
+      <c r="B41" s="110"/>
+      <c r="C41" s="23">
         <v>3</v>
       </c>
-      <c r="D41" s="161" t="s">
+      <c r="D41" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="162"/>
-      <c r="F41" s="51" t="s">
+      <c r="E41" s="138"/>
+      <c r="F41" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="12"/>
+      <c r="G41" s="11"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="119"/>
-      <c r="C42" s="20">
+      <c r="B42" s="111"/>
+      <c r="C42" s="16">
         <v>4</v>
       </c>
-      <c r="D42" s="113" t="s">
+      <c r="D42" s="131" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="166"/>
-      <c r="F42" s="63" t="s">
+      <c r="E42" s="139"/>
+      <c r="F42" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="17"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
+      <c r="D43" s="88"/>
+      <c r="E43" s="88"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
+      <c r="D47" s="88"/>
+      <c r="E47" s="88"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="88"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="88"/>
     </row>
     <row r="54" spans="4:5">
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
+      <c r="D54" s="88"/>
+      <c r="E54" s="88"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="88"/>
     </row>
     <row r="56" spans="4:5">
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
     </row>
     <row r="57" spans="4:5">
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
+      <c r="D57" s="88"/>
+      <c r="E57" s="88"/>
     </row>
     <row r="58" spans="4:5">
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
+      <c r="D58" s="88"/>
+      <c r="E58" s="88"/>
     </row>
     <row r="59" spans="4:5">
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
+      <c r="D59" s="88"/>
+      <c r="E59" s="88"/>
     </row>
     <row r="60" spans="4:5">
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
+      <c r="D60" s="88"/>
+      <c r="E60" s="88"/>
     </row>
     <row r="61" spans="4:5">
-      <c r="D61" s="75"/>
-      <c r="E61" s="75"/>
+      <c r="D61" s="88"/>
+      <c r="E61" s="88"/>
     </row>
     <row r="62" spans="4:5">
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="88"/>
     </row>
     <row r="63" spans="4:5">
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
+      <c r="D63" s="88"/>
+      <c r="E63" s="88"/>
     </row>
     <row r="64" spans="4:5">
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
+      <c r="D64" s="88"/>
+      <c r="E64" s="88"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
+      <c r="D65" s="88"/>
+      <c r="E65" s="88"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
+      <c r="D66" s="88"/>
+      <c r="E66" s="88"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
+      <c r="D67" s="88"/>
+      <c r="E67" s="88"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
+      <c r="D68" s="88"/>
+      <c r="E68" s="88"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
+      <c r="D69" s="88"/>
+      <c r="E69" s="88"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
+      <c r="D70" s="88"/>
+      <c r="E70" s="88"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
+      <c r="D71" s="88"/>
+      <c r="E71" s="88"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
+      <c r="D72" s="88"/>
+      <c r="E72" s="88"/>
     </row>
     <row r="73" spans="4:5">
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
+      <c r="D73" s="88"/>
+      <c r="E73" s="88"/>
     </row>
     <row r="74" spans="4:5">
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
+      <c r="D74" s="88"/>
+      <c r="E74" s="88"/>
     </row>
     <row r="75" spans="4:5">
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
     </row>
     <row r="76" spans="4:5">
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="88"/>
     </row>
     <row r="77" spans="4:5">
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
+      <c r="D77" s="88"/>
+      <c r="E77" s="88"/>
     </row>
     <row r="78" spans="4:5">
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
+      <c r="D78" s="88"/>
+      <c r="E78" s="88"/>
     </row>
     <row r="79" spans="4:5">
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
+      <c r="D79" s="88"/>
+      <c r="E79" s="88"/>
     </row>
     <row r="80" spans="4:5">
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="88"/>
     </row>
     <row r="81" spans="4:5">
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
+      <c r="D81" s="88"/>
+      <c r="E81" s="88"/>
     </row>
     <row r="82" spans="4:5">
-      <c r="D82" s="75"/>
-      <c r="E82" s="75"/>
+      <c r="D82" s="88"/>
+      <c r="E82" s="88"/>
     </row>
     <row r="83" spans="4:5">
-      <c r="D83" s="75"/>
-      <c r="E83" s="75"/>
+      <c r="D83" s="88"/>
+      <c r="E83" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="B35:B38"/>
@@ -4355,73 +4484,13 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B6:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
coloquei os status nos cenarios dos testes no excel
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0604CC6-319D-4FA8-88EB-F5EC09812933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14169466-00FE-4780-B6C1-B8E47B7B0A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="120">
   <si>
     <t>Cenário</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>O sistema deverá aceitar o número inserido no campo.</t>
+  </si>
+  <si>
+    <t>falhou</t>
   </si>
   <si>
     <t>Atualizar a pagina e o carrinho mantém os itens</t>
@@ -397,7 +400,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +418,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
@@ -1095,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1126,7 +1136,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1289,6 +1298,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1565,21 +1593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1916,385 +1930,385 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="22"/>
+    <col min="7" max="7" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>1</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="67" t="s">
+      <c r="E6" s="91"/>
+      <c r="F6" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="90"/>
-      <c r="C7" s="23">
+      <c r="B7" s="98"/>
+      <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="80"/>
+      <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="90"/>
-      <c r="C8" s="23">
+      <c r="B8" s="98"/>
+      <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="42" t="s">
+      <c r="E8" s="80"/>
+      <c r="F8" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="29.25">
-      <c r="B9" s="90"/>
-      <c r="C9" s="23">
+      <c r="B9" s="98"/>
+      <c r="C9" s="22">
         <v>4</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="39" t="s">
+      <c r="E9" s="95"/>
+      <c r="F9" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="90"/>
-      <c r="C10" s="23">
+      <c r="B10" s="98"/>
+      <c r="C10" s="22">
         <v>5</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="87"/>
-      <c r="F10" s="23" t="s">
+      <c r="E10" s="95"/>
+      <c r="F10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="90"/>
-      <c r="C11" s="23">
+      <c r="B11" s="98"/>
+      <c r="C11" s="22">
         <v>6</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="39" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="90"/>
-      <c r="C12" s="23">
+      <c r="B12" s="98"/>
+      <c r="C12" s="22">
         <v>7</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="23" t="s">
+      <c r="E12" s="95"/>
+      <c r="F12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="43.5">
-      <c r="B13" s="90"/>
-      <c r="C13" s="23">
+      <c r="B13" s="98"/>
+      <c r="C13" s="22">
         <v>8</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="39" t="s">
+      <c r="E13" s="93"/>
+      <c r="F13" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1">
-      <c r="B14" s="90"/>
-      <c r="C14" s="23">
+      <c r="B14" s="98"/>
+      <c r="C14" s="22">
         <v>9</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="39" t="s">
+      <c r="E14" s="95"/>
+      <c r="F14" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="90"/>
-      <c r="C15" s="23">
+      <c r="B15" s="98"/>
+      <c r="C15" s="22">
         <v>10</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="42" t="s">
+      <c r="E15" s="80"/>
+      <c r="F15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="90"/>
-      <c r="C16" s="23">
+      <c r="B16" s="98"/>
+      <c r="C16" s="22">
         <v>11</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="72"/>
-      <c r="F16" s="42" t="s">
+      <c r="E16" s="80"/>
+      <c r="F16" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="90"/>
-      <c r="C17" s="23">
+      <c r="B17" s="98"/>
+      <c r="C17" s="22">
         <v>12</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="42" t="s">
+      <c r="E17" s="80"/>
+      <c r="F17" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="90"/>
-      <c r="C18" s="23">
+      <c r="B18" s="98"/>
+      <c r="C18" s="22">
         <v>13</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="95"/>
+      <c r="F18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="43.5">
-      <c r="B19" s="90"/>
-      <c r="C19" s="23">
-        <v>14</v>
-      </c>
-      <c r="D19" s="84" t="s">
+      <c r="B19" s="98"/>
+      <c r="C19" s="22">
+        <v>14</v>
+      </c>
+      <c r="D19" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="85"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="93"/>
+      <c r="F19" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="43.5">
-      <c r="B20" s="90"/>
-      <c r="C20" s="23">
+      <c r="B20" s="98"/>
+      <c r="C20" s="22">
         <v>15</v>
       </c>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="39" t="s">
+      <c r="E20" s="93"/>
+      <c r="F20" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="90"/>
-      <c r="C21" s="23">
+      <c r="B21" s="98"/>
+      <c r="C21" s="22">
         <v>16</v>
       </c>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="72"/>
-      <c r="F21" s="51" t="s">
+      <c r="E21" s="80"/>
+      <c r="F21" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="90"/>
-      <c r="C22" s="23">
+      <c r="B22" s="98"/>
+      <c r="C22" s="22">
         <v>17</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="87"/>
-      <c r="F22" s="51" t="s">
+      <c r="E22" s="95"/>
+      <c r="F22" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="91"/>
-      <c r="C23" s="16">
+      <c r="B23" s="99"/>
+      <c r="C23" s="15">
         <v>18</v>
       </c>
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="93"/>
-      <c r="F23" s="68" t="s">
+      <c r="E23" s="101"/>
+      <c r="F23" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -2337,16 +2351,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36:G38"/>
+    <sheetView topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="21"/>
-    <col min="5" max="5" width="61.42578125" style="21" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="61.42578125" style="20" customWidth="1"/>
     <col min="6" max="6" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2355,31 +2369,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
@@ -2388,564 +2402,564 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="104"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="106"/>
+      <c r="F6" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="95"/>
-      <c r="C7" s="19">
+      <c r="B7" s="103"/>
+      <c r="C7" s="18">
         <v>2</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="100"/>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="108"/>
+      <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="96"/>
-      <c r="C8" s="18">
+      <c r="B8" s="104"/>
+      <c r="C8" s="17">
         <v>3</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="106"/>
-      <c r="F8" s="70" t="s">
+      <c r="E8" s="114"/>
+      <c r="F8" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>1</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="106"/>
+      <c r="F9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="95"/>
-      <c r="C10" s="19">
+      <c r="B10" s="103"/>
+      <c r="C10" s="18">
         <v>2</v>
       </c>
-      <c r="D10" s="99" t="s">
+      <c r="D10" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="100"/>
-      <c r="F10" s="42" t="s">
+      <c r="E10" s="108"/>
+      <c r="F10" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="96"/>
-      <c r="C11" s="18">
+      <c r="B11" s="104"/>
+      <c r="C11" s="17">
         <v>3</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="102"/>
-      <c r="F11" s="163" t="s">
+      <c r="E11" s="110"/>
+      <c r="F11" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>1</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="98"/>
-      <c r="F12" s="41" t="s">
+      <c r="E12" s="106"/>
+      <c r="F12" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="95"/>
-      <c r="C13" s="19">
+      <c r="B13" s="103"/>
+      <c r="C13" s="18">
         <v>2</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="42" t="s">
+      <c r="E13" s="108"/>
+      <c r="F13" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="29.25">
-      <c r="B14" s="96"/>
-      <c r="C14" s="17">
+      <c r="B14" s="104"/>
+      <c r="C14" s="16">
         <v>3</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="102"/>
-      <c r="F14" s="163" t="s">
+      <c r="E14" s="110"/>
+      <c r="F14" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="97" t="s">
+      <c r="D15" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="98"/>
-      <c r="F15" s="41" t="s">
+      <c r="E15" s="106"/>
+      <c r="F15" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="95"/>
-      <c r="C16" s="19">
+      <c r="B16" s="103"/>
+      <c r="C16" s="18">
         <v>2</v>
       </c>
-      <c r="D16" s="99" t="s">
+      <c r="D16" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="100"/>
-      <c r="F16" s="164" t="s">
+      <c r="E16" s="108"/>
+      <c r="F16" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="96"/>
-      <c r="C17" s="17">
+      <c r="B17" s="104"/>
+      <c r="C17" s="16">
         <v>3</v>
       </c>
-      <c r="D17" s="105" t="s">
+      <c r="D17" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="106"/>
-      <c r="F17" s="165" t="s">
+      <c r="E17" s="114"/>
+      <c r="F17" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="53" t="s">
+      <c r="G17" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="97" t="s">
+      <c r="D18" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="164" t="s">
+      <c r="E18" s="106"/>
+      <c r="F18" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="95"/>
-      <c r="C19" s="19">
+      <c r="B19" s="103"/>
+      <c r="C19" s="18">
         <v>2</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="100"/>
-      <c r="F19" s="42" t="s">
+      <c r="E19" s="108"/>
+      <c r="F19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="96"/>
-      <c r="C20" s="17">
+      <c r="B20" s="104"/>
+      <c r="C20" s="16">
         <v>3</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="165" t="s">
+      <c r="E20" s="114"/>
+      <c r="F20" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="53" t="s">
+      <c r="G20" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="D21" s="97" t="s">
+      <c r="D21" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="98"/>
-      <c r="F21" s="164" t="s">
+      <c r="E21" s="106"/>
+      <c r="F21" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="95"/>
-      <c r="C22" s="19">
+      <c r="B22" s="103"/>
+      <c r="C22" s="18">
         <v>2</v>
       </c>
-      <c r="D22" s="99" t="s">
+      <c r="D22" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="100"/>
-      <c r="F22" s="164" t="s">
+      <c r="E22" s="108"/>
+      <c r="F22" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="96"/>
-      <c r="C23" s="18">
+      <c r="B23" s="104"/>
+      <c r="C23" s="17">
         <v>3</v>
       </c>
-      <c r="D23" s="107" t="s">
+      <c r="D23" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="108"/>
-      <c r="F23" s="166" t="s">
+      <c r="E23" s="116"/>
+      <c r="F23" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="53" t="s">
+      <c r="G23" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="19">
         <v>1</v>
       </c>
-      <c r="D24" s="97" t="s">
+      <c r="D24" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="98"/>
-      <c r="F24" s="41" t="s">
+      <c r="E24" s="106"/>
+      <c r="F24" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="95"/>
-      <c r="C25" s="19">
+      <c r="B25" s="103"/>
+      <c r="C25" s="18">
         <v>2</v>
       </c>
-      <c r="D25" s="99" t="s">
+      <c r="D25" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="100"/>
-      <c r="F25" s="42" t="s">
+      <c r="E25" s="108"/>
+      <c r="F25" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="29.25">
-      <c r="B26" s="96"/>
-      <c r="C26" s="17">
+      <c r="B26" s="104"/>
+      <c r="C26" s="16">
         <v>3</v>
       </c>
-      <c r="D26" s="101" t="s">
+      <c r="D26" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="102"/>
-      <c r="F26" s="167" t="s">
+      <c r="E26" s="110"/>
+      <c r="F26" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="53" t="s">
+      <c r="G26" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="19">
         <v>1</v>
       </c>
-      <c r="D27" s="97" t="s">
+      <c r="D27" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="98"/>
-      <c r="F27" s="41" t="s">
+      <c r="E27" s="106"/>
+      <c r="F27" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="95"/>
-      <c r="C28" s="19">
+      <c r="B28" s="103"/>
+      <c r="C28" s="18">
         <v>2</v>
       </c>
-      <c r="D28" s="99" t="s">
+      <c r="D28" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="100"/>
-      <c r="F28" s="42" t="s">
+      <c r="E28" s="108"/>
+      <c r="F28" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="29.25">
-      <c r="B29" s="96"/>
-      <c r="C29" s="17">
+      <c r="B29" s="104"/>
+      <c r="C29" s="16">
         <v>3</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="102"/>
-      <c r="F29" s="167" t="s">
+      <c r="E29" s="110"/>
+      <c r="F29" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="53" t="s">
+      <c r="G29" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="19">
         <v>1</v>
       </c>
-      <c r="D30" s="97" t="s">
+      <c r="D30" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="98"/>
-      <c r="F30" s="41" t="s">
+      <c r="E30" s="106"/>
+      <c r="F30" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="95"/>
-      <c r="C31" s="19">
+      <c r="B31" s="103"/>
+      <c r="C31" s="18">
         <v>2</v>
       </c>
-      <c r="D31" s="99" t="s">
+      <c r="D31" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="100"/>
-      <c r="F31" s="42" t="s">
+      <c r="E31" s="108"/>
+      <c r="F31" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="96"/>
-      <c r="C32" s="17">
+      <c r="B32" s="104"/>
+      <c r="C32" s="16">
         <v>3</v>
       </c>
-      <c r="D32" s="101" t="s">
+      <c r="D32" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="102"/>
-      <c r="F32" s="167" t="s">
+      <c r="E32" s="110"/>
+      <c r="F32" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="94" t="s">
+      <c r="B33" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="19">
         <v>1</v>
       </c>
-      <c r="D33" s="97" t="s">
+      <c r="D33" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="98"/>
-      <c r="F33" s="41" t="s">
+      <c r="E33" s="106"/>
+      <c r="F33" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="95"/>
-      <c r="C34" s="19">
+      <c r="B34" s="103"/>
+      <c r="C34" s="18">
         <v>2</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="100"/>
-      <c r="F34" s="42" t="s">
+      <c r="E34" s="108"/>
+      <c r="F34" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="32" t="s">
+      <c r="G34" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="96"/>
-      <c r="C35" s="17">
+      <c r="B35" s="104"/>
+      <c r="C35" s="16">
         <v>3</v>
       </c>
-      <c r="D35" s="101" t="s">
+      <c r="D35" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="102"/>
-      <c r="F35" s="69" t="s">
+      <c r="E35" s="110"/>
+      <c r="F35" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="53" t="s">
+      <c r="G35" s="52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="94" t="s">
+      <c r="B36" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="19">
         <v>1</v>
       </c>
-      <c r="D36" s="97" t="s">
+      <c r="D36" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="98"/>
-      <c r="F36" s="41" t="s">
+      <c r="E36" s="106"/>
+      <c r="F36" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="95"/>
-      <c r="C37" s="19">
+      <c r="B37" s="103"/>
+      <c r="C37" s="18">
         <v>2</v>
       </c>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="100"/>
-      <c r="F37" s="42" t="s">
+      <c r="E37" s="108"/>
+      <c r="F37" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="32" t="s">
+      <c r="G37" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="96"/>
-      <c r="C38" s="17">
+      <c r="B38" s="104"/>
+      <c r="C38" s="16">
         <v>3</v>
       </c>
-      <c r="D38" s="101" t="s">
+      <c r="D38" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="102"/>
-      <c r="F38" s="69" t="s">
+      <c r="E38" s="110"/>
+      <c r="F38" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="32" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3008,422 +3022,460 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
   <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="22"/>
-    <col min="5" max="5" width="45.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="21"/>
+    <col min="5" max="5" width="45.42578125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="112" t="s">
+      <c r="C2" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="114"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="122"/>
     </row>
     <row r="3" spans="2:7" ht="28.5" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="126" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="120"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="128"/>
     </row>
     <row r="4" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="120"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="128"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="89"/>
+      <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="29.25">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>1</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="128"/>
-      <c r="F6" s="43" t="s">
+      <c r="E6" s="136"/>
+      <c r="F6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="30" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="110"/>
-      <c r="C7" s="23">
+      <c r="B7" s="118"/>
+      <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="23" t="s">
+      <c r="E7" s="95"/>
+      <c r="F7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="2:7" ht="43.5">
-      <c r="B8" s="110"/>
-      <c r="C8" s="23">
+      <c r="B8" s="118"/>
+      <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="85"/>
-      <c r="F8" s="39" t="s">
+      <c r="E8" s="93"/>
+      <c r="F8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="110"/>
-      <c r="C9" s="23">
+      <c r="B9" s="118"/>
+      <c r="C9" s="22">
         <v>4</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="23" t="s">
+      <c r="E9" s="95"/>
+      <c r="F9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="43.5">
-      <c r="B10" s="110"/>
-      <c r="C10" s="23">
+      <c r="B10" s="118"/>
+      <c r="C10" s="22">
         <v>5</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="85"/>
-      <c r="F10" s="39" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="110"/>
-      <c r="C11" s="16">
+      <c r="B11" s="118"/>
+      <c r="C11" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="131" t="s">
+      <c r="D11" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="132"/>
-      <c r="F11" s="62" t="s">
+      <c r="E11" s="140"/>
+      <c r="F11" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="33"/>
+      <c r="G11" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:7" ht="29.25">
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="51">
         <v>1</v>
       </c>
-      <c r="D12" s="127" t="s">
+      <c r="D12" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="128"/>
-      <c r="F12" s="63" t="s">
+      <c r="E12" s="136"/>
+      <c r="F12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1">
-      <c r="B13" s="110"/>
-      <c r="C13" s="35">
+      <c r="B13" s="118"/>
+      <c r="C13" s="34">
         <v>2</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="19" t="s">
+      <c r="E13" s="95"/>
+      <c r="F13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="2:7" ht="43.5">
-      <c r="B14" s="110"/>
-      <c r="C14" s="35">
+      <c r="B14" s="118"/>
+      <c r="C14" s="34">
         <v>3</v>
       </c>
-      <c r="D14" s="84" t="s">
+      <c r="D14" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="64" t="s">
+      <c r="E14" s="93"/>
+      <c r="F14" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="110"/>
-      <c r="C15" s="35">
+      <c r="B15" s="118"/>
+      <c r="C15" s="34">
         <v>4</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="87"/>
-      <c r="F15" s="19" t="s">
+      <c r="E15" s="95"/>
+      <c r="F15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="110"/>
-      <c r="C16" s="35">
+      <c r="B16" s="118"/>
+      <c r="C16" s="34">
         <v>5</v>
       </c>
-      <c r="D16" s="129" t="s">
+      <c r="D16" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="135"/>
+      <c r="E16" s="143"/>
       <c r="F16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="76" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="43.5">
-      <c r="B17" s="110"/>
-      <c r="C17" s="35">
+      <c r="B17" s="118"/>
+      <c r="C17" s="34">
         <v>6</v>
       </c>
-      <c r="D17" s="84" t="s">
+      <c r="D17" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="85"/>
-      <c r="F17" s="64" t="s">
+      <c r="E17" s="93"/>
+      <c r="F17" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="29.25">
-      <c r="B18" s="111"/>
-      <c r="C18" s="45">
+      <c r="B18" s="119"/>
+      <c r="C18" s="44">
         <v>7</v>
       </c>
-      <c r="D18" s="131" t="s">
+      <c r="D18" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="132"/>
-      <c r="F18" s="65" t="s">
+      <c r="E18" s="140"/>
+      <c r="F18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="66"/>
-      <c r="F19" s="26"/>
+      <c r="B19" s="65"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="112" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="113"/>
-      <c r="E23" s="114"/>
+      <c r="C23" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="121"/>
+      <c r="E23" s="122"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="118" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="119"/>
-      <c r="E24" s="120"/>
+      <c r="C24" s="126" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="127"/>
+      <c r="E24" s="128"/>
     </row>
     <row r="25" spans="2:7" ht="15" customHeight="1">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="118" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="119"/>
-      <c r="E25" s="120"/>
+      <c r="C25" s="126" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="127"/>
+      <c r="E25" s="128"/>
     </row>
     <row r="26" spans="2:7" ht="29.25" customHeight="1">
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="103" t="s">
+      <c r="D26" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="104"/>
-      <c r="F26" s="24" t="s">
+      <c r="E26" s="112"/>
+      <c r="F26" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="29.25">
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="27">
         <v>1</v>
       </c>
-      <c r="D27" s="121" t="s">
+      <c r="D27" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="122"/>
-      <c r="F27" s="34" t="s">
+      <c r="E27" s="130"/>
+      <c r="F27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="31"/>
+      <c r="G27" s="30" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="110"/>
-      <c r="C28" s="19">
+      <c r="B28" s="118"/>
+      <c r="C28" s="18">
         <v>2</v>
       </c>
-      <c r="D28" s="123" t="s">
+      <c r="D28" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="124"/>
-      <c r="F28" s="35" t="s">
+      <c r="E28" s="132"/>
+      <c r="F28" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B29" s="110"/>
-      <c r="C29" s="19">
+      <c r="B29" s="118"/>
+      <c r="C29" s="18">
         <v>3</v>
       </c>
-      <c r="D29" s="123" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="124"/>
-      <c r="F29" s="26" t="s">
+      <c r="D29" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="110"/>
-      <c r="C30" s="19">
+      <c r="B30" s="118"/>
+      <c r="C30" s="18">
         <v>4</v>
       </c>
-      <c r="D30" s="129" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="130"/>
-      <c r="F30" s="35" t="s">
+      <c r="D30" s="137" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="138"/>
+      <c r="F30" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="43.5">
-      <c r="B31" s="110"/>
-      <c r="C31" s="29">
+      <c r="B31" s="118"/>
+      <c r="C31" s="28">
         <v>5</v>
       </c>
-      <c r="D31" s="84" t="s">
+      <c r="D31" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="85"/>
-      <c r="F31" s="39" t="s">
+      <c r="E31" s="93"/>
+      <c r="F31" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="111"/>
-      <c r="C32" s="30">
+      <c r="B32" s="119"/>
+      <c r="C32" s="29">
         <v>6</v>
       </c>
-      <c r="D32" s="125" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="126"/>
-      <c r="F32" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="33"/>
+      <c r="D32" s="133" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="134"/>
+      <c r="F32" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1"/>
     <row r="36" spans="2:7">
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="112" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="113"/>
-      <c r="E36" s="114"/>
+      <c r="C36" s="120" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="121"/>
+      <c r="E36" s="122"/>
     </row>
     <row r="37" spans="2:7" ht="28.5" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="119"/>
-      <c r="E37" s="120"/>
+      <c r="C37" s="126" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="127"/>
+      <c r="E37" s="128"/>
     </row>
     <row r="38" spans="2:7" ht="48" customHeight="1">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="115" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="116"/>
-      <c r="E38" s="117"/>
+      <c r="C38" s="123" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="124"/>
+      <c r="E38" s="125"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="6" t="s">
@@ -3432,10 +3484,10 @@
       <c r="C39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="103" t="s">
+      <c r="D39" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="104"/>
+      <c r="E39" s="112"/>
       <c r="F39" s="7" t="s">
         <v>9</v>
       </c>
@@ -3444,142 +3496,160 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="29.25">
-      <c r="B40" s="109" t="s">
+      <c r="B40" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="24">
         <v>1</v>
       </c>
-      <c r="D40" s="121" t="s">
+      <c r="D40" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="122"/>
-      <c r="F40" s="27" t="s">
+      <c r="E40" s="130"/>
+      <c r="F40" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="110"/>
-      <c r="C41" s="23">
+      <c r="B41" s="118"/>
+      <c r="C41" s="22">
         <v>2</v>
       </c>
-      <c r="D41" s="123" t="s">
+      <c r="D41" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="124"/>
-      <c r="F41" s="19" t="s">
+      <c r="E41" s="132"/>
+      <c r="F41" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="11"/>
+      <c r="G41" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="2:7" ht="15" customHeight="1">
-      <c r="B42" s="110"/>
-      <c r="C42" s="23">
+      <c r="B42" s="118"/>
+      <c r="C42" s="22">
         <v>3</v>
       </c>
-      <c r="D42" s="129" t="s">
+      <c r="D42" s="137" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="130"/>
-      <c r="F42" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="11"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="111"/>
-      <c r="C43" s="59">
+      <c r="B43" s="119"/>
+      <c r="C43" s="58">
         <v>4</v>
       </c>
-      <c r="D43" s="101" t="s">
+      <c r="D43" s="109" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="142"/>
+      <c r="F43" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="29.25">
+      <c r="B44" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="51">
+        <v>1</v>
+      </c>
+      <c r="D44" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="130"/>
+      <c r="F44" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="118"/>
+      <c r="C45" s="34">
+        <v>2</v>
+      </c>
+      <c r="D45" s="131" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="132"/>
+      <c r="F45" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="118"/>
+      <c r="C46" s="34">
+        <v>3</v>
+      </c>
+      <c r="D46" s="137" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="138"/>
+      <c r="F46" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="134"/>
-      <c r="F43" s="61" t="s">
+      <c r="G46" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="43.5">
+      <c r="B47" s="118"/>
+      <c r="C47" s="34">
+        <v>4</v>
+      </c>
+      <c r="D47" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="44" spans="2:7" ht="29.25">
-      <c r="B44" s="109" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="52">
-        <v>1</v>
-      </c>
-      <c r="D44" s="121" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="122"/>
-      <c r="F44" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="31"/>
-    </row>
-    <row r="45" spans="2:7">
-      <c r="B45" s="110"/>
-      <c r="C45" s="35">
-        <v>2</v>
-      </c>
-      <c r="D45" s="123" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="124"/>
-      <c r="F45" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" spans="2:7">
-      <c r="B46" s="110"/>
-      <c r="C46" s="35">
-        <v>3</v>
-      </c>
-      <c r="D46" s="129" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="130"/>
-      <c r="F46" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G46" s="32"/>
-    </row>
-    <row r="47" spans="2:7" ht="43.5">
-      <c r="B47" s="110"/>
-      <c r="C47" s="35">
-        <v>4</v>
-      </c>
-      <c r="D47" s="129" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="130"/>
-      <c r="F47" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="32"/>
+      <c r="E47" s="138"/>
+      <c r="F47" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G47" s="77" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="48" spans="2:7" ht="35.25" customHeight="1">
-      <c r="B48" s="111"/>
-      <c r="C48" s="45">
+      <c r="B48" s="119"/>
+      <c r="C48" s="44">
         <v>5</v>
       </c>
-      <c r="D48" s="101" t="s">
+      <c r="D48" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="134"/>
-      <c r="F48" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G48" s="33"/>
+      <c r="E48" s="142"/>
+      <c r="F48" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" s="78" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="133"/>
-      <c r="E49" s="133"/>
+      <c r="D49" s="141"/>
+      <c r="E49" s="141"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="133"/>
-      <c r="E50" s="133"/>
+      <c r="D50" s="141"/>
+      <c r="E50" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -3639,16 +3709,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="22"/>
+    <col min="3" max="3" width="6.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="21"/>
     <col min="5" max="5" width="52.85546875" customWidth="1"/>
     <col min="6" max="6" width="57.85546875" customWidth="1"/>
   </cols>
@@ -3657,747 +3727,821 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="155" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="156"/>
-      <c r="E2" s="157"/>
+      <c r="C2" s="163" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
     </row>
     <row r="3" spans="2:7" ht="30" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="79"/>
+      <c r="C3" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="86"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="78" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
+      <c r="C4" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="51">
         <v>1</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="146"/>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="154"/>
+      <c r="F6" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="30" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="110"/>
-      <c r="C7" s="35">
+      <c r="B7" s="118"/>
+      <c r="C7" s="34">
         <v>2</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="80"/>
+      <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="110"/>
-      <c r="C8" s="35">
+      <c r="B8" s="118"/>
+      <c r="C8" s="34">
         <v>3</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="42" t="s">
+      <c r="E8" s="80"/>
+      <c r="F8" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="110"/>
-      <c r="C9" s="35">
+      <c r="B9" s="118"/>
+      <c r="C9" s="34">
         <v>4</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="39" t="s">
+      <c r="E9" s="95"/>
+      <c r="F9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="45.75" customHeight="1">
-      <c r="B10" s="110"/>
-      <c r="C10" s="35">
+      <c r="B10" s="118"/>
+      <c r="C10" s="34">
         <v>5</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="85"/>
-      <c r="F10" s="39" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="110"/>
-      <c r="C11" s="35">
+      <c r="B11" s="118"/>
+      <c r="C11" s="34">
         <v>6</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="39" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="110"/>
-      <c r="C12" s="35">
+      <c r="B12" s="118"/>
+      <c r="C12" s="34">
         <v>7</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="51" t="s">
+      <c r="E12" s="80"/>
+      <c r="F12" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="110"/>
-      <c r="C13" s="35">
+      <c r="B13" s="118"/>
+      <c r="C13" s="34">
         <v>8</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="51" t="s">
+      <c r="E13" s="95"/>
+      <c r="F13" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="111"/>
-      <c r="C14" s="55">
+      <c r="B14" s="119"/>
+      <c r="C14" s="54">
         <v>9</v>
       </c>
-      <c r="D14" s="160" t="s">
+      <c r="D14" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="54" t="s">
+      <c r="E14" s="169"/>
+      <c r="F14" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="52" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="27">
         <v>1</v>
       </c>
-      <c r="D15" s="159" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="146"/>
+      <c r="D15" s="167" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="154"/>
       <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="110"/>
-      <c r="C16" s="19">
+      <c r="B16" s="118"/>
+      <c r="C16" s="18">
         <v>2</v>
       </c>
-      <c r="D16" s="143" t="s">
+      <c r="D16" s="151" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="80"/>
+      <c r="F16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="118"/>
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="152" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="153"/>
+      <c r="F17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="119"/>
+      <c r="C18" s="29">
+        <v>4</v>
+      </c>
+      <c r="D18" s="148" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="140"/>
+      <c r="F18" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="171" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="117" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="27">
+        <v>1</v>
+      </c>
+      <c r="D19" s="149" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="154"/>
+      <c r="F19" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="118"/>
+      <c r="C20" s="18">
+        <v>2</v>
+      </c>
+      <c r="D20" s="151" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="80"/>
+      <c r="F20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="118"/>
+      <c r="C21" s="18">
+        <v>3</v>
+      </c>
+      <c r="D21" s="152" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="153"/>
+      <c r="F21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="119"/>
+      <c r="C22" s="29">
+        <v>4</v>
+      </c>
+      <c r="D22" s="148" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="140"/>
+      <c r="F22" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="117" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="27">
+        <v>1</v>
+      </c>
+      <c r="D23" s="149" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="72"/>
-      <c r="F16" s="15" t="s">
+      <c r="E23" s="154"/>
+      <c r="F23" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="110"/>
-      <c r="C17" s="19">
-        <v>3</v>
-      </c>
-      <c r="D17" s="144" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="145"/>
-      <c r="F17" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="111"/>
-      <c r="C18" s="30">
-        <v>4</v>
-      </c>
-      <c r="D18" s="140" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="132"/>
-      <c r="F18" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="109" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="28">
-        <v>1</v>
-      </c>
-      <c r="D19" s="141" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="146"/>
-      <c r="F19" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="110"/>
-      <c r="C20" s="19">
+      <c r="G23" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="118"/>
+      <c r="C24" s="18">
         <v>2</v>
       </c>
-      <c r="D20" s="143" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="72"/>
-      <c r="F20" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="110"/>
-      <c r="C21" s="19">
-        <v>3</v>
-      </c>
-      <c r="D21" s="144" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="145"/>
-      <c r="F21" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="111"/>
-      <c r="C22" s="30">
-        <v>4</v>
-      </c>
-      <c r="D22" s="140" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="132"/>
-      <c r="F22" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="109" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="28">
-        <v>1</v>
-      </c>
-      <c r="D23" s="141" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="146"/>
-      <c r="F23" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="110"/>
-      <c r="C24" s="19">
-        <v>2</v>
-      </c>
-      <c r="D24" s="143" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="72"/>
+      <c r="D24" s="151" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="80"/>
       <c r="F24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="110"/>
-      <c r="C25" s="19">
+      <c r="B25" s="118"/>
+      <c r="C25" s="18">
         <v>3</v>
       </c>
-      <c r="D25" s="144" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="145"/>
-      <c r="F25" s="15" t="s">
+      <c r="D25" s="152" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="153"/>
+      <c r="F25" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="110"/>
-      <c r="C26" s="30">
+      <c r="B26" s="118"/>
+      <c r="C26" s="29">
         <v>4</v>
       </c>
-      <c r="D26" s="140" t="s">
+      <c r="D26" s="148" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="132"/>
-      <c r="F26" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="G26" s="14"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="47">
+      <c r="C27" s="46">
         <v>1</v>
       </c>
-      <c r="D27" s="97" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="162"/>
-      <c r="F27" s="15" t="s">
+      <c r="D27" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="170"/>
+      <c r="F27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="110"/>
-      <c r="C28" s="46">
+      <c r="B28" s="118"/>
+      <c r="C28" s="45">
         <v>2</v>
       </c>
-      <c r="D28" s="143" t="s">
+      <c r="D28" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="80"/>
+      <c r="F28" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="118"/>
+      <c r="C29" s="45">
+        <v>3</v>
+      </c>
+      <c r="D29" s="152" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="153"/>
+      <c r="F29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="119"/>
+      <c r="C30" s="47">
+        <v>4</v>
+      </c>
+      <c r="D30" s="148" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="140"/>
+      <c r="F30" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="72"/>
-      <c r="F28" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="110"/>
-      <c r="C29" s="46">
-        <v>3</v>
-      </c>
-      <c r="D29" s="144" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="145"/>
-      <c r="F29" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="111"/>
-      <c r="C30" s="48">
-        <v>4</v>
-      </c>
-      <c r="D30" s="140" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="132"/>
-      <c r="F30" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="27">
         <v>1</v>
       </c>
-      <c r="D31" s="141" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="146"/>
+      <c r="D31" s="149" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="154"/>
       <c r="F31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="13"/>
+      <c r="G31" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="110"/>
-      <c r="C32" s="19">
+      <c r="B32" s="118"/>
+      <c r="C32" s="18">
         <v>2</v>
       </c>
-      <c r="D32" s="141" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="146"/>
+      <c r="D32" s="149" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="154"/>
       <c r="F32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="110"/>
-      <c r="C33" s="19">
+      <c r="B33" s="118"/>
+      <c r="C33" s="18">
         <v>3</v>
       </c>
-      <c r="D33" s="147" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" s="148"/>
-      <c r="F33" s="19" t="s">
+      <c r="D33" s="155" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="156"/>
+      <c r="F33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="11"/>
+      <c r="G33" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="2:7" ht="29.25">
-      <c r="B34" s="111"/>
-      <c r="C34" s="30">
+      <c r="B34" s="119"/>
+      <c r="C34" s="29">
         <v>4</v>
       </c>
-      <c r="D34" s="149" t="s">
+      <c r="D34" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="150"/>
-      <c r="F34" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="G34" s="14"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" s="171" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" spans="2:7" ht="31.5" customHeight="1">
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="39">
         <v>1</v>
       </c>
-      <c r="D35" s="151" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="152"/>
-      <c r="F35" s="47" t="s">
+      <c r="D35" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="160"/>
+      <c r="F35" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="13"/>
+      <c r="G35" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B36" s="110"/>
-      <c r="C36" s="23">
+      <c r="B36" s="118"/>
+      <c r="C36" s="22">
         <v>2</v>
       </c>
-      <c r="D36" s="137" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="138"/>
-      <c r="F36" s="46" t="s">
+      <c r="D36" s="145" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="146"/>
+      <c r="F36" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="11"/>
+      <c r="G36" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B37" s="110"/>
-      <c r="C37" s="23">
+      <c r="B37" s="118"/>
+      <c r="C37" s="22">
         <v>3</v>
       </c>
-      <c r="D37" s="137" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="138"/>
-      <c r="F37" s="46" t="s">
+      <c r="D37" s="145" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="146"/>
+      <c r="F37" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="11"/>
+      <c r="G37" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="29.25">
-      <c r="B38" s="111"/>
-      <c r="C38" s="16">
+      <c r="B38" s="119"/>
+      <c r="C38" s="15">
         <v>4</v>
       </c>
-      <c r="D38" s="153" t="s">
+      <c r="D38" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="154"/>
-      <c r="F38" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="14"/>
+      <c r="E38" s="162"/>
+      <c r="F38" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="171" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
-      <c r="B39" s="110" t="s">
+      <c r="B39" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="40">
+      <c r="C39" s="39">
         <v>1</v>
       </c>
-      <c r="D39" s="141" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="142"/>
-      <c r="F39" s="56" t="s">
+      <c r="D39" s="149" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="150"/>
+      <c r="F39" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="13"/>
+      <c r="G39" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="15" customHeight="1">
-      <c r="B40" s="110"/>
-      <c r="C40" s="23">
+      <c r="B40" s="118"/>
+      <c r="C40" s="22">
         <v>2</v>
       </c>
-      <c r="D40" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="136"/>
-      <c r="F40" s="57" t="s">
+      <c r="D40" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="144"/>
+      <c r="F40" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="11"/>
+      <c r="G40" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1">
-      <c r="B41" s="110"/>
-      <c r="C41" s="23">
+      <c r="B41" s="118"/>
+      <c r="C41" s="22">
         <v>3</v>
       </c>
-      <c r="D41" s="137" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" s="138"/>
-      <c r="F41" s="46" t="s">
+      <c r="D41" s="145" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="146"/>
+      <c r="F41" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="11"/>
+      <c r="G41" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="111"/>
-      <c r="C42" s="16">
+      <c r="B42" s="119"/>
+      <c r="C42" s="15">
         <v>4</v>
       </c>
-      <c r="D42" s="131" t="s">
-        <v>107</v>
-      </c>
-      <c r="E42" s="139"/>
-      <c r="F42" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="G42" s="14"/>
+      <c r="D42" s="139" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="147"/>
+      <c r="F42" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="171" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="D43" s="88"/>
-      <c r="E43" s="88"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="D44" s="88"/>
-      <c r="E44" s="88"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="D46" s="88"/>
-      <c r="E46" s="88"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="D47" s="88"/>
-      <c r="E47" s="88"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="88"/>
-      <c r="E49" s="88"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="88"/>
-      <c r="E50" s="88"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="88"/>
-      <c r="E51" s="88"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="96"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="88"/>
-      <c r="E52" s="88"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="88"/>
-      <c r="E53" s="88"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="96"/>
     </row>
     <row r="54" spans="4:5">
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="96"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="96"/>
     </row>
     <row r="56" spans="4:5">
-      <c r="D56" s="88"/>
-      <c r="E56" s="88"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="96"/>
     </row>
     <row r="57" spans="4:5">
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
+      <c r="D57" s="96"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="4:5">
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="96"/>
     </row>
     <row r="59" spans="4:5">
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
+      <c r="D59" s="96"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="4:5">
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
+      <c r="D60" s="96"/>
+      <c r="E60" s="96"/>
     </row>
     <row r="61" spans="4:5">
-      <c r="D61" s="88"/>
-      <c r="E61" s="88"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
     </row>
     <row r="62" spans="4:5">
-      <c r="D62" s="88"/>
-      <c r="E62" s="88"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="96"/>
     </row>
     <row r="63" spans="4:5">
-      <c r="D63" s="88"/>
-      <c r="E63" s="88"/>
+      <c r="D63" s="96"/>
+      <c r="E63" s="96"/>
     </row>
     <row r="64" spans="4:5">
-      <c r="D64" s="88"/>
-      <c r="E64" s="88"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="96"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="88"/>
-      <c r="E65" s="88"/>
+      <c r="D65" s="96"/>
+      <c r="E65" s="96"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="88"/>
-      <c r="E66" s="88"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="96"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="88"/>
-      <c r="E67" s="88"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="88"/>
-      <c r="E68" s="88"/>
+      <c r="D68" s="96"/>
+      <c r="E68" s="96"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="88"/>
-      <c r="E69" s="88"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="96"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="88"/>
-      <c r="E70" s="88"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="96"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="88"/>
-      <c r="E71" s="88"/>
+      <c r="D71" s="96"/>
+      <c r="E71" s="96"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="88"/>
-      <c r="E72" s="88"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="4:5">
-      <c r="D73" s="88"/>
-      <c r="E73" s="88"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="96"/>
     </row>
     <row r="74" spans="4:5">
-      <c r="D74" s="88"/>
-      <c r="E74" s="88"/>
+      <c r="D74" s="96"/>
+      <c r="E74" s="96"/>
     </row>
     <row r="75" spans="4:5">
-      <c r="D75" s="88"/>
-      <c r="E75" s="88"/>
+      <c r="D75" s="96"/>
+      <c r="E75" s="96"/>
     </row>
     <row r="76" spans="4:5">
-      <c r="D76" s="88"/>
-      <c r="E76" s="88"/>
+      <c r="D76" s="96"/>
+      <c r="E76" s="96"/>
     </row>
     <row r="77" spans="4:5">
-      <c r="D77" s="88"/>
-      <c r="E77" s="88"/>
+      <c r="D77" s="96"/>
+      <c r="E77" s="96"/>
     </row>
     <row r="78" spans="4:5">
-      <c r="D78" s="88"/>
-      <c r="E78" s="88"/>
+      <c r="D78" s="96"/>
+      <c r="E78" s="96"/>
     </row>
     <row r="79" spans="4:5">
-      <c r="D79" s="88"/>
-      <c r="E79" s="88"/>
+      <c r="D79" s="96"/>
+      <c r="E79" s="96"/>
     </row>
     <row r="80" spans="4:5">
-      <c r="D80" s="88"/>
-      <c r="E80" s="88"/>
+      <c r="D80" s="96"/>
+      <c r="E80" s="96"/>
     </row>
     <row r="81" spans="4:5">
-      <c r="D81" s="88"/>
-      <c r="E81" s="88"/>
+      <c r="D81" s="96"/>
+      <c r="E81" s="96"/>
     </row>
     <row r="82" spans="4:5">
-      <c r="D82" s="88"/>
-      <c r="E82" s="88"/>
+      <c r="D82" s="96"/>
+      <c r="E82" s="96"/>
     </row>
     <row r="83" spans="4:5">
-      <c r="D83" s="88"/>
-      <c r="E83" s="88"/>
+      <c r="D83" s="96"/>
+      <c r="E83" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="90">

</xml_diff>

<commit_message>
adicionei mais dois bdds de imagens dos produtos e bloqueio de conta do usuario. Testou negativo CT009
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14169466-00FE-4780-B6C1-B8E47B7B0A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D93B441A-0C5D-459E-8975-32B3E8806DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
     <sheet name="LOGIN" sheetId="1" r:id="rId2"/>
     <sheet name="PRODUCTS - YOUR CART" sheetId="2" r:id="rId3"/>
     <sheet name="CHECKOUT - FINISH" sheetId="4" r:id="rId4"/>
+    <sheet name="EXTRA" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="132">
   <si>
     <t>Cenário</t>
   </si>
@@ -394,6 +395,42 @@
   </si>
   <si>
     <t>Preencher o campo de Postal Code com o  caracteres especiais.</t>
+  </si>
+  <si>
+    <t>Bloqueio de Conta no Login</t>
+  </si>
+  <si>
+    <t>Garantir que o sistema bloqueie o acesso de contas desativadas e informe o usuário adequadamente.</t>
+  </si>
+  <si>
+    <t>O sistema deve impedir o acesso de usuários com contas bloqueadas e exibir uma mensagem clara informando o motivo do bloqueio.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Username com um username com 'locked_out_user'</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Password com uma senha 'secret_sauce'.</t>
+  </si>
+  <si>
+    <t>O sistema deverá impedir a próxima etapa. O sistema exibirá a mensagem: 'Epic sadface: Sorry, this user has been locked out.'.</t>
+  </si>
+  <si>
+    <t>Login com usuário problemático e verificação das imagens dos produtos</t>
+  </si>
+  <si>
+    <t>Garantir que, após o login com um usuário problemático, as imagens dos produtos sejam carregadas e exibidas corretamente na página de produtos.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir o login de usuários com o username "problem_user" e garantir que as imagens dos produtos sejam visíveis na página de produtos após o login.</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Username com um username com 'problem_user'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar as imgens dos produtos são visiveis </t>
+  </si>
+  <si>
+    <t>As imagens dos produtos devem ser visíveis na página de products.</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1317,12 +1354,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1356,36 +1424,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,12 +1451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1431,6 +1463,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1440,13 +1484,55 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1458,142 +1544,115 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1930,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1948,31 +2007,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="43" t="s">
@@ -1981,10 +2040,10 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1993,16 +2052,16 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="39">
         <v>1</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="91"/>
+      <c r="E6" s="102"/>
       <c r="F6" s="66" t="s">
         <v>13</v>
       </c>
@@ -2011,14 +2070,14 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="98"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
@@ -2027,14 +2086,14 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="98"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="41" t="s">
         <v>17</v>
       </c>
@@ -2043,14 +2102,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="29.25">
-      <c r="B9" s="98"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="22">
         <v>4</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="38" t="s">
         <v>19</v>
       </c>
@@ -2059,14 +2118,14 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="98"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="22">
         <v>5</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="95"/>
+      <c r="E10" s="87"/>
       <c r="F10" s="22" t="s">
         <v>21</v>
       </c>
@@ -2075,14 +2134,14 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="98"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="22">
         <v>6</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="93"/>
+      <c r="E11" s="91"/>
       <c r="F11" s="38" t="s">
         <v>23</v>
       </c>
@@ -2091,14 +2150,14 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="98"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="22">
         <v>7</v>
       </c>
-      <c r="D12" s="94" t="s">
+      <c r="D12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="22" t="s">
         <v>25</v>
       </c>
@@ -2107,14 +2166,14 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="43.5">
-      <c r="B13" s="98"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="22">
         <v>8</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="93"/>
+      <c r="E13" s="91"/>
       <c r="F13" s="38" t="s">
         <v>27</v>
       </c>
@@ -2123,14 +2182,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1">
-      <c r="B14" s="98"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="22">
         <v>9</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="95"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="38" t="s">
         <v>29</v>
       </c>
@@ -2139,14 +2198,14 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="98"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="22">
         <v>10</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="80"/>
+      <c r="E15" s="85"/>
       <c r="F15" s="41" t="s">
         <v>13</v>
       </c>
@@ -2155,14 +2214,14 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="98"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="22">
         <v>11</v>
       </c>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="85"/>
       <c r="F16" s="41" t="s">
         <v>13</v>
       </c>
@@ -2171,14 +2230,14 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="98"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="22">
         <v>12</v>
       </c>
-      <c r="D17" s="79" t="s">
+      <c r="D17" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="80"/>
+      <c r="E17" s="85"/>
       <c r="F17" s="41" t="s">
         <v>13</v>
       </c>
@@ -2187,14 +2246,14 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="98"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="22">
         <v>13</v>
       </c>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="95"/>
+      <c r="E18" s="87"/>
       <c r="F18" s="38" t="s">
         <v>34</v>
       </c>
@@ -2203,14 +2262,14 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="43.5">
-      <c r="B19" s="98"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="22">
         <v>14</v>
       </c>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="93"/>
+      <c r="E19" s="91"/>
       <c r="F19" s="38" t="s">
         <v>36</v>
       </c>
@@ -2219,14 +2278,14 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="43.5">
-      <c r="B20" s="98"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="22">
         <v>15</v>
       </c>
-      <c r="D20" s="92" t="s">
+      <c r="D20" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="93"/>
+      <c r="E20" s="91"/>
       <c r="F20" s="38" t="s">
         <v>38</v>
       </c>
@@ -2235,14 +2294,14 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="98"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="22">
         <v>16</v>
       </c>
-      <c r="D21" s="79" t="s">
+      <c r="D21" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="80"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="50" t="s">
         <v>40</v>
       </c>
@@ -2251,14 +2310,14 @@
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="98"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="22">
         <v>17</v>
       </c>
-      <c r="D22" s="94" t="s">
+      <c r="D22" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="95"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="50" t="s">
         <v>42</v>
       </c>
@@ -2267,14 +2326,14 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="99"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="15">
         <v>18</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D23" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="101"/>
+      <c r="E23" s="89"/>
       <c r="F23" s="67" t="s">
         <v>44</v>
       </c>
@@ -2283,35 +2342,49 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="D26" s="96"/>
-      <c r="E26" s="96"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="D30" s="96"/>
-      <c r="E30" s="96"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
@@ -2328,20 +2401,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2351,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2369,31 +2428,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
@@ -2402,10 +2461,10 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="117"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2414,16 +2473,16 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="103" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="106"/>
+      <c r="E6" s="107"/>
       <c r="F6" s="40" t="s">
         <v>13</v>
       </c>
@@ -2432,14 +2491,14 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="103"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="18">
         <v>2</v>
       </c>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="108"/>
+      <c r="E7" s="109"/>
       <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
@@ -2448,14 +2507,14 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="104"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="17">
         <v>3</v>
       </c>
-      <c r="D8" s="113" t="s">
+      <c r="D8" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="114"/>
+      <c r="E8" s="113"/>
       <c r="F8" s="69" t="s">
         <v>17</v>
       </c>
@@ -2464,16 +2523,16 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="103" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="106"/>
+      <c r="E9" s="107"/>
       <c r="F9" s="40" t="s">
         <v>13</v>
       </c>
@@ -2482,14 +2541,14 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="103"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="18">
         <v>2</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="108"/>
+      <c r="E10" s="109"/>
       <c r="F10" s="41" t="s">
         <v>13</v>
       </c>
@@ -2498,14 +2557,14 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="104"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="17">
         <v>3</v>
       </c>
-      <c r="D11" s="109" t="s">
+      <c r="D11" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="110"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="70" t="s">
         <v>50</v>
       </c>
@@ -2514,16 +2573,16 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="103" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="19">
         <v>1</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="106"/>
+      <c r="E12" s="107"/>
       <c r="F12" s="40" t="s">
         <v>13</v>
       </c>
@@ -2532,14 +2591,14 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="103"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="18">
         <v>2</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="108"/>
+      <c r="E13" s="109"/>
       <c r="F13" s="41" t="s">
         <v>13</v>
       </c>
@@ -2548,14 +2607,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="29.25">
-      <c r="B14" s="104"/>
+      <c r="B14" s="105"/>
       <c r="C14" s="16">
         <v>3</v>
       </c>
-      <c r="D14" s="109" t="s">
+      <c r="D14" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="110"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="70" t="s">
         <v>50</v>
       </c>
@@ -2564,16 +2623,16 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="103" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="106"/>
+      <c r="E15" s="107"/>
       <c r="F15" s="40" t="s">
         <v>13</v>
       </c>
@@ -2582,14 +2641,14 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="103"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="18">
         <v>2</v>
       </c>
-      <c r="D16" s="107" t="s">
+      <c r="D16" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="F16" s="71" t="s">
         <v>55</v>
       </c>
@@ -2598,14 +2657,14 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="104"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="16">
         <v>3</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D17" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="114"/>
+      <c r="E17" s="113"/>
       <c r="F17" s="72" t="s">
         <v>56</v>
       </c>
@@ -2614,16 +2673,16 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="103" t="s">
         <v>57</v>
       </c>
       <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="105" t="s">
+      <c r="D18" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="106"/>
+      <c r="E18" s="107"/>
       <c r="F18" s="71" t="s">
         <v>55</v>
       </c>
@@ -2632,14 +2691,14 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="103"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="18">
         <v>2</v>
       </c>
-      <c r="D19" s="107" t="s">
+      <c r="D19" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="108"/>
+      <c r="E19" s="109"/>
       <c r="F19" s="41" t="s">
         <v>13</v>
       </c>
@@ -2648,14 +2707,14 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="104"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="16">
         <v>3</v>
       </c>
-      <c r="D20" s="113" t="s">
+      <c r="D20" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="114"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="72" t="s">
         <v>59</v>
       </c>
@@ -2664,16 +2723,16 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="102" t="s">
+      <c r="B21" s="103" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="106"/>
+      <c r="E21" s="107"/>
       <c r="F21" s="71" t="s">
         <v>55</v>
       </c>
@@ -2682,14 +2741,14 @@
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="103"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="18">
         <v>2</v>
       </c>
-      <c r="D22" s="107" t="s">
+      <c r="D22" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="108"/>
+      <c r="E22" s="109"/>
       <c r="F22" s="71" t="s">
         <v>55</v>
       </c>
@@ -2698,14 +2757,14 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="104"/>
+      <c r="B23" s="105"/>
       <c r="C23" s="17">
         <v>3</v>
       </c>
-      <c r="D23" s="115" t="s">
+      <c r="D23" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="116"/>
+      <c r="E23" s="115"/>
       <c r="F23" s="73" t="s">
         <v>59</v>
       </c>
@@ -2714,16 +2773,16 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="102" t="s">
+      <c r="B24" s="103" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="19">
         <v>1</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="106"/>
+      <c r="E24" s="107"/>
       <c r="F24" s="40" t="s">
         <v>13</v>
       </c>
@@ -2732,14 +2791,14 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="103"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="18">
         <v>2</v>
       </c>
-      <c r="D25" s="107" t="s">
+      <c r="D25" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="108"/>
+      <c r="E25" s="109"/>
       <c r="F25" s="41" t="s">
         <v>13</v>
       </c>
@@ -2748,14 +2807,14 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="29.25">
-      <c r="B26" s="104"/>
+      <c r="B26" s="105"/>
       <c r="C26" s="16">
         <v>3</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="110"/>
+      <c r="E26" s="111"/>
       <c r="F26" s="74" t="s">
         <v>50</v>
       </c>
@@ -2764,16 +2823,16 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="102" t="s">
+      <c r="B27" s="103" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="19">
         <v>1</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="106"/>
+      <c r="E27" s="107"/>
       <c r="F27" s="40" t="s">
         <v>13</v>
       </c>
@@ -2782,14 +2841,14 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="103"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="18">
         <v>2</v>
       </c>
-      <c r="D28" s="107" t="s">
+      <c r="D28" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="108"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="41" t="s">
         <v>13</v>
       </c>
@@ -2798,14 +2857,14 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="29.25">
-      <c r="B29" s="104"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="16">
         <v>3</v>
       </c>
-      <c r="D29" s="109" t="s">
+      <c r="D29" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="110"/>
+      <c r="E29" s="111"/>
       <c r="F29" s="74" t="s">
         <v>50</v>
       </c>
@@ -2814,16 +2873,16 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="102" t="s">
+      <c r="B30" s="103" t="s">
         <v>66</v>
       </c>
       <c r="C30" s="19">
         <v>1</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="106"/>
+      <c r="E30" s="107"/>
       <c r="F30" s="40" t="s">
         <v>13</v>
       </c>
@@ -2832,14 +2891,14 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="103"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="18">
         <v>2</v>
       </c>
-      <c r="D31" s="107" t="s">
+      <c r="D31" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="108"/>
+      <c r="E31" s="109"/>
       <c r="F31" s="41" t="s">
         <v>13</v>
       </c>
@@ -2848,14 +2907,14 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="104"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="16">
         <v>3</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="110"/>
+      <c r="E32" s="111"/>
       <c r="F32" s="74" t="s">
         <v>50</v>
       </c>
@@ -2864,16 +2923,16 @@
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="102" t="s">
+      <c r="B33" s="103" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="19">
         <v>1</v>
       </c>
-      <c r="D33" s="105" t="s">
+      <c r="D33" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="106"/>
+      <c r="E33" s="107"/>
       <c r="F33" s="40" t="s">
         <v>13</v>
       </c>
@@ -2882,14 +2941,14 @@
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="103"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="18">
         <v>2</v>
       </c>
-      <c r="D34" s="107" t="s">
+      <c r="D34" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="108"/>
+      <c r="E34" s="109"/>
       <c r="F34" s="41" t="s">
         <v>13</v>
       </c>
@@ -2898,14 +2957,14 @@
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="104"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="16">
         <v>3</v>
       </c>
-      <c r="D35" s="109" t="s">
+      <c r="D35" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="110"/>
+      <c r="E35" s="111"/>
       <c r="F35" s="68" t="s">
         <v>17</v>
       </c>
@@ -2914,16 +2973,16 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="102" t="s">
+      <c r="B36" s="103" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="19">
         <v>1</v>
       </c>
-      <c r="D36" s="105" t="s">
+      <c r="D36" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="106"/>
+      <c r="E36" s="107"/>
       <c r="F36" s="40" t="s">
         <v>13</v>
       </c>
@@ -2932,14 +2991,14 @@
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="103"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="18">
         <v>2</v>
       </c>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="108"/>
+      <c r="E37" s="109"/>
       <c r="F37" s="41" t="s">
         <v>13</v>
       </c>
@@ -2948,14 +3007,14 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="104"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="16">
         <v>3</v>
       </c>
-      <c r="D38" s="109" t="s">
+      <c r="D38" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="110"/>
+      <c r="E38" s="111"/>
       <c r="F38" s="68" t="s">
         <v>17</v>
       </c>
@@ -2965,38 +3024,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -3013,6 +3040,38 @@
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3022,8 +3081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
   <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3040,11 +3099,11 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="121"/>
-      <c r="E2" s="122"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="137"/>
     </row>
     <row r="3" spans="2:7" ht="28.5" customHeight="1">
       <c r="B3" s="2" t="s">
@@ -3073,10 +3132,10 @@
       <c r="C5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
@@ -3085,16 +3144,16 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="29.25">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="120" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="39">
         <v>1</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="136"/>
+      <c r="E6" s="124"/>
       <c r="F6" s="42" t="s">
         <v>19</v>
       </c>
@@ -3103,14 +3162,14 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="118"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="22" t="s">
         <v>21</v>
       </c>
@@ -3119,14 +3178,14 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="43.5">
-      <c r="B8" s="118"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="93"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="38" t="s">
         <v>23</v>
       </c>
@@ -3135,14 +3194,14 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="118"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="22">
         <v>4</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="22" t="s">
         <v>25</v>
       </c>
@@ -3151,14 +3210,14 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="43.5">
-      <c r="B10" s="118"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="22">
         <v>5</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="93"/>
+      <c r="E10" s="91"/>
       <c r="F10" s="38" t="s">
         <v>27</v>
       </c>
@@ -3167,14 +3226,14 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="29.25">
-      <c r="B11" s="118"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="139" t="s">
+      <c r="D11" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="139"/>
       <c r="F11" s="61" t="s">
         <v>29</v>
       </c>
@@ -3183,16 +3242,16 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="29.25">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="120" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="51">
         <v>1</v>
       </c>
-      <c r="D12" s="135" t="s">
+      <c r="D12" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="136"/>
+      <c r="E12" s="124"/>
       <c r="F12" s="62" t="s">
         <v>19</v>
       </c>
@@ -3201,14 +3260,14 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1">
-      <c r="B13" s="118"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="34">
         <v>2</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="95"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="18" t="s">
         <v>21</v>
       </c>
@@ -3217,14 +3276,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="43.5">
-      <c r="B14" s="118"/>
+      <c r="B14" s="121"/>
       <c r="C14" s="34">
         <v>3</v>
       </c>
-      <c r="D14" s="92" t="s">
+      <c r="D14" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="93"/>
+      <c r="E14" s="91"/>
       <c r="F14" s="63" t="s">
         <v>77</v>
       </c>
@@ -3233,14 +3292,14 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="118"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="34">
         <v>4</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="95"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="18" t="s">
         <v>25</v>
       </c>
@@ -3249,14 +3308,14 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="118"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="34">
         <v>5</v>
       </c>
-      <c r="D16" s="137" t="s">
+      <c r="D16" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="143"/>
+      <c r="E16" s="119"/>
       <c r="F16" s="10" t="s">
         <v>79</v>
       </c>
@@ -3265,14 +3324,14 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="43.5">
-      <c r="B17" s="118"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="34">
         <v>6</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="93"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="63" t="s">
         <v>27</v>
       </c>
@@ -3281,14 +3340,14 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="29.25">
-      <c r="B18" s="119"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="44">
         <v>7</v>
       </c>
-      <c r="D18" s="139" t="s">
+      <c r="D18" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="140"/>
+      <c r="E18" s="139"/>
       <c r="F18" s="64" t="s">
         <v>29</v>
       </c>
@@ -3304,11 +3363,11 @@
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="135" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="121"/>
-      <c r="E23" s="122"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="2" t="s">
@@ -3337,10 +3396,10 @@
       <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="111" t="s">
+      <c r="D26" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="112"/>
+      <c r="E26" s="117"/>
       <c r="F26" s="23" t="s">
         <v>9</v>
       </c>
@@ -3349,7 +3408,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="29.25">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="120" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="27">
@@ -3367,14 +3426,14 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="118"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="18">
         <v>2</v>
       </c>
-      <c r="D28" s="131" t="s">
+      <c r="D28" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="132"/>
+      <c r="E28" s="133"/>
       <c r="F28" s="34" t="s">
         <v>21</v>
       </c>
@@ -3383,14 +3442,14 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B29" s="118"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="18">
         <v>3</v>
       </c>
-      <c r="D29" s="131" t="s">
+      <c r="D29" s="132" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="132"/>
+      <c r="E29" s="133"/>
       <c r="F29" s="25" t="s">
         <v>85</v>
       </c>
@@ -3399,14 +3458,14 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="118"/>
+      <c r="B30" s="121"/>
       <c r="C30" s="18">
         <v>4</v>
       </c>
-      <c r="D30" s="137" t="s">
+      <c r="D30" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="138"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="34" t="s">
         <v>25</v>
       </c>
@@ -3415,14 +3474,14 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="43.5">
-      <c r="B31" s="118"/>
+      <c r="B31" s="121"/>
       <c r="C31" s="28">
         <v>5</v>
       </c>
-      <c r="D31" s="92" t="s">
+      <c r="D31" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="93"/>
+      <c r="E31" s="91"/>
       <c r="F31" s="38" t="s">
         <v>27</v>
       </c>
@@ -3431,14 +3490,14 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="29.25">
-      <c r="B32" s="119"/>
+      <c r="B32" s="122"/>
       <c r="C32" s="29">
         <v>6</v>
       </c>
-      <c r="D32" s="133" t="s">
+      <c r="D32" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="134"/>
+      <c r="E32" s="144"/>
       <c r="F32" s="35" t="s">
         <v>87</v>
       </c>
@@ -3451,11 +3510,11 @@
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="120" t="s">
+      <c r="C36" s="135" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="121"/>
-      <c r="E36" s="122"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
     </row>
     <row r="37" spans="2:7" ht="28.5" customHeight="1">
       <c r="B37" s="2" t="s">
@@ -3471,11 +3530,11 @@
       <c r="B38" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="123" t="s">
+      <c r="C38" s="140" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="124"/>
-      <c r="E38" s="125"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="142"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="6" t="s">
@@ -3484,10 +3543,10 @@
       <c r="C39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="111" t="s">
+      <c r="D39" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="112"/>
+      <c r="E39" s="117"/>
       <c r="F39" s="7" t="s">
         <v>9</v>
       </c>
@@ -3496,7 +3555,7 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="29.25">
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="120" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="24">
@@ -3514,14 +3573,14 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="118"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="22">
         <v>2</v>
       </c>
-      <c r="D41" s="131" t="s">
+      <c r="D41" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="132"/>
+      <c r="E41" s="133"/>
       <c r="F41" s="18" t="s">
         <v>21</v>
       </c>
@@ -3530,14 +3589,14 @@
       </c>
     </row>
     <row r="42" spans="2:7" ht="15" customHeight="1">
-      <c r="B42" s="118"/>
+      <c r="B42" s="121"/>
       <c r="C42" s="22">
         <v>3</v>
       </c>
-      <c r="D42" s="137" t="s">
+      <c r="D42" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="138"/>
+      <c r="E42" s="131"/>
       <c r="F42" s="18" t="s">
         <v>91</v>
       </c>
@@ -3546,14 +3605,14 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="119"/>
+      <c r="B43" s="122"/>
       <c r="C43" s="58">
         <v>4</v>
       </c>
-      <c r="D43" s="109" t="s">
+      <c r="D43" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="142"/>
+      <c r="E43" s="134"/>
       <c r="F43" s="60" t="s">
         <v>93</v>
       </c>
@@ -3562,7 +3621,7 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="29.25">
-      <c r="B44" s="117" t="s">
+      <c r="B44" s="120" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="51">
@@ -3580,14 +3639,14 @@
       </c>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="118"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="34">
         <v>2</v>
       </c>
-      <c r="D45" s="131" t="s">
+      <c r="D45" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="132"/>
+      <c r="E45" s="133"/>
       <c r="F45" s="22" t="s">
         <v>21</v>
       </c>
@@ -3596,14 +3655,14 @@
       </c>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="118"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="34">
         <v>3</v>
       </c>
-      <c r="D46" s="137" t="s">
+      <c r="D46" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="138"/>
+      <c r="E46" s="131"/>
       <c r="F46" s="22" t="s">
         <v>91</v>
       </c>
@@ -3612,14 +3671,14 @@
       </c>
     </row>
     <row r="47" spans="2:7" ht="43.5">
-      <c r="B47" s="118"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="34">
         <v>4</v>
       </c>
-      <c r="D47" s="137" t="s">
+      <c r="D47" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="E47" s="138"/>
+      <c r="E47" s="131"/>
       <c r="F47" s="60" t="s">
         <v>93</v>
       </c>
@@ -3628,14 +3687,14 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="35.25" customHeight="1">
-      <c r="B48" s="119"/>
+      <c r="B48" s="122"/>
       <c r="C48" s="44">
         <v>5</v>
       </c>
-      <c r="D48" s="109" t="s">
+      <c r="D48" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="142"/>
+      <c r="E48" s="134"/>
       <c r="F48" s="48" t="s">
         <v>94</v>
       </c>
@@ -3644,36 +3703,25 @@
       </c>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="141"/>
-      <c r="E49" s="141"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="125"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="141"/>
-      <c r="E50" s="141"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
@@ -3690,16 +3738,27 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3709,7 +3768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -3727,31 +3786,31 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="164"/>
-      <c r="E2" s="165"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="152"/>
     </row>
     <row r="3" spans="2:7" ht="30" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="43" t="s">
@@ -3760,10 +3819,10 @@
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="166" t="s">
+      <c r="D5" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
@@ -3772,16 +3831,16 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="120" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="51">
         <v>1</v>
       </c>
-      <c r="D6" s="149" t="s">
+      <c r="D6" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="154"/>
+      <c r="E6" s="146"/>
       <c r="F6" s="40" t="s">
         <v>13</v>
       </c>
@@ -3790,14 +3849,14 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="118"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="34">
         <v>2</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="41" t="s">
         <v>13</v>
       </c>
@@ -3806,14 +3865,14 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="118"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="34">
         <v>3</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="41" t="s">
         <v>13</v>
       </c>
@@ -3822,14 +3881,14 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="118"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="34">
         <v>4</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="38" t="s">
         <v>34</v>
       </c>
@@ -3838,14 +3897,14 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="45.75" customHeight="1">
-      <c r="B10" s="118"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="34">
         <v>5</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="93"/>
+      <c r="E10" s="91"/>
       <c r="F10" s="38" t="s">
         <v>36</v>
       </c>
@@ -3854,14 +3913,14 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.5">
-      <c r="B11" s="118"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="34">
         <v>6</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="93"/>
+      <c r="E11" s="91"/>
       <c r="F11" s="38" t="s">
         <v>38</v>
       </c>
@@ -3870,14 +3929,14 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="118"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="34">
         <v>7</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="80"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="50" t="s">
         <v>40</v>
       </c>
@@ -3886,14 +3945,14 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="118"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="34">
         <v>8</v>
       </c>
-      <c r="D13" s="94" t="s">
+      <c r="D13" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="95"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="50" t="s">
         <v>42</v>
       </c>
@@ -3902,14 +3961,14 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="119"/>
+      <c r="B14" s="122"/>
       <c r="C14" s="54">
         <v>9</v>
       </c>
-      <c r="D14" s="168" t="s">
+      <c r="D14" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="169"/>
+      <c r="E14" s="148"/>
       <c r="F14" s="53" t="s">
         <v>44</v>
       </c>
@@ -3918,16 +3977,16 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="120" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="27">
         <v>1</v>
       </c>
-      <c r="D15" s="167" t="s">
+      <c r="D15" s="145" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="154"/>
+      <c r="E15" s="146"/>
       <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
@@ -3936,14 +3995,14 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="118"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="18">
         <v>2</v>
       </c>
-      <c r="D16" s="151" t="s">
+      <c r="D16" s="155" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="85"/>
       <c r="F16" s="14" t="s">
         <v>55</v>
       </c>
@@ -3952,14 +4011,14 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="118"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="18">
         <v>3</v>
       </c>
-      <c r="D17" s="152" t="s">
+      <c r="D17" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="153"/>
+      <c r="E17" s="157"/>
       <c r="F17" s="14" t="s">
         <v>55</v>
       </c>
@@ -3968,32 +4027,32 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="119"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="29">
         <v>4</v>
       </c>
-      <c r="D18" s="148" t="s">
+      <c r="D18" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="140"/>
+      <c r="E18" s="139"/>
       <c r="F18" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="171" t="s">
+      <c r="G18" s="79" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="120" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="27">
         <v>1</v>
       </c>
-      <c r="D19" s="149" t="s">
+      <c r="D19" s="154" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="154"/>
+      <c r="E19" s="146"/>
       <c r="F19" s="59" t="s">
         <v>13</v>
       </c>
@@ -4002,14 +4061,14 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="118"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="18">
         <v>2</v>
       </c>
-      <c r="D20" s="151" t="s">
+      <c r="D20" s="155" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="80"/>
+      <c r="E20" s="85"/>
       <c r="F20" s="14" t="s">
         <v>55</v>
       </c>
@@ -4018,14 +4077,14 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="118"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="18">
         <v>3</v>
       </c>
-      <c r="D21" s="152" t="s">
+      <c r="D21" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="153"/>
+      <c r="E21" s="157"/>
       <c r="F21" s="14" t="s">
         <v>55</v>
       </c>
@@ -4034,14 +4093,14 @@
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="119"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="29">
         <v>4</v>
       </c>
-      <c r="D22" s="148" t="s">
+      <c r="D22" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="140"/>
+      <c r="E22" s="139"/>
       <c r="F22" s="49" t="s">
         <v>103</v>
       </c>
@@ -4050,16 +4109,16 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="120" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="27">
         <v>1</v>
       </c>
-      <c r="D23" s="149" t="s">
+      <c r="D23" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="154"/>
+      <c r="E23" s="146"/>
       <c r="F23" s="14" t="s">
         <v>55</v>
       </c>
@@ -4068,14 +4127,14 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="118"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="18">
         <v>2</v>
       </c>
-      <c r="D24" s="151" t="s">
+      <c r="D24" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="80"/>
+      <c r="E24" s="85"/>
       <c r="F24" s="10" t="s">
         <v>13</v>
       </c>
@@ -4084,14 +4143,14 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="118"/>
+      <c r="B25" s="121"/>
       <c r="C25" s="18">
         <v>3</v>
       </c>
-      <c r="D25" s="152" t="s">
+      <c r="D25" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="153"/>
+      <c r="E25" s="157"/>
       <c r="F25" s="14" t="s">
         <v>55</v>
       </c>
@@ -4100,14 +4159,14 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="118"/>
+      <c r="B26" s="121"/>
       <c r="C26" s="29">
         <v>4</v>
       </c>
-      <c r="D26" s="148" t="s">
+      <c r="D26" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="140"/>
+      <c r="E26" s="139"/>
       <c r="F26" s="49" t="s">
         <v>105</v>
       </c>
@@ -4116,16 +4175,16 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="120" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="46">
         <v>1</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="170"/>
+      <c r="E27" s="149"/>
       <c r="F27" s="14" t="s">
         <v>55</v>
       </c>
@@ -4134,14 +4193,14 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="118"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="45">
         <v>2</v>
       </c>
-      <c r="D28" s="151" t="s">
+      <c r="D28" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="80"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="14" t="s">
         <v>55</v>
       </c>
@@ -4150,14 +4209,14 @@
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="118"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="45">
         <v>3</v>
       </c>
-      <c r="D29" s="152" t="s">
+      <c r="D29" s="156" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="153"/>
+      <c r="E29" s="157"/>
       <c r="F29" s="18" t="s">
         <v>13</v>
       </c>
@@ -4166,14 +4225,14 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="119"/>
+      <c r="B30" s="122"/>
       <c r="C30" s="47">
         <v>4</v>
       </c>
-      <c r="D30" s="148" t="s">
+      <c r="D30" s="158" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="140"/>
+      <c r="E30" s="139"/>
       <c r="F30" s="49" t="s">
         <v>105</v>
       </c>
@@ -4182,16 +4241,16 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="118" t="s">
+      <c r="B31" s="121" t="s">
         <v>60</v>
       </c>
       <c r="C31" s="27">
         <v>1</v>
       </c>
-      <c r="D31" s="149" t="s">
+      <c r="D31" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="154"/>
+      <c r="E31" s="146"/>
       <c r="F31" s="8" t="s">
         <v>13</v>
       </c>
@@ -4200,14 +4259,14 @@
       </c>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="118"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="18">
         <v>2</v>
       </c>
-      <c r="D32" s="149" t="s">
+      <c r="D32" s="154" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="154"/>
+      <c r="E32" s="146"/>
       <c r="F32" s="10" t="s">
         <v>13</v>
       </c>
@@ -4216,14 +4275,14 @@
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="118"/>
+      <c r="B33" s="121"/>
       <c r="C33" s="18">
         <v>3</v>
       </c>
-      <c r="D33" s="155" t="s">
+      <c r="D33" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="156"/>
+      <c r="E33" s="161"/>
       <c r="F33" s="18" t="s">
         <v>13</v>
       </c>
@@ -4232,32 +4291,32 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="29.25">
-      <c r="B34" s="119"/>
+      <c r="B34" s="122"/>
       <c r="C34" s="29">
         <v>4</v>
       </c>
-      <c r="D34" s="157" t="s">
+      <c r="D34" s="162" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="158"/>
+      <c r="E34" s="163"/>
       <c r="F34" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="G34" s="171" t="s">
+      <c r="G34" s="79" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="31.5" customHeight="1">
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="120" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="39">
         <v>1</v>
       </c>
-      <c r="D35" s="159" t="s">
+      <c r="D35" s="164" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="160"/>
+      <c r="E35" s="165"/>
       <c r="F35" s="46" t="s">
         <v>13</v>
       </c>
@@ -4266,14 +4325,14 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B36" s="118"/>
+      <c r="B36" s="121"/>
       <c r="C36" s="22">
         <v>2</v>
       </c>
-      <c r="D36" s="145" t="s">
+      <c r="D36" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="146"/>
+      <c r="E36" s="167"/>
       <c r="F36" s="45" t="s">
         <v>13</v>
       </c>
@@ -4282,14 +4341,14 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B37" s="118"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="22">
         <v>3</v>
       </c>
-      <c r="D37" s="145" t="s">
+      <c r="D37" s="166" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="146"/>
+      <c r="E37" s="167"/>
       <c r="F37" s="45" t="s">
         <v>13</v>
       </c>
@@ -4298,32 +4357,32 @@
       </c>
     </row>
     <row r="38" spans="2:7" ht="29.25">
-      <c r="B38" s="119"/>
+      <c r="B38" s="122"/>
       <c r="C38" s="15">
         <v>4</v>
       </c>
-      <c r="D38" s="161" t="s">
+      <c r="D38" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="162"/>
+      <c r="E38" s="169"/>
       <c r="F38" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="G38" s="171" t="s">
+      <c r="G38" s="79" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="15" customHeight="1">
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="121" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="39">
         <v>1</v>
       </c>
-      <c r="D39" s="149" t="s">
+      <c r="D39" s="154" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="150"/>
+      <c r="E39" s="159"/>
       <c r="F39" s="55" t="s">
         <v>13</v>
       </c>
@@ -4332,14 +4391,14 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15" customHeight="1">
-      <c r="B40" s="118"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="22">
         <v>2</v>
       </c>
-      <c r="D40" s="79" t="s">
+      <c r="D40" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="144"/>
+      <c r="E40" s="170"/>
       <c r="F40" s="56" t="s">
         <v>13</v>
       </c>
@@ -4348,14 +4407,14 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="15" customHeight="1">
-      <c r="B41" s="118"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="22">
         <v>3</v>
       </c>
-      <c r="D41" s="145" t="s">
+      <c r="D41" s="166" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="146"/>
+      <c r="E41" s="167"/>
       <c r="F41" s="45" t="s">
         <v>13</v>
       </c>
@@ -4364,187 +4423,261 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="119"/>
+      <c r="B42" s="122"/>
       <c r="C42" s="15">
         <v>4</v>
       </c>
-      <c r="D42" s="139" t="s">
+      <c r="D42" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="147"/>
+      <c r="E42" s="171"/>
       <c r="F42" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="G42" s="171" t="s">
+      <c r="G42" s="79" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="D43" s="96"/>
-      <c r="E43" s="96"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="D44" s="96"/>
-      <c r="E44" s="96"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="D45" s="96"/>
-      <c r="E45" s="96"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="D47" s="96"/>
-      <c r="E47" s="96"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="D48" s="96"/>
-      <c r="E48" s="96"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="96"/>
-      <c r="E49" s="96"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="80"/>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="96"/>
-      <c r="E50" s="96"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="96"/>
-      <c r="E51" s="96"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="96"/>
-      <c r="E53" s="96"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
     </row>
     <row r="54" spans="4:5">
-      <c r="D54" s="96"/>
-      <c r="E54" s="96"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
     </row>
     <row r="55" spans="4:5">
-      <c r="D55" s="96"/>
-      <c r="E55" s="96"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
     </row>
     <row r="56" spans="4:5">
-      <c r="D56" s="96"/>
-      <c r="E56" s="96"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
     </row>
     <row r="57" spans="4:5">
-      <c r="D57" s="96"/>
-      <c r="E57" s="96"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
     </row>
     <row r="58" spans="4:5">
-      <c r="D58" s="96"/>
-      <c r="E58" s="96"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
     </row>
     <row r="59" spans="4:5">
-      <c r="D59" s="96"/>
-      <c r="E59" s="96"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="80"/>
     </row>
     <row r="60" spans="4:5">
-      <c r="D60" s="96"/>
-      <c r="E60" s="96"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
     </row>
     <row r="61" spans="4:5">
-      <c r="D61" s="96"/>
-      <c r="E61" s="96"/>
+      <c r="D61" s="80"/>
+      <c r="E61" s="80"/>
     </row>
     <row r="62" spans="4:5">
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
+      <c r="D62" s="80"/>
+      <c r="E62" s="80"/>
     </row>
     <row r="63" spans="4:5">
-      <c r="D63" s="96"/>
-      <c r="E63" s="96"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
     </row>
     <row r="64" spans="4:5">
-      <c r="D64" s="96"/>
-      <c r="E64" s="96"/>
+      <c r="D64" s="80"/>
+      <c r="E64" s="80"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="96"/>
-      <c r="E65" s="96"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="96"/>
-      <c r="E66" s="96"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="96"/>
-      <c r="E67" s="96"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="80"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="96"/>
-      <c r="E68" s="96"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="96"/>
-      <c r="E69" s="96"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="80"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="96"/>
-      <c r="E71" s="96"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="96"/>
-      <c r="E72" s="96"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
     </row>
     <row r="73" spans="4:5">
-      <c r="D73" s="96"/>
-      <c r="E73" s="96"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
     </row>
     <row r="74" spans="4:5">
-      <c r="D74" s="96"/>
-      <c r="E74" s="96"/>
+      <c r="D74" s="80"/>
+      <c r="E74" s="80"/>
     </row>
     <row r="75" spans="4:5">
-      <c r="D75" s="96"/>
-      <c r="E75" s="96"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
     </row>
     <row r="76" spans="4:5">
-      <c r="D76" s="96"/>
-      <c r="E76" s="96"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="80"/>
     </row>
     <row r="77" spans="4:5">
-      <c r="D77" s="96"/>
-      <c r="E77" s="96"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="80"/>
     </row>
     <row r="78" spans="4:5">
-      <c r="D78" s="96"/>
-      <c r="E78" s="96"/>
+      <c r="D78" s="80"/>
+      <c r="E78" s="80"/>
     </row>
     <row r="79" spans="4:5">
-      <c r="D79" s="96"/>
-      <c r="E79" s="96"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
     </row>
     <row r="80" spans="4:5">
-      <c r="D80" s="96"/>
-      <c r="E80" s="96"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="80"/>
     </row>
     <row r="81" spans="4:5">
-      <c r="D81" s="96"/>
-      <c r="E81" s="96"/>
+      <c r="D81" s="80"/>
+      <c r="E81" s="80"/>
     </row>
     <row r="82" spans="4:5">
-      <c r="D82" s="96"/>
-      <c r="E82" s="96"/>
+      <c r="D82" s="80"/>
+      <c r="E82" s="80"/>
     </row>
     <row r="83" spans="4:5">
-      <c r="D83" s="96"/>
-      <c r="E83" s="96"/>
+      <c r="D83" s="80"/>
+      <c r="E83" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="90">
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="D9:E9"/>
@@ -4561,80 +4694,279 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D27:E27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DDDF08-D476-4F4C-A33B-D4FE5576860C}">
+  <dimension ref="B2:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="135" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="136"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" ht="30" customHeight="1">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="127"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1">
+      <c r="B4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="127"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="100"/>
+      <c r="F5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="39">
+        <v>1</v>
+      </c>
+      <c r="D6" s="154" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="146"/>
+      <c r="F6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="82"/>
+      <c r="C7" s="22">
+        <v>2</v>
+      </c>
+      <c r="D7" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="85"/>
+      <c r="F7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="2:7" ht="43.5">
+      <c r="B8" s="83"/>
+      <c r="C8" s="15">
+        <v>3</v>
+      </c>
+      <c r="D8" s="138" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="139"/>
+      <c r="F8" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="177"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="175"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="177"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="173"/>
+      <c r="E10" s="173"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="175"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="177"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="174"/>
+      <c r="G11" s="175"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="135" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="126" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="127"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1">
+      <c r="B14" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="126" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="127"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="100"/>
+      <c r="F15" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="39">
+        <v>1</v>
+      </c>
+      <c r="D16" s="154" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="146"/>
+      <c r="F16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="82"/>
+      <c r="C17" s="22">
+        <v>2</v>
+      </c>
+      <c r="D17" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="85"/>
+      <c r="F17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="82"/>
+      <c r="C18" s="22">
+        <v>3</v>
+      </c>
+      <c r="D18" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="87"/>
+      <c r="F18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="83"/>
+      <c r="C19" s="15">
+        <v>4</v>
+      </c>
+      <c r="D19" s="178" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="179"/>
+      <c r="F19" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testes todas classses foram sucessos, e coloquei as pastas bugs
</commit_message>
<xml_diff>
--- a/documents/scenarios/Cenarios de Sauce Demo.xlsx
+++ b/documents/scenarios/Cenarios de Sauce Demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6818742-197D-46C2-A9DF-169925C541E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D75403D2-08A9-4B13-B7CC-90527A963FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login e Finalizar a comprar" sheetId="5" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="CHECKOUT - FINISH" sheetId="4" r:id="rId4"/>
     <sheet name="PROBLEM USER" sheetId="6" r:id="rId5"/>
     <sheet name="LOCKED USER" sheetId="7" r:id="rId6"/>
+    <sheet name="PERFORMANCE" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="170">
   <si>
     <t>Cenário</t>
   </si>
@@ -525,13 +526,34 @@
   </si>
   <si>
     <t>O sistema deverá impedir a próxima etapa. O sistema exibirá a mensagem: 'Epic sadface: Sorry, this user has been locked out.'.</t>
+  </si>
+  <si>
+    <t>Verificar a performance do carregamento ao fazer login</t>
+  </si>
+  <si>
+    <t>Para garantir uma experiência de medição de tempos de carregamento de página.</t>
+  </si>
+  <si>
+    <t>Realizar login e o tempo de carregamento não ultrapasse 3 segundos</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Username com um username  com 'performance_glitch_user'</t>
+  </si>
+  <si>
+    <t>Preencher o campo de Password com uma senha com 'secret_sauce'</t>
+  </si>
+  <si>
+    <t>Medir o tempo entre o envio da requisição e o carregamento completo da tela de "Products"</t>
+  </si>
+  <si>
+    <t>O tempo de carregamento não ultrapassa 3 segundos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,6 +590,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -589,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1238,11 +1266,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1450,122 +1487,120 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1758,16 +1793,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2106,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC91AAE-4EFC-46C7-989E-817CB8D6485D}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2527,7 +2610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="F8" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3198,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0926458F-1E1F-4599-873A-7C8AA3D763A7}">
   <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3885,8 +3968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B67A05C-29F6-4770-BA8C-345876741247}">
   <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51:E51"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4152,7 +4235,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="148"/>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="77" t="s">
         <v>101</v>
       </c>
       <c r="G18" s="11" t="s">
@@ -4869,10 +4952,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DDDF08-D476-4F4C-A33B-D4FE5576860C}">
-  <dimension ref="B2:H63"/>
+  <dimension ref="B2:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4995,7 +5078,7 @@
         <v>128</v>
       </c>
       <c r="E9" s="180"/>
-      <c r="F9" s="80" t="s">
+      <c r="F9" s="78" t="s">
         <v>129</v>
       </c>
       <c r="G9" s="76" t="s">
@@ -5136,7 +5219,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="28.5" customHeight="1"/>
-    <row r="25" spans="2:7" ht="29.25" customHeight="1">
+    <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
@@ -5230,7 +5313,7 @@
         <v>139</v>
       </c>
       <c r="E31" s="146"/>
-      <c r="F31" s="82" t="s">
+      <c r="F31" s="80" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="11" t="s">
@@ -5246,7 +5329,7 @@
         <v>140</v>
       </c>
       <c r="E32" s="146"/>
-      <c r="F32" s="83" t="s">
+      <c r="F32" s="81" t="s">
         <v>141</v>
       </c>
       <c r="G32" s="11" t="s">
@@ -5262,7 +5345,7 @@
         <v>142</v>
       </c>
       <c r="E33" s="140"/>
-      <c r="F33" s="81" t="s">
+      <c r="F33" s="79" t="s">
         <v>143</v>
       </c>
       <c r="G33" s="11" t="s">
@@ -5278,7 +5361,7 @@
         <v>140</v>
       </c>
       <c r="E34" s="150"/>
-      <c r="F34" s="79" t="s">
+      <c r="F34" s="77" t="s">
         <v>144</v>
       </c>
       <c r="G34" s="76" t="s">
@@ -5343,7 +5426,7 @@
       <c r="D38" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="181"/>
+      <c r="E38" s="184"/>
       <c r="F38" s="62" t="s">
         <v>145</v>
       </c>
@@ -5356,10 +5439,10 @@
       <c r="C39" s="34">
         <v>5</v>
       </c>
-      <c r="D39" s="139" t="s">
+      <c r="D39" s="182" t="s">
         <v>146</v>
       </c>
-      <c r="E39" s="181"/>
+      <c r="E39" s="183"/>
       <c r="F39" s="59" t="s">
         <v>147</v>
       </c>
@@ -5377,8 +5460,8 @@
       <c r="D40" s="156" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="162"/>
-      <c r="F40" s="8" t="s">
+      <c r="E40" s="157"/>
+      <c r="F40" s="55" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="12" t="s">
@@ -5393,8 +5476,8 @@
       <c r="D41" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="88"/>
-      <c r="F41" s="10" t="s">
+      <c r="E41" s="152"/>
+      <c r="F41" s="56" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="11" t="s">
@@ -5409,25 +5492,23 @@
       <c r="D42" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="103"/>
-      <c r="F42" s="10" t="s">
+      <c r="E42" s="181"/>
+      <c r="F42" s="56" t="s">
         <v>17</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="15" customHeight="1">
+    <row r="43" spans="2:8">
       <c r="B43" s="126"/>
-      <c r="C43" s="34">
-        <v>4</v>
-      </c>
-      <c r="D43" s="139" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" s="181"/>
-      <c r="F43" s="81" t="s">
-        <v>143</v>
+      <c r="C43" s="34"/>
+      <c r="D43" s="145" t="s">
+        <v>148</v>
+      </c>
+      <c r="E43" s="146"/>
+      <c r="F43" s="45" t="s">
+        <v>21</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>14</v>
@@ -5435,250 +5516,300 @@
     </row>
     <row r="44" spans="2:8" ht="15" customHeight="1">
       <c r="B44" s="126"/>
-      <c r="C44" s="54">
+      <c r="C44" s="34">
+        <v>4</v>
+      </c>
+      <c r="D44" s="139" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="140"/>
+      <c r="F44" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15" customHeight="1">
+      <c r="B45" s="126"/>
+      <c r="C45" s="54">
         <v>5</v>
       </c>
-      <c r="D44" s="139" t="s">
+      <c r="D45" s="139" t="s">
         <v>148</v>
       </c>
-      <c r="E44" s="181"/>
-      <c r="F44" s="18" t="s">
+      <c r="E45" s="140"/>
+      <c r="F45" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="G44" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="G45" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="29.25">
-      <c r="B45" s="127"/>
-      <c r="C45" s="44">
+    <row r="46" spans="2:8" ht="29.25">
+      <c r="B46" s="127"/>
+      <c r="C46" s="44">
         <v>5</v>
       </c>
-      <c r="D45" s="147" t="s">
+      <c r="D46" s="147" t="s">
         <v>150</v>
       </c>
-      <c r="E45" s="148"/>
-      <c r="F45" s="63" t="s">
+      <c r="E46" s="155"/>
+      <c r="F46" s="83" t="s">
         <v>145</v>
       </c>
-      <c r="G45" s="76" t="s">
+      <c r="G46" s="76" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="31.5" customHeight="1">
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="2:7" ht="31.5" customHeight="1">
+      <c r="B50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="131" t="s">
+      <c r="C50" s="131" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="132"/>
-      <c r="E49" s="133"/>
-      <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="2:7" ht="29.25" customHeight="1">
-      <c r="B50" s="2" t="s">
+      <c r="D50" s="132"/>
+      <c r="E50" s="133"/>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="2:7" ht="29.25" customHeight="1">
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="134" t="s">
+      <c r="C51" s="134" t="s">
         <v>152</v>
-      </c>
-      <c r="D50" s="135"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="21"/>
-    </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1">
-      <c r="B51" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="134" t="s">
-        <v>153</v>
       </c>
       <c r="D51" s="135"/>
       <c r="E51" s="136"/>
       <c r="F51" s="21"/>
     </row>
-    <row r="52" spans="2:7">
-      <c r="B52" s="4" t="s">
+    <row r="52" spans="2:7" ht="30" customHeight="1">
+      <c r="B52" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="134" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="135"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="21"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C53" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="96" t="s">
+      <c r="D53" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="E52" s="97"/>
-      <c r="F52" s="23" t="s">
+      <c r="E53" s="97"/>
+      <c r="F53" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G52" s="23" t="s">
+      <c r="G53" s="23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
-      <c r="B53" s="125" t="s">
+    <row r="54" spans="2:7">
+      <c r="B54" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="51">
+      <c r="C54" s="51">
         <v>1</v>
       </c>
-      <c r="D53" s="156" t="s">
+      <c r="D54" s="156" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="157"/>
-      <c r="F53" s="77" t="s">
+      <c r="E54" s="162"/>
+      <c r="F54" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G53" s="30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7">
-      <c r="B54" s="126"/>
-      <c r="C54" s="34">
-        <v>2</v>
-      </c>
-      <c r="D54" s="87" t="s">
-        <v>127</v>
-      </c>
-      <c r="E54" s="152"/>
-      <c r="F54" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="126"/>
       <c r="C55" s="34">
-        <v>3</v>
-      </c>
-      <c r="D55" s="102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" s="184"/>
-      <c r="F55" s="78" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="29.25">
+        <v>2</v>
+      </c>
+      <c r="D55" s="87" t="s">
+        <v>127</v>
+      </c>
+      <c r="E55" s="88"/>
+      <c r="F55" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
       <c r="B56" s="126"/>
       <c r="C56" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D56" s="102" t="s">
-        <v>140</v>
-      </c>
-      <c r="E56" s="184"/>
-      <c r="F56" s="85" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7">
+        <v>16</v>
+      </c>
+      <c r="E56" s="103"/>
+      <c r="F56" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="29.25">
       <c r="B57" s="126"/>
       <c r="C57" s="34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D57" s="102" t="s">
-        <v>142</v>
-      </c>
-      <c r="E57" s="184"/>
-      <c r="F57" s="78" t="s">
-        <v>143</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="29.25">
+        <v>140</v>
+      </c>
+      <c r="E57" s="103"/>
+      <c r="F57" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
       <c r="B58" s="126"/>
       <c r="C58" s="34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="102" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="184"/>
-      <c r="F58" s="85" t="s">
-        <v>141</v>
-      </c>
-      <c r="G58" s="86" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7">
+        <v>142</v>
+      </c>
+      <c r="E58" s="103"/>
+      <c r="F58" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="29.25">
       <c r="B59" s="126"/>
       <c r="C59" s="34">
+        <v>6</v>
+      </c>
+      <c r="D59" s="102" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="103"/>
+      <c r="F59" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="85" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" s="126"/>
+      <c r="C60" s="34">
         <v>7</v>
       </c>
-      <c r="D59" s="87" t="s">
+      <c r="D60" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="E60" s="103"/>
+      <c r="F60" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="29.25">
+      <c r="B61" s="126"/>
+      <c r="C61" s="34">
+        <v>8</v>
+      </c>
+      <c r="D61" s="102" t="s">
+        <v>150</v>
+      </c>
+      <c r="E61" s="103"/>
+      <c r="F61" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62" s="126"/>
+      <c r="C62" s="34">
+        <v>9</v>
+      </c>
+      <c r="D62" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="E59" s="152"/>
-      <c r="F59" s="78" t="s">
+      <c r="E62" s="88"/>
+      <c r="F62" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="G59" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7">
-      <c r="B60" s="127"/>
-      <c r="C60" s="44">
-        <v>8</v>
-      </c>
-      <c r="D60" s="182" t="s">
+      <c r="G62" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="127"/>
+      <c r="C63" s="44">
+        <v>10</v>
+      </c>
+      <c r="D63" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="E60" s="183"/>
-      <c r="F60" s="35" t="s">
+      <c r="E63" s="186"/>
+      <c r="F63" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="G60" s="75" t="s">
+      <c r="G63" s="76" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="2:7">
-      <c r="D61" s="104"/>
-      <c r="E61" s="104"/>
-    </row>
-    <row r="62" spans="2:7">
-      <c r="D62" s="104"/>
-      <c r="E62" s="104"/>
-    </row>
-    <row r="63" spans="2:7">
-      <c r="D63" s="104"/>
-      <c r="E63" s="104"/>
+    <row r="64" spans="2:7">
+      <c r="D64" s="104"/>
+      <c r="E64" s="104"/>
+    </row>
+    <row r="65" spans="4:5">
+      <c r="D65" s="104"/>
+      <c r="E65" s="104"/>
+    </row>
+    <row r="66" spans="4:5">
+      <c r="D66" s="104"/>
+      <c r="E66" s="104"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
+  <mergeCells count="61">
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="D57:E57"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C51:E51"/>
-    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="C52:E52"/>
     <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -5698,13 +5829,14 @@
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="B40:B46"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D44:E44"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="B17:B21"/>
@@ -5731,7 +5863,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5754,7 +5886,7 @@
       <c r="E2" s="130"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" ht="28.5" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5765,7 +5897,7 @@
       <c r="E3" s="136"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="30.75" customHeight="1">
       <c r="B4" s="36" t="s">
         <v>4</v>
       </c>
@@ -5808,7 +5940,9 @@
       <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="106"/>
@@ -5822,7 +5956,9 @@
       <c r="F7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="2:7" ht="43.5">
       <c r="B8" s="107"/>
@@ -5836,7 +5972,9 @@
       <c r="F8" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5851,4 +5989,288 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCCBA6D-ABAD-480A-B0AD-FAEDEF2A0600}">
+  <dimension ref="B2:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" ht="28.5" customHeight="1">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="94"/>
+      <c r="E4" s="95"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B6" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="39">
+        <v>1</v>
+      </c>
+      <c r="D6" s="187" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="188"/>
+      <c r="F6" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="29.25" customHeight="1">
+      <c r="B7" s="106"/>
+      <c r="C7" s="22">
+        <v>2</v>
+      </c>
+      <c r="D7" s="153" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="161"/>
+      <c r="F7" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="106"/>
+      <c r="C8" s="22">
+        <v>3</v>
+      </c>
+      <c r="D8" s="87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="88"/>
+      <c r="F8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="27.75" customHeight="1">
+      <c r="B9" s="107"/>
+      <c r="C9" s="15">
+        <v>4</v>
+      </c>
+      <c r="D9" s="198" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="199"/>
+      <c r="F9" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="200" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="197"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="190"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="189"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1">
+      <c r="B11" s="197"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="192"/>
+      <c r="E11" s="190"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="197"/>
+      <c r="C12" s="189"/>
+      <c r="D12" s="192"/>
+      <c r="E12" s="192"/>
+      <c r="F12" s="191"/>
+      <c r="G12" s="189"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="197"/>
+      <c r="C13" s="189"/>
+      <c r="D13" s="190"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="189"/>
+      <c r="G13" s="189"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="197"/>
+      <c r="C14" s="189"/>
+      <c r="D14" s="192"/>
+      <c r="E14" s="192"/>
+      <c r="F14" s="191"/>
+      <c r="G14" s="189"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="197"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="190"/>
+      <c r="E15" s="190"/>
+      <c r="F15" s="191"/>
+      <c r="G15" s="189"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="197"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="193"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="194"/>
+      <c r="G16" s="189"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="197"/>
+      <c r="C17" s="189"/>
+      <c r="D17" s="193"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="194"/>
+      <c r="G17" s="189"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="197"/>
+      <c r="C18" s="189"/>
+      <c r="D18" s="193"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="194"/>
+      <c r="G18" s="189"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="197"/>
+      <c r="C19" s="189"/>
+      <c r="D19" s="190"/>
+      <c r="E19" s="190"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="189"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="197"/>
+      <c r="C20" s="189"/>
+      <c r="D20" s="192"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="191"/>
+      <c r="G20" s="189"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="197"/>
+      <c r="C21" s="189"/>
+      <c r="D21" s="192"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="191"/>
+      <c r="G21" s="189"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="197"/>
+      <c r="C22" s="189"/>
+      <c r="D22" s="193"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="195"/>
+      <c r="G22" s="189"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="197"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="195"/>
+      <c r="G23" s="189"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="197"/>
+      <c r="C24" s="189"/>
+      <c r="D24" s="196"/>
+      <c r="E24" s="196"/>
+      <c r="F24" s="195"/>
+      <c r="G24" s="189"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>